<commit_message>
Script updates. Change bin status to three past years.
</commit_message>
<xml_diff>
--- a/ratings-2022.xlsx
+++ b/ratings-2022.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10911"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mike/PycharmProjects/tvratings-ssac2023/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{042117E5-739D-7A4B-AAE9-FF8DA3A476DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9714AA1-637B-3841-A1BF-8677594967B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="13360" windowWidth="40960" windowHeight="11000" xr2:uid="{BBDA95F9-3552-704A-ADE2-3350C5179C3F}"/>
   </bookViews>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1190" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1346" uniqueCount="190">
   <si>
     <t>Time</t>
   </si>
@@ -630,6 +630,9 @@
   <si>
     <t>North Dakota State</t>
   </si>
+  <si>
+    <t>North Carolina State</t>
+  </si>
 </sst>
 </file>
 
@@ -989,8 +992,8 @@
   <dimension ref="A1:AA105"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="760" topLeftCell="A93" activePane="bottomLeft"/>
-      <selection pane="bottomLeft" activeCell="E106" sqref="E106"/>
+      <pane ySplit="760" topLeftCell="A86" activePane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="F90" sqref="F90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8578,7 +8581,7 @@
         <v>58</v>
       </c>
       <c r="F86">
-        <v>0</v>
+        <v>1255000</v>
       </c>
       <c r="G86">
         <v>2022</v>
@@ -8622,6 +8625,21 @@
         <f t="array" ref="R86">_xlfn.XLOOKUP(E86&amp;I86,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!D$2:D$13000,"")</f>
         <v>36</v>
       </c>
+      <c r="S86">
+        <v>0</v>
+      </c>
+      <c r="T86">
+        <v>0</v>
+      </c>
+      <c r="U86">
+        <v>0</v>
+      </c>
+      <c r="V86">
+        <v>0</v>
+      </c>
+      <c r="W86">
+        <v>0</v>
+      </c>
       <c r="X86" cm="1">
         <f t="array" ref="X86">_xlfn.XLOOKUP(D86&amp;I86,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!E$2:E$13000,"")</f>
         <v>3</v>
@@ -8656,7 +8674,7 @@
         <v>173</v>
       </c>
       <c r="F87">
-        <v>0</v>
+        <v>1224000</v>
       </c>
       <c r="G87">
         <v>2022</v>
@@ -8700,6 +8718,21 @@
         <f t="array" ref="R87">_xlfn.XLOOKUP(E87&amp;I87,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!D$2:D$13000,"")</f>
         <v>11.8</v>
       </c>
+      <c r="S87">
+        <v>0</v>
+      </c>
+      <c r="T87">
+        <v>0</v>
+      </c>
+      <c r="U87">
+        <v>0</v>
+      </c>
+      <c r="V87">
+        <v>0</v>
+      </c>
+      <c r="W87">
+        <v>0</v>
+      </c>
       <c r="X87" cm="1">
         <f t="array" ref="X87">_xlfn.XLOOKUP(D87&amp;I87,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!E$2:E$13000,"")</f>
         <v>2</v>
@@ -8734,7 +8767,7 @@
         <v>161</v>
       </c>
       <c r="F88">
-        <v>0</v>
+        <v>407000</v>
       </c>
       <c r="G88">
         <v>2022</v>
@@ -8778,6 +8811,21 @@
         <f t="array" ref="R88">_xlfn.XLOOKUP(E88&amp;I88,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!D$2:D$13000,"")</f>
         <v>23.5</v>
       </c>
+      <c r="S88">
+        <v>0</v>
+      </c>
+      <c r="T88">
+        <v>0</v>
+      </c>
+      <c r="U88">
+        <v>0</v>
+      </c>
+      <c r="V88">
+        <v>0</v>
+      </c>
+      <c r="W88">
+        <v>0</v>
+      </c>
       <c r="X88" cm="1">
         <f t="array" ref="X88">_xlfn.XLOOKUP(D88&amp;I88,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!E$2:E$13000,"")</f>
         <v>2</v>
@@ -8812,7 +8860,7 @@
         <v>181</v>
       </c>
       <c r="F89">
-        <v>0</v>
+        <v>1704000</v>
       </c>
       <c r="G89">
         <v>2022</v>
@@ -8856,6 +8904,21 @@
         <f t="array" ref="R89">_xlfn.XLOOKUP(E89&amp;I89,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!D$2:D$13000,"")</f>
         <v>19</v>
       </c>
+      <c r="S89">
+        <v>0</v>
+      </c>
+      <c r="T89">
+        <v>0</v>
+      </c>
+      <c r="U89">
+        <v>0</v>
+      </c>
+      <c r="V89">
+        <v>0</v>
+      </c>
+      <c r="W89">
+        <v>0</v>
+      </c>
       <c r="X89" cm="1">
         <f t="array" ref="X89">_xlfn.XLOOKUP(D89&amp;I89,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!E$2:E$13000,"")</f>
         <v>4</v>
@@ -8934,6 +8997,21 @@
         <f t="array" ref="R90">_xlfn.XLOOKUP(E90&amp;I90,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!D$2:D$13000,"")</f>
         <v>11</v>
       </c>
+      <c r="S90">
+        <v>0</v>
+      </c>
+      <c r="T90">
+        <v>0</v>
+      </c>
+      <c r="U90">
+        <v>0</v>
+      </c>
+      <c r="V90">
+        <v>0</v>
+      </c>
+      <c r="W90">
+        <v>0</v>
+      </c>
       <c r="X90" cm="1">
         <f t="array" ref="X90">_xlfn.XLOOKUP(D90&amp;I90,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!E$2:E$13000,"")</f>
         <v>3</v>
@@ -9012,6 +9090,21 @@
         <f t="array" ref="R91">_xlfn.XLOOKUP(E91&amp;I91,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!D$2:D$13000,"")</f>
         <v>13</v>
       </c>
+      <c r="S91">
+        <v>0</v>
+      </c>
+      <c r="T91">
+        <v>0</v>
+      </c>
+      <c r="U91">
+        <v>0</v>
+      </c>
+      <c r="V91">
+        <v>0</v>
+      </c>
+      <c r="W91">
+        <v>0</v>
+      </c>
       <c r="X91" cm="1">
         <f t="array" ref="X91">_xlfn.XLOOKUP(D91&amp;I91,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!E$2:E$13000,"")</f>
         <v>4</v>
@@ -9090,6 +9183,21 @@
         <f t="array" ref="R92">_xlfn.XLOOKUP(E92&amp;I92,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!D$2:D$13000,"")</f>
         <v>17.8</v>
       </c>
+      <c r="S92">
+        <v>0</v>
+      </c>
+      <c r="T92">
+        <v>0</v>
+      </c>
+      <c r="U92">
+        <v>0</v>
+      </c>
+      <c r="V92">
+        <v>0</v>
+      </c>
+      <c r="W92">
+        <v>0</v>
+      </c>
       <c r="X92" cm="1">
         <f t="array" ref="X92">_xlfn.XLOOKUP(D92&amp;I92,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!E$2:E$13000,"")</f>
         <v>3</v>
@@ -9168,6 +9276,21 @@
         <f t="array" ref="R93">_xlfn.XLOOKUP(E93&amp;I93,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!D$2:D$13000,"")</f>
         <v>23.3</v>
       </c>
+      <c r="S93">
+        <v>0</v>
+      </c>
+      <c r="T93">
+        <v>0</v>
+      </c>
+      <c r="U93">
+        <v>0</v>
+      </c>
+      <c r="V93">
+        <v>0</v>
+      </c>
+      <c r="W93">
+        <v>0</v>
+      </c>
       <c r="X93" cm="1">
         <f t="array" ref="X93">_xlfn.XLOOKUP(D93&amp;I93,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!E$2:E$13000,"")</f>
         <v>4</v>
@@ -9246,6 +9369,21 @@
         <f t="array" ref="R94">_xlfn.XLOOKUP(E94&amp;I94,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!D$2:D$13000,"")</f>
         <v>23.7</v>
       </c>
+      <c r="S94">
+        <v>0</v>
+      </c>
+      <c r="T94">
+        <v>0</v>
+      </c>
+      <c r="U94">
+        <v>0</v>
+      </c>
+      <c r="V94">
+        <v>0</v>
+      </c>
+      <c r="W94">
+        <v>0</v>
+      </c>
       <c r="X94" cm="1">
         <f t="array" ref="X94">_xlfn.XLOOKUP(D94&amp;I94,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!E$2:E$13000,"")</f>
         <v>3</v>
@@ -9324,6 +9462,21 @@
         <f t="array" ref="R95">_xlfn.XLOOKUP(E95&amp;I95,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!D$2:D$13000,"")</f>
         <v>7.3</v>
       </c>
+      <c r="S95">
+        <v>0</v>
+      </c>
+      <c r="T95">
+        <v>0</v>
+      </c>
+      <c r="U95">
+        <v>0</v>
+      </c>
+      <c r="V95">
+        <v>0</v>
+      </c>
+      <c r="W95">
+        <v>0</v>
+      </c>
       <c r="X95" cm="1">
         <f t="array" ref="X95">_xlfn.XLOOKUP(D95&amp;I95,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!E$2:E$13000,"")</f>
         <v>3</v>
@@ -9402,6 +9555,21 @@
         <f t="array" ref="R96">_xlfn.XLOOKUP(E96&amp;I96,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!D$2:D$13000,"")</f>
         <v>22.7</v>
       </c>
+      <c r="S96">
+        <v>0</v>
+      </c>
+      <c r="T96">
+        <v>0</v>
+      </c>
+      <c r="U96">
+        <v>0</v>
+      </c>
+      <c r="V96">
+        <v>0</v>
+      </c>
+      <c r="W96">
+        <v>0</v>
+      </c>
       <c r="X96" cm="1">
         <f t="array" ref="X96">_xlfn.XLOOKUP(D96&amp;I96,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!E$2:E$13000,"")</f>
         <v>3</v>
@@ -9480,6 +9648,21 @@
         <f t="array" ref="R97">_xlfn.XLOOKUP(E97&amp;I97,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!D$2:D$13000,"")</f>
         <v>26.8</v>
       </c>
+      <c r="S97">
+        <v>0</v>
+      </c>
+      <c r="T97">
+        <v>0</v>
+      </c>
+      <c r="U97">
+        <v>0</v>
+      </c>
+      <c r="V97">
+        <v>0</v>
+      </c>
+      <c r="W97">
+        <v>0</v>
+      </c>
       <c r="X97" cm="1">
         <f t="array" ref="X97">_xlfn.XLOOKUP(D97&amp;I97,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!E$2:E$13000,"")</f>
         <v>4</v>
@@ -9558,6 +9741,21 @@
         <f t="array" ref="R98">_xlfn.XLOOKUP(E98&amp;I98,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!D$2:D$13000,"")</f>
         <v>30.5</v>
       </c>
+      <c r="S98">
+        <v>0</v>
+      </c>
+      <c r="T98">
+        <v>0</v>
+      </c>
+      <c r="U98">
+        <v>0</v>
+      </c>
+      <c r="V98">
+        <v>0</v>
+      </c>
+      <c r="W98">
+        <v>0</v>
+      </c>
       <c r="X98" cm="1">
         <f t="array" ref="X98">_xlfn.XLOOKUP(D98&amp;I98,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!E$2:E$13000,"")</f>
         <v>4</v>
@@ -9636,6 +9834,21 @@
         <f t="array" ref="R99">_xlfn.XLOOKUP(E99&amp;I99,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!D$2:D$13000,"")</f>
         <v>14.5</v>
       </c>
+      <c r="S99">
+        <v>0</v>
+      </c>
+      <c r="T99">
+        <v>0</v>
+      </c>
+      <c r="U99">
+        <v>0</v>
+      </c>
+      <c r="V99">
+        <v>0</v>
+      </c>
+      <c r="W99">
+        <v>0</v>
+      </c>
       <c r="X99" cm="1">
         <f t="array" ref="X99">_xlfn.XLOOKUP(D99&amp;I99,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!E$2:E$13000,"")</f>
         <v>4</v>
@@ -9714,6 +9927,21 @@
         <f t="array" ref="R100">_xlfn.XLOOKUP(E100&amp;I100,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!D$2:D$13000,"")</f>
         <v>21.5</v>
       </c>
+      <c r="S100">
+        <v>0</v>
+      </c>
+      <c r="T100">
+        <v>0</v>
+      </c>
+      <c r="U100">
+        <v>0</v>
+      </c>
+      <c r="V100">
+        <v>0</v>
+      </c>
+      <c r="W100">
+        <v>0</v>
+      </c>
       <c r="X100" cm="1">
         <f t="array" ref="X100">_xlfn.XLOOKUP(D100&amp;I100,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!E$2:E$13000,"")</f>
         <v>3</v>
@@ -9792,6 +10020,21 @@
         <f t="array" ref="R101">_xlfn.XLOOKUP(E101&amp;I101,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!D$2:D$13000,"")</f>
         <v>14.3</v>
       </c>
+      <c r="S101">
+        <v>0</v>
+      </c>
+      <c r="T101">
+        <v>0</v>
+      </c>
+      <c r="U101">
+        <v>0</v>
+      </c>
+      <c r="V101">
+        <v>0</v>
+      </c>
+      <c r="W101">
+        <v>0</v>
+      </c>
       <c r="X101" cm="1">
         <f t="array" ref="X101">_xlfn.XLOOKUP(D101&amp;I101,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!E$2:E$13000,"")</f>
         <v>3</v>
@@ -9870,6 +10113,21 @@
         <f t="array" ref="R102">_xlfn.XLOOKUP(E102&amp;I102,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!D$2:D$13000,"")</f>
         <v>11.8</v>
       </c>
+      <c r="S102">
+        <v>0</v>
+      </c>
+      <c r="T102">
+        <v>0</v>
+      </c>
+      <c r="U102">
+        <v>0</v>
+      </c>
+      <c r="V102">
+        <v>0</v>
+      </c>
+      <c r="W102">
+        <v>0</v>
+      </c>
       <c r="X102" cm="1">
         <f t="array" ref="X102">_xlfn.XLOOKUP(D102&amp;I102,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!E$2:E$13000,"")</f>
         <v>4</v>
@@ -9948,6 +10206,21 @@
         <f t="array" ref="R103">_xlfn.XLOOKUP(E103&amp;I103,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!D$2:D$13000,"")</f>
         <v>27.5</v>
       </c>
+      <c r="S103">
+        <v>0</v>
+      </c>
+      <c r="T103">
+        <v>0</v>
+      </c>
+      <c r="U103">
+        <v>0</v>
+      </c>
+      <c r="V103">
+        <v>0</v>
+      </c>
+      <c r="W103">
+        <v>0</v>
+      </c>
       <c r="X103" cm="1">
         <f t="array" ref="X103">_xlfn.XLOOKUP(D103&amp;I103,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!E$2:E$13000,"")</f>
         <v>2</v>
@@ -10026,6 +10299,21 @@
         <f t="array" ref="R104">_xlfn.XLOOKUP(E104&amp;I104,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!D$2:D$13000,"")</f>
         <v>25.3</v>
       </c>
+      <c r="S104">
+        <v>0</v>
+      </c>
+      <c r="T104">
+        <v>0</v>
+      </c>
+      <c r="U104">
+        <v>0</v>
+      </c>
+      <c r="V104">
+        <v>0</v>
+      </c>
+      <c r="W104">
+        <v>0</v>
+      </c>
       <c r="X104" cm="1">
         <f t="array" ref="X104">_xlfn.XLOOKUP(D104&amp;I104,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!E$2:E$13000,"")</f>
         <v>4</v>
@@ -10103,6 +10391,21 @@
       <c r="R105" cm="1">
         <f t="array" ref="R105">_xlfn.XLOOKUP(E105&amp;I105,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!D$2:D$13000,"")</f>
         <v>30.3</v>
+      </c>
+      <c r="S105">
+        <v>0</v>
+      </c>
+      <c r="T105">
+        <v>0</v>
+      </c>
+      <c r="U105">
+        <v>0</v>
+      </c>
+      <c r="V105">
+        <v>0</v>
+      </c>
+      <c r="W105">
+        <v>0</v>
       </c>
       <c r="X105" cm="1">
         <f t="array" ref="X105">_xlfn.XLOOKUP(D105&amp;I105,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!E$2:E$13000,"")</f>
@@ -10130,10 +10433,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF262906-C2E8-EB40-9ABF-94137CE271DB}">
-  <dimension ref="A1:F523"/>
+  <dimension ref="A1:F654"/>
   <sheetViews>
-    <sheetView topLeftCell="A452" workbookViewId="0">
-      <selection activeCell="A468" sqref="A468"/>
+    <sheetView topLeftCell="A551" workbookViewId="0">
+      <selection activeCell="A524" sqref="A524:F654"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -20598,6 +20901,2626 @@
         <v>2</v>
       </c>
     </row>
+    <row r="524" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A524" t="s">
+        <v>106</v>
+      </c>
+      <c r="B524">
+        <v>6</v>
+      </c>
+      <c r="C524">
+        <v>32.799999999999997</v>
+      </c>
+      <c r="D524">
+        <v>14.8</v>
+      </c>
+      <c r="E524">
+        <v>4</v>
+      </c>
+      <c r="F524">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="525" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A525" t="s">
+        <v>119</v>
+      </c>
+      <c r="B525">
+        <v>6</v>
+      </c>
+      <c r="C525">
+        <v>15.2</v>
+      </c>
+      <c r="D525">
+        <v>38</v>
+      </c>
+      <c r="E525">
+        <v>1</v>
+      </c>
+      <c r="F525">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="526" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A526" t="s">
+        <v>91</v>
+      </c>
+      <c r="B526">
+        <v>6</v>
+      </c>
+      <c r="C526">
+        <v>48.4</v>
+      </c>
+      <c r="D526">
+        <v>11</v>
+      </c>
+      <c r="E526">
+        <v>5</v>
+      </c>
+      <c r="F526">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="527" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A527" t="s">
+        <v>102</v>
+      </c>
+      <c r="B527">
+        <v>6</v>
+      </c>
+      <c r="C527">
+        <v>37.4</v>
+      </c>
+      <c r="D527">
+        <v>27.4</v>
+      </c>
+      <c r="E527">
+        <v>3</v>
+      </c>
+      <c r="F527">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="528" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A528" t="s">
+        <v>112</v>
+      </c>
+      <c r="B528">
+        <v>6</v>
+      </c>
+      <c r="C528">
+        <v>32</v>
+      </c>
+      <c r="D528">
+        <v>31.2</v>
+      </c>
+      <c r="E528">
+        <v>3</v>
+      </c>
+      <c r="F528">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="529" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A529" t="s">
+        <v>96</v>
+      </c>
+      <c r="B529">
+        <v>6</v>
+      </c>
+      <c r="C529">
+        <v>23.2</v>
+      </c>
+      <c r="D529">
+        <v>28.6</v>
+      </c>
+      <c r="E529">
+        <v>1</v>
+      </c>
+      <c r="F529">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="530" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A530" t="s">
+        <v>50</v>
+      </c>
+      <c r="B530">
+        <v>6</v>
+      </c>
+      <c r="C530">
+        <v>32</v>
+      </c>
+      <c r="D530">
+        <v>30.6</v>
+      </c>
+      <c r="E530">
+        <v>3</v>
+      </c>
+      <c r="F530">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="531" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A531" t="s">
+        <v>120</v>
+      </c>
+      <c r="B531">
+        <v>6</v>
+      </c>
+      <c r="C531">
+        <v>34.6</v>
+      </c>
+      <c r="D531">
+        <v>29.8</v>
+      </c>
+      <c r="E531">
+        <v>2</v>
+      </c>
+      <c r="F531">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="532" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A532" t="s">
+        <v>121</v>
+      </c>
+      <c r="B532">
+        <v>6</v>
+      </c>
+      <c r="C532">
+        <v>32.299999999999997</v>
+      </c>
+      <c r="D532">
+        <v>30</v>
+      </c>
+      <c r="E532">
+        <v>1</v>
+      </c>
+      <c r="F532">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="533" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A533" t="s">
+        <v>122</v>
+      </c>
+      <c r="B533">
+        <v>6</v>
+      </c>
+      <c r="C533">
+        <v>22.4</v>
+      </c>
+      <c r="D533">
+        <v>21.6</v>
+      </c>
+      <c r="E533">
+        <v>3</v>
+      </c>
+      <c r="F533">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="534" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A534" t="s">
+        <v>123</v>
+      </c>
+      <c r="B534">
+        <v>6</v>
+      </c>
+      <c r="C534">
+        <v>27.6</v>
+      </c>
+      <c r="D534">
+        <v>33.6</v>
+      </c>
+      <c r="E534">
+        <v>2</v>
+      </c>
+      <c r="F534">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="535" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A535" t="s">
+        <v>98</v>
+      </c>
+      <c r="B535">
+        <v>6</v>
+      </c>
+      <c r="C535">
+        <v>37.4</v>
+      </c>
+      <c r="D535">
+        <v>20.6</v>
+      </c>
+      <c r="E535">
+        <v>3</v>
+      </c>
+      <c r="F535">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="536" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A536" t="s">
+        <v>27</v>
+      </c>
+      <c r="B536">
+        <v>6</v>
+      </c>
+      <c r="C536">
+        <v>24.6</v>
+      </c>
+      <c r="D536">
+        <v>19</v>
+      </c>
+      <c r="E536">
+        <v>3</v>
+      </c>
+      <c r="F536">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="537" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A537" t="s">
+        <v>124</v>
+      </c>
+      <c r="B537">
+        <v>6</v>
+      </c>
+      <c r="C537">
+        <v>23.4</v>
+      </c>
+      <c r="D537">
+        <v>28.6</v>
+      </c>
+      <c r="E537">
+        <v>2</v>
+      </c>
+      <c r="F537">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="538" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A538" t="s">
+        <v>125</v>
+      </c>
+      <c r="B538">
+        <v>6</v>
+      </c>
+      <c r="C538">
+        <v>30.6</v>
+      </c>
+      <c r="D538">
+        <v>41.6</v>
+      </c>
+      <c r="E538">
+        <v>2</v>
+      </c>
+      <c r="F538">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="539" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A539" t="s">
+        <v>126</v>
+      </c>
+      <c r="B539">
+        <v>6</v>
+      </c>
+      <c r="C539">
+        <v>28.2</v>
+      </c>
+      <c r="D539">
+        <v>31.4</v>
+      </c>
+      <c r="E539">
+        <v>2</v>
+      </c>
+      <c r="F539">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="540" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A540" t="s">
+        <v>97</v>
+      </c>
+      <c r="B540">
+        <v>6</v>
+      </c>
+      <c r="C540">
+        <v>34.4</v>
+      </c>
+      <c r="D540">
+        <v>26.4</v>
+      </c>
+      <c r="E540">
+        <v>4</v>
+      </c>
+      <c r="F540">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="541" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A541" t="s">
+        <v>127</v>
+      </c>
+      <c r="B541">
+        <v>6</v>
+      </c>
+      <c r="C541">
+        <v>25.8</v>
+      </c>
+      <c r="D541">
+        <v>22</v>
+      </c>
+      <c r="E541">
+        <v>3</v>
+      </c>
+      <c r="F541">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="542" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A542" t="s">
+        <v>61</v>
+      </c>
+      <c r="B542">
+        <v>6</v>
+      </c>
+      <c r="C542">
+        <v>28</v>
+      </c>
+      <c r="D542">
+        <v>33.4</v>
+      </c>
+      <c r="E542">
+        <v>1</v>
+      </c>
+      <c r="F542">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="543" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A543" t="s">
+        <v>82</v>
+      </c>
+      <c r="B543">
+        <v>6</v>
+      </c>
+      <c r="C543">
+        <v>25.8</v>
+      </c>
+      <c r="D543">
+        <v>46.3</v>
+      </c>
+      <c r="E543">
+        <v>1</v>
+      </c>
+      <c r="F543">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="544" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A544" t="s">
+        <v>57</v>
+      </c>
+      <c r="B544">
+        <v>6</v>
+      </c>
+      <c r="C544">
+        <v>40.200000000000003</v>
+      </c>
+      <c r="D544">
+        <v>20.6</v>
+      </c>
+      <c r="E544">
+        <v>4</v>
+      </c>
+      <c r="F544">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="545" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A545" t="s">
+        <v>87</v>
+      </c>
+      <c r="B545">
+        <v>6</v>
+      </c>
+      <c r="C545">
+        <v>41</v>
+      </c>
+      <c r="D545">
+        <v>21.4</v>
+      </c>
+      <c r="E545">
+        <v>5</v>
+      </c>
+      <c r="F545">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="546" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A546" t="s">
+        <v>128</v>
+      </c>
+      <c r="B546">
+        <v>6</v>
+      </c>
+      <c r="C546">
+        <v>36.4</v>
+      </c>
+      <c r="D546">
+        <v>27</v>
+      </c>
+      <c r="E546">
+        <v>5</v>
+      </c>
+      <c r="F546">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="547" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A547" t="s">
+        <v>107</v>
+      </c>
+      <c r="B547">
+        <v>6</v>
+      </c>
+      <c r="C547">
+        <v>13.4</v>
+      </c>
+      <c r="D547">
+        <v>43.2</v>
+      </c>
+      <c r="E547">
+        <v>0</v>
+      </c>
+      <c r="F547">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="548" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A548" t="s">
+        <v>59</v>
+      </c>
+      <c r="B548">
+        <v>6</v>
+      </c>
+      <c r="C548">
+        <v>10.8</v>
+      </c>
+      <c r="D548">
+        <v>41</v>
+      </c>
+      <c r="E548">
+        <v>0</v>
+      </c>
+      <c r="F548">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="549" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A549" t="s">
+        <v>80</v>
+      </c>
+      <c r="B549">
+        <v>6</v>
+      </c>
+      <c r="C549">
+        <v>15.2</v>
+      </c>
+      <c r="D549">
+        <v>32.700000000000003</v>
+      </c>
+      <c r="E549">
+        <v>2</v>
+      </c>
+      <c r="F549">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="550" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A550" t="s">
+        <v>129</v>
+      </c>
+      <c r="B550">
+        <v>6</v>
+      </c>
+      <c r="C550">
+        <v>35</v>
+      </c>
+      <c r="D550">
+        <v>19</v>
+      </c>
+      <c r="E550">
+        <v>4</v>
+      </c>
+      <c r="F550">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="551" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A551" t="s">
+        <v>28</v>
+      </c>
+      <c r="B551">
+        <v>6</v>
+      </c>
+      <c r="C551">
+        <v>35.200000000000003</v>
+      </c>
+      <c r="D551">
+        <v>20.6</v>
+      </c>
+      <c r="E551">
+        <v>3</v>
+      </c>
+      <c r="F551">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="552" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A552" t="s">
+        <v>130</v>
+      </c>
+      <c r="B552">
+        <v>6</v>
+      </c>
+      <c r="C552">
+        <v>28.8</v>
+      </c>
+      <c r="D552">
+        <v>33.4</v>
+      </c>
+      <c r="E552">
+        <v>3</v>
+      </c>
+      <c r="F552">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="553" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A553" t="s">
+        <v>52</v>
+      </c>
+      <c r="B553">
+        <v>6</v>
+      </c>
+      <c r="C553">
+        <v>32.200000000000003</v>
+      </c>
+      <c r="D553">
+        <v>27</v>
+      </c>
+      <c r="E553">
+        <v>3</v>
+      </c>
+      <c r="F553">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="554" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A554" t="s">
+        <v>81</v>
+      </c>
+      <c r="B554">
+        <v>6</v>
+      </c>
+      <c r="C554">
+        <v>31.8</v>
+      </c>
+      <c r="D554">
+        <v>29.3</v>
+      </c>
+      <c r="E554">
+        <v>2</v>
+      </c>
+      <c r="F554">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="555" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A555" t="s">
+        <v>131</v>
+      </c>
+      <c r="B555">
+        <v>6</v>
+      </c>
+      <c r="C555">
+        <v>17.8</v>
+      </c>
+      <c r="D555">
+        <v>39.5</v>
+      </c>
+      <c r="E555">
+        <v>2</v>
+      </c>
+      <c r="F555">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="556" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A556" t="s">
+        <v>115</v>
+      </c>
+      <c r="B556">
+        <v>6</v>
+      </c>
+      <c r="C556">
+        <v>34.200000000000003</v>
+      </c>
+      <c r="D556">
+        <v>21.2</v>
+      </c>
+      <c r="E556">
+        <v>4</v>
+      </c>
+      <c r="F556">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="557" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A557" t="s">
+        <v>132</v>
+      </c>
+      <c r="B557">
+        <v>6</v>
+      </c>
+      <c r="C557">
+        <v>24.5</v>
+      </c>
+      <c r="D557">
+        <v>26.5</v>
+      </c>
+      <c r="E557">
+        <v>1</v>
+      </c>
+      <c r="F557">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="558" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A558" t="s">
+        <v>32</v>
+      </c>
+      <c r="B558">
+        <v>6</v>
+      </c>
+      <c r="C558">
+        <v>39</v>
+      </c>
+      <c r="D558">
+        <v>10.8</v>
+      </c>
+      <c r="E558">
+        <v>5</v>
+      </c>
+      <c r="F558">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="559" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A559" t="s">
+        <v>111</v>
+      </c>
+      <c r="B559">
+        <v>6</v>
+      </c>
+      <c r="C559">
+        <v>37.799999999999997</v>
+      </c>
+      <c r="D559">
+        <v>28.2</v>
+      </c>
+      <c r="E559">
+        <v>3</v>
+      </c>
+      <c r="F559">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="560" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A560" t="s">
+        <v>133</v>
+      </c>
+      <c r="B560">
+        <v>6</v>
+      </c>
+      <c r="C560">
+        <v>27.6</v>
+      </c>
+      <c r="D560">
+        <v>33.4</v>
+      </c>
+      <c r="E560">
+        <v>1</v>
+      </c>
+      <c r="F560">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="561" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A561" t="s">
+        <v>86</v>
+      </c>
+      <c r="B561">
+        <v>6</v>
+      </c>
+      <c r="C561">
+        <v>16.2</v>
+      </c>
+      <c r="D561">
+        <v>29.6</v>
+      </c>
+      <c r="E561">
+        <v>2</v>
+      </c>
+      <c r="F561">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="562" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A562" t="s">
+        <v>134</v>
+      </c>
+      <c r="B562">
+        <v>6</v>
+      </c>
+      <c r="C562">
+        <v>17.399999999999999</v>
+      </c>
+      <c r="D562">
+        <v>45.4</v>
+      </c>
+      <c r="E562">
+        <v>1</v>
+      </c>
+      <c r="F562">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="563" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A563" t="s">
+        <v>40</v>
+      </c>
+      <c r="B563">
+        <v>6</v>
+      </c>
+      <c r="C563">
+        <v>31</v>
+      </c>
+      <c r="D563">
+        <v>34</v>
+      </c>
+      <c r="E563">
+        <v>2</v>
+      </c>
+      <c r="F563">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="564" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A564" t="s">
+        <v>23</v>
+      </c>
+      <c r="B564">
+        <v>6</v>
+      </c>
+      <c r="C564">
+        <v>29.4</v>
+      </c>
+      <c r="D564">
+        <v>8.4</v>
+      </c>
+      <c r="E564">
+        <v>4</v>
+      </c>
+      <c r="F564">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="565" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A565" t="s">
+        <v>41</v>
+      </c>
+      <c r="B565">
+        <v>6</v>
+      </c>
+      <c r="C565">
+        <v>27.2</v>
+      </c>
+      <c r="D565">
+        <v>30.4</v>
+      </c>
+      <c r="E565">
+        <v>3</v>
+      </c>
+      <c r="F565">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="566" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A566" t="s">
+        <v>135</v>
+      </c>
+      <c r="B566">
+        <v>6</v>
+      </c>
+      <c r="C566">
+        <v>16.399999999999999</v>
+      </c>
+      <c r="D566">
+        <v>10</v>
+      </c>
+      <c r="E566">
+        <v>3</v>
+      </c>
+      <c r="F566">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="567" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A567" t="s">
+        <v>136</v>
+      </c>
+      <c r="B567">
+        <v>6</v>
+      </c>
+      <c r="C567">
+        <v>26</v>
+      </c>
+      <c r="D567">
+        <v>14.4</v>
+      </c>
+      <c r="E567">
+        <v>3</v>
+      </c>
+      <c r="F567">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="568" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A568" t="s">
+        <v>137</v>
+      </c>
+      <c r="B568">
+        <v>6</v>
+      </c>
+      <c r="C568">
+        <v>44.8</v>
+      </c>
+      <c r="D568">
+        <v>13.8</v>
+      </c>
+      <c r="E568">
+        <v>4</v>
+      </c>
+      <c r="F568">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="569" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A569" t="s">
+        <v>138</v>
+      </c>
+      <c r="B569">
+        <v>6</v>
+      </c>
+      <c r="C569">
+        <v>41.6</v>
+      </c>
+      <c r="D569">
+        <v>24</v>
+      </c>
+      <c r="E569">
+        <v>5</v>
+      </c>
+      <c r="F569">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="570" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A570" t="s">
+        <v>93</v>
+      </c>
+      <c r="B570">
+        <v>6</v>
+      </c>
+      <c r="C570">
+        <v>32.4</v>
+      </c>
+      <c r="D570">
+        <v>18.2</v>
+      </c>
+      <c r="E570">
+        <v>4</v>
+      </c>
+      <c r="F570">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="571" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A571" t="s">
+        <v>139</v>
+      </c>
+      <c r="B571">
+        <v>6</v>
+      </c>
+      <c r="C571">
+        <v>27.8</v>
+      </c>
+      <c r="D571">
+        <v>30.2</v>
+      </c>
+      <c r="E571">
+        <v>2</v>
+      </c>
+      <c r="F571">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="572" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A572" t="s">
+        <v>108</v>
+      </c>
+      <c r="B572">
+        <v>6</v>
+      </c>
+      <c r="C572">
+        <v>28.8</v>
+      </c>
+      <c r="D572">
+        <v>14.8</v>
+      </c>
+      <c r="E572">
+        <v>4</v>
+      </c>
+      <c r="F572">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="573" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A573" t="s">
+        <v>140</v>
+      </c>
+      <c r="B573">
+        <v>6</v>
+      </c>
+      <c r="C573">
+        <v>29</v>
+      </c>
+      <c r="D573">
+        <v>22.8</v>
+      </c>
+      <c r="E573">
+        <v>4</v>
+      </c>
+      <c r="F573">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="574" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A574" t="s">
+        <v>141</v>
+      </c>
+      <c r="B574">
+        <v>6</v>
+      </c>
+      <c r="C574">
+        <v>27.5</v>
+      </c>
+      <c r="D574">
+        <v>38.799999999999997</v>
+      </c>
+      <c r="E574">
+        <v>1</v>
+      </c>
+      <c r="F574">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="575" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A575" t="s">
+        <v>142</v>
+      </c>
+      <c r="B575">
+        <v>6</v>
+      </c>
+      <c r="C575">
+        <v>25.6</v>
+      </c>
+      <c r="D575">
+        <v>20.399999999999999</v>
+      </c>
+      <c r="E575">
+        <v>2</v>
+      </c>
+      <c r="F575">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="576" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A576" t="s">
+        <v>143</v>
+      </c>
+      <c r="B576">
+        <v>6</v>
+      </c>
+      <c r="C576">
+        <v>20.2</v>
+      </c>
+      <c r="D576">
+        <v>36.799999999999997</v>
+      </c>
+      <c r="E576">
+        <v>2</v>
+      </c>
+      <c r="F576">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="577" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A577" t="s">
+        <v>89</v>
+      </c>
+      <c r="B577">
+        <v>6</v>
+      </c>
+      <c r="C577">
+        <v>26.4</v>
+      </c>
+      <c r="D577">
+        <v>23.4</v>
+      </c>
+      <c r="E577">
+        <v>2</v>
+      </c>
+      <c r="F577">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="578" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A578" t="s">
+        <v>114</v>
+      </c>
+      <c r="B578">
+        <v>6</v>
+      </c>
+      <c r="C578">
+        <v>35.6</v>
+      </c>
+      <c r="D578">
+        <v>14.8</v>
+      </c>
+      <c r="E578">
+        <v>4</v>
+      </c>
+      <c r="F578">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="579" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A579" t="s">
+        <v>100</v>
+      </c>
+      <c r="B579">
+        <v>6</v>
+      </c>
+      <c r="C579">
+        <v>29.4</v>
+      </c>
+      <c r="D579">
+        <v>16.2</v>
+      </c>
+      <c r="E579">
+        <v>3</v>
+      </c>
+      <c r="F579">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="580" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A580" t="s">
+        <v>144</v>
+      </c>
+      <c r="B580">
+        <v>6</v>
+      </c>
+      <c r="C580">
+        <v>35</v>
+      </c>
+      <c r="D580">
+        <v>21</v>
+      </c>
+      <c r="E580">
+        <v>4</v>
+      </c>
+      <c r="F580">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="581" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A581" t="s">
+        <v>145</v>
+      </c>
+      <c r="B581">
+        <v>6</v>
+      </c>
+      <c r="C581">
+        <v>10.6</v>
+      </c>
+      <c r="D581">
+        <v>29.6</v>
+      </c>
+      <c r="E581">
+        <v>1</v>
+      </c>
+      <c r="F581">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="582" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A582" t="s">
+        <v>146</v>
+      </c>
+      <c r="B582">
+        <v>6</v>
+      </c>
+      <c r="C582">
+        <v>34.4</v>
+      </c>
+      <c r="D582">
+        <v>26.2</v>
+      </c>
+      <c r="E582">
+        <v>4</v>
+      </c>
+      <c r="F582">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="583" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A583" t="s">
+        <v>147</v>
+      </c>
+      <c r="B583">
+        <v>6</v>
+      </c>
+      <c r="C583">
+        <v>35</v>
+      </c>
+      <c r="D583">
+        <v>20.5</v>
+      </c>
+      <c r="E583">
+        <v>2</v>
+      </c>
+      <c r="F583">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="584" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A584" t="s">
+        <v>148</v>
+      </c>
+      <c r="B584">
+        <v>6</v>
+      </c>
+      <c r="C584">
+        <v>19.600000000000001</v>
+      </c>
+      <c r="D584">
+        <v>25.4</v>
+      </c>
+      <c r="E584">
+        <v>2</v>
+      </c>
+      <c r="F584">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="585" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A585" t="s">
+        <v>38</v>
+      </c>
+      <c r="B585">
+        <v>6</v>
+      </c>
+      <c r="C585">
+        <v>45.4</v>
+      </c>
+      <c r="D585">
+        <v>11.6</v>
+      </c>
+      <c r="E585">
+        <v>5</v>
+      </c>
+      <c r="F585">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="586" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A586" t="s">
+        <v>29</v>
+      </c>
+      <c r="B586">
+        <v>6</v>
+      </c>
+      <c r="C586">
+        <v>27</v>
+      </c>
+      <c r="D586">
+        <v>22.6</v>
+      </c>
+      <c r="E586">
+        <v>2</v>
+      </c>
+      <c r="F586">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="587" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A587" t="s">
+        <v>149</v>
+      </c>
+      <c r="B587">
+        <v>6</v>
+      </c>
+      <c r="C587">
+        <v>33</v>
+      </c>
+      <c r="D587">
+        <v>29</v>
+      </c>
+      <c r="E587">
+        <v>3</v>
+      </c>
+      <c r="F587">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="588" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A588" t="s">
+        <v>150</v>
+      </c>
+      <c r="B588">
+        <v>6</v>
+      </c>
+      <c r="C588">
+        <v>38.6</v>
+      </c>
+      <c r="D588">
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="E588">
+        <v>4</v>
+      </c>
+      <c r="F588">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="589" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A589" t="s">
+        <v>151</v>
+      </c>
+      <c r="B589">
+        <v>6</v>
+      </c>
+      <c r="C589">
+        <v>37.200000000000003</v>
+      </c>
+      <c r="D589">
+        <v>11.8</v>
+      </c>
+      <c r="E589">
+        <v>5</v>
+      </c>
+      <c r="F589">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="590" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A590" t="s">
+        <v>113</v>
+      </c>
+      <c r="B590">
+        <v>6</v>
+      </c>
+      <c r="C590">
+        <v>38.200000000000003</v>
+      </c>
+      <c r="D590">
+        <v>21.8</v>
+      </c>
+      <c r="E590">
+        <v>4</v>
+      </c>
+      <c r="F590">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="591" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A591" t="s">
+        <v>94</v>
+      </c>
+      <c r="B591">
+        <v>6</v>
+      </c>
+      <c r="C591">
+        <v>26.8</v>
+      </c>
+      <c r="D591">
+        <v>24.8</v>
+      </c>
+      <c r="E591">
+        <v>2</v>
+      </c>
+      <c r="F591">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="592" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A592" t="s">
+        <v>152</v>
+      </c>
+      <c r="B592">
+        <v>6</v>
+      </c>
+      <c r="C592">
+        <v>13.3</v>
+      </c>
+      <c r="D592">
+        <v>21</v>
+      </c>
+      <c r="E592">
+        <v>1</v>
+      </c>
+      <c r="F592">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="593" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A593" t="s">
+        <v>22</v>
+      </c>
+      <c r="B593">
+        <v>6</v>
+      </c>
+      <c r="C593">
+        <v>31.4</v>
+      </c>
+      <c r="D593">
+        <v>32.6</v>
+      </c>
+      <c r="E593">
+        <v>2</v>
+      </c>
+      <c r="F593">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="594" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A594" t="s">
+        <v>44</v>
+      </c>
+      <c r="B594">
+        <v>6</v>
+      </c>
+      <c r="C594">
+        <v>24.4</v>
+      </c>
+      <c r="D594">
+        <v>31.2</v>
+      </c>
+      <c r="E594">
+        <v>2</v>
+      </c>
+      <c r="F594">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="595" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A595" t="s">
+        <v>153</v>
+      </c>
+      <c r="B595">
+        <v>6</v>
+      </c>
+      <c r="C595">
+        <v>20.399999999999999</v>
+      </c>
+      <c r="D595">
+        <v>22</v>
+      </c>
+      <c r="E595">
+        <v>2</v>
+      </c>
+      <c r="F595">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="596" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A596" t="s">
+        <v>83</v>
+      </c>
+      <c r="B596">
+        <v>6</v>
+      </c>
+      <c r="C596">
+        <v>14</v>
+      </c>
+      <c r="D596">
+        <v>32.299999999999997</v>
+      </c>
+      <c r="E596">
+        <v>1</v>
+      </c>
+      <c r="F596">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="597" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A597" t="s">
+        <v>154</v>
+      </c>
+      <c r="B597">
+        <v>6</v>
+      </c>
+      <c r="C597">
+        <v>45.4</v>
+      </c>
+      <c r="D597">
+        <v>33.6</v>
+      </c>
+      <c r="E597">
+        <v>4</v>
+      </c>
+      <c r="F597">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="598" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A598" t="s">
+        <v>189</v>
+      </c>
+      <c r="B598">
+        <v>6</v>
+      </c>
+      <c r="C598">
+        <v>32.799999999999997</v>
+      </c>
+      <c r="D598">
+        <v>15.4</v>
+      </c>
+      <c r="E598">
+        <v>4</v>
+      </c>
+      <c r="F598">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="599" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A599" t="s">
+        <v>155</v>
+      </c>
+      <c r="B599">
+        <v>6</v>
+      </c>
+      <c r="C599">
+        <v>34.299999999999997</v>
+      </c>
+      <c r="D599">
+        <v>36.299999999999997</v>
+      </c>
+      <c r="E599">
+        <v>3</v>
+      </c>
+      <c r="F599">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="600" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A600" t="s">
+        <v>156</v>
+      </c>
+      <c r="B600">
+        <v>6</v>
+      </c>
+      <c r="C600">
+        <v>31.6</v>
+      </c>
+      <c r="D600">
+        <v>35.6</v>
+      </c>
+      <c r="E600">
+        <v>1</v>
+      </c>
+      <c r="F600">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="601" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A601" t="s">
+        <v>30</v>
+      </c>
+      <c r="B601">
+        <v>6</v>
+      </c>
+      <c r="C601">
+        <v>19.8</v>
+      </c>
+      <c r="D601">
+        <v>24.8</v>
+      </c>
+      <c r="E601">
+        <v>1</v>
+      </c>
+      <c r="F601">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="602" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A602" t="s">
+        <v>46</v>
+      </c>
+      <c r="B602">
+        <v>6</v>
+      </c>
+      <c r="C602">
+        <v>25</v>
+      </c>
+      <c r="D602">
+        <v>24</v>
+      </c>
+      <c r="E602">
+        <v>2</v>
+      </c>
+      <c r="F602">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="603" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A603" t="s">
+        <v>157</v>
+      </c>
+      <c r="B603">
+        <v>6</v>
+      </c>
+      <c r="C603">
+        <v>28.8</v>
+      </c>
+      <c r="D603">
+        <v>42</v>
+      </c>
+      <c r="E603">
+        <v>2</v>
+      </c>
+      <c r="F603">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="604" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A604" t="s">
+        <v>26</v>
+      </c>
+      <c r="B604">
+        <v>6</v>
+      </c>
+      <c r="C604">
+        <v>48.8</v>
+      </c>
+      <c r="D604">
+        <v>14.8</v>
+      </c>
+      <c r="E604">
+        <v>5</v>
+      </c>
+      <c r="F604">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="605" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A605" t="s">
+        <v>36</v>
+      </c>
+      <c r="B605">
+        <v>6</v>
+      </c>
+      <c r="C605">
+        <v>37</v>
+      </c>
+      <c r="D605">
+        <v>25.2</v>
+      </c>
+      <c r="E605">
+        <v>3</v>
+      </c>
+      <c r="F605">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="606" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A606" t="s">
+        <v>56</v>
+      </c>
+      <c r="B606">
+        <v>6</v>
+      </c>
+      <c r="C606">
+        <v>47.8</v>
+      </c>
+      <c r="D606">
+        <v>23.3</v>
+      </c>
+      <c r="E606">
+        <v>4</v>
+      </c>
+      <c r="F606">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="607" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A607" t="s">
+        <v>158</v>
+      </c>
+      <c r="B607">
+        <v>6</v>
+      </c>
+      <c r="C607">
+        <v>21.6</v>
+      </c>
+      <c r="D607">
+        <v>27.2</v>
+      </c>
+      <c r="E607">
+        <v>2</v>
+      </c>
+      <c r="F607">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="608" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A608" t="s">
+        <v>49</v>
+      </c>
+      <c r="B608">
+        <v>6</v>
+      </c>
+      <c r="C608">
+        <v>40.6</v>
+      </c>
+      <c r="D608">
+        <v>30.2</v>
+      </c>
+      <c r="E608">
+        <v>4</v>
+      </c>
+      <c r="F608">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="609" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A609" t="s">
+        <v>42</v>
+      </c>
+      <c r="B609">
+        <v>6</v>
+      </c>
+      <c r="C609">
+        <v>33.4</v>
+      </c>
+      <c r="D609">
+        <v>27.2</v>
+      </c>
+      <c r="E609">
+        <v>3</v>
+      </c>
+      <c r="F609">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="610" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A610" t="s">
+        <v>34</v>
+      </c>
+      <c r="B610">
+        <v>6</v>
+      </c>
+      <c r="C610">
+        <v>34.4</v>
+      </c>
+      <c r="D610">
+        <v>14.8</v>
+      </c>
+      <c r="E610">
+        <v>5</v>
+      </c>
+      <c r="F610">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="611" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A611" t="s">
+        <v>51</v>
+      </c>
+      <c r="B611">
+        <v>6</v>
+      </c>
+      <c r="C611">
+        <v>33</v>
+      </c>
+      <c r="D611">
+        <v>25.6</v>
+      </c>
+      <c r="E611">
+        <v>3</v>
+      </c>
+      <c r="F611">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="612" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A612" t="s">
+        <v>43</v>
+      </c>
+      <c r="B612">
+        <v>6</v>
+      </c>
+      <c r="C612">
+        <v>32.799999999999997</v>
+      </c>
+      <c r="D612">
+        <v>20.6</v>
+      </c>
+      <c r="E612">
+        <v>3</v>
+      </c>
+      <c r="F612">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="613" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A613" t="s">
+        <v>159</v>
+      </c>
+      <c r="B613">
+        <v>6</v>
+      </c>
+      <c r="C613">
+        <v>30.8</v>
+      </c>
+      <c r="D613">
+        <v>31</v>
+      </c>
+      <c r="E613">
+        <v>3</v>
+      </c>
+      <c r="F613">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="614" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A614" t="s">
+        <v>160</v>
+      </c>
+      <c r="B614">
+        <v>6</v>
+      </c>
+      <c r="C614">
+        <v>24.8</v>
+      </c>
+      <c r="D614">
+        <v>23.6</v>
+      </c>
+      <c r="E614">
+        <v>3</v>
+      </c>
+      <c r="F614">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="615" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A615" t="s">
+        <v>161</v>
+      </c>
+      <c r="B615">
+        <v>6</v>
+      </c>
+      <c r="C615">
+        <v>19</v>
+      </c>
+      <c r="D615">
+        <v>25.8</v>
+      </c>
+      <c r="E615">
+        <v>2</v>
+      </c>
+      <c r="F615">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="616" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A616" t="s">
+        <v>162</v>
+      </c>
+      <c r="B616">
+        <v>6</v>
+      </c>
+      <c r="C616">
+        <v>26</v>
+      </c>
+      <c r="D616">
+        <v>15.8</v>
+      </c>
+      <c r="E616">
+        <v>3</v>
+      </c>
+      <c r="F616">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="617" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A617" t="s">
+        <v>163</v>
+      </c>
+      <c r="B617">
+        <v>6</v>
+      </c>
+      <c r="C617">
+        <v>38.5</v>
+      </c>
+      <c r="D617">
+        <v>25.5</v>
+      </c>
+      <c r="E617">
+        <v>2</v>
+      </c>
+      <c r="F617">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="618" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A618" t="s">
+        <v>164</v>
+      </c>
+      <c r="B618">
+        <v>6</v>
+      </c>
+      <c r="C618">
+        <v>35</v>
+      </c>
+      <c r="D618">
+        <v>18.8</v>
+      </c>
+      <c r="E618">
+        <v>4</v>
+      </c>
+      <c r="F618">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="619" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A619" t="s">
+        <v>92</v>
+      </c>
+      <c r="B619">
+        <v>6</v>
+      </c>
+      <c r="C619">
+        <v>35.6</v>
+      </c>
+      <c r="D619">
+        <v>27.2</v>
+      </c>
+      <c r="E619">
+        <v>3</v>
+      </c>
+      <c r="F619">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="620" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A620" t="s">
+        <v>165</v>
+      </c>
+      <c r="B620">
+        <v>6</v>
+      </c>
+      <c r="C620">
+        <v>24.4</v>
+      </c>
+      <c r="D620">
+        <v>38</v>
+      </c>
+      <c r="E620">
+        <v>1</v>
+      </c>
+      <c r="F620">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="621" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A621" t="s">
+        <v>166</v>
+      </c>
+      <c r="B621">
+        <v>6</v>
+      </c>
+      <c r="C621">
+        <v>31.3</v>
+      </c>
+      <c r="D621">
+        <v>23.3</v>
+      </c>
+      <c r="E621">
+        <v>2</v>
+      </c>
+      <c r="F621">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="622" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A622" t="s">
+        <v>109</v>
+      </c>
+      <c r="B622">
+        <v>6</v>
+      </c>
+      <c r="C622">
+        <v>29.5</v>
+      </c>
+      <c r="D622">
+        <v>34</v>
+      </c>
+      <c r="E622">
+        <v>1</v>
+      </c>
+      <c r="F622">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="623" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A623" t="s">
+        <v>167</v>
+      </c>
+      <c r="B623">
+        <v>6</v>
+      </c>
+      <c r="C623">
+        <v>38.4</v>
+      </c>
+      <c r="D623">
+        <v>14</v>
+      </c>
+      <c r="E623">
+        <v>5</v>
+      </c>
+      <c r="F623">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="624" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A624" t="s">
+        <v>168</v>
+      </c>
+      <c r="B624">
+        <v>6</v>
+      </c>
+      <c r="C624">
+        <v>48.5</v>
+      </c>
+      <c r="D624">
+        <v>22</v>
+      </c>
+      <c r="E624">
+        <v>4</v>
+      </c>
+      <c r="F624">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="625" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A625" t="s">
+        <v>169</v>
+      </c>
+      <c r="B625">
+        <v>6</v>
+      </c>
+      <c r="C625">
+        <v>15</v>
+      </c>
+      <c r="D625">
+        <v>16.8</v>
+      </c>
+      <c r="E625">
+        <v>2</v>
+      </c>
+      <c r="F625">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="626" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A626" t="s">
+        <v>104</v>
+      </c>
+      <c r="B626">
+        <v>6</v>
+      </c>
+      <c r="C626">
+        <v>48.5</v>
+      </c>
+      <c r="D626">
+        <v>19</v>
+      </c>
+      <c r="E626">
+        <v>4</v>
+      </c>
+      <c r="F626">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="627" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A627" t="s">
+        <v>90</v>
+      </c>
+      <c r="B627">
+        <v>6</v>
+      </c>
+      <c r="C627">
+        <v>36.799999999999997</v>
+      </c>
+      <c r="D627">
+        <v>21.4</v>
+      </c>
+      <c r="E627">
+        <v>3</v>
+      </c>
+      <c r="F627">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="628" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A628" t="s">
+        <v>101</v>
+      </c>
+      <c r="B628">
+        <v>6</v>
+      </c>
+      <c r="C628">
+        <v>21.8</v>
+      </c>
+      <c r="D628">
+        <v>17.8</v>
+      </c>
+      <c r="E628">
+        <v>3</v>
+      </c>
+      <c r="F628">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="629" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A629" t="s">
+        <v>170</v>
+      </c>
+      <c r="B629">
+        <v>6</v>
+      </c>
+      <c r="C629">
+        <v>21.8</v>
+      </c>
+      <c r="D629">
+        <v>26.4</v>
+      </c>
+      <c r="E629">
+        <v>2</v>
+      </c>
+      <c r="F629">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="630" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A630" t="s">
+        <v>95</v>
+      </c>
+      <c r="B630">
+        <v>6</v>
+      </c>
+      <c r="C630">
+        <v>35</v>
+      </c>
+      <c r="D630">
+        <v>27.6</v>
+      </c>
+      <c r="E630">
+        <v>3</v>
+      </c>
+      <c r="F630">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="631" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A631" t="s">
+        <v>171</v>
+      </c>
+      <c r="B631">
+        <v>6</v>
+      </c>
+      <c r="C631">
+        <v>33</v>
+      </c>
+      <c r="D631">
+        <v>24.2</v>
+      </c>
+      <c r="E631">
+        <v>3</v>
+      </c>
+      <c r="F631">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="632" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A632" t="s">
+        <v>172</v>
+      </c>
+      <c r="B632">
+        <v>6</v>
+      </c>
+      <c r="C632">
+        <v>25.2</v>
+      </c>
+      <c r="D632">
+        <v>22.2</v>
+      </c>
+      <c r="E632">
+        <v>3</v>
+      </c>
+      <c r="F632">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="633" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A633" t="s">
+        <v>173</v>
+      </c>
+      <c r="B633">
+        <v>6</v>
+      </c>
+      <c r="C633">
+        <v>32.4</v>
+      </c>
+      <c r="D633">
+        <v>14.2</v>
+      </c>
+      <c r="E633">
+        <v>4</v>
+      </c>
+      <c r="F633">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="634" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A634" t="s">
+        <v>55</v>
+      </c>
+      <c r="B634">
+        <v>6</v>
+      </c>
+      <c r="C634">
+        <v>35.4</v>
+      </c>
+      <c r="D634">
+        <v>31.6</v>
+      </c>
+      <c r="E634">
+        <v>2</v>
+      </c>
+      <c r="F634">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="635" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A635" t="s">
+        <v>174</v>
+      </c>
+      <c r="B635">
+        <v>6</v>
+      </c>
+      <c r="C635">
+        <v>33</v>
+      </c>
+      <c r="D635">
+        <v>17.5</v>
+      </c>
+      <c r="E635">
+        <v>2</v>
+      </c>
+      <c r="F635">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="636" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A636" t="s">
+        <v>88</v>
+      </c>
+      <c r="B636">
+        <v>6</v>
+      </c>
+      <c r="C636">
+        <v>34.299999999999997</v>
+      </c>
+      <c r="D636">
+        <v>13.5</v>
+      </c>
+      <c r="E636">
+        <v>3</v>
+      </c>
+      <c r="F636">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="637" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A637" t="s">
+        <v>175</v>
+      </c>
+      <c r="B637">
+        <v>6</v>
+      </c>
+      <c r="C637">
+        <v>41.4</v>
+      </c>
+      <c r="D637">
+        <v>20.8</v>
+      </c>
+      <c r="E637">
+        <v>5</v>
+      </c>
+      <c r="F637">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="638" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A638" t="s">
+        <v>176</v>
+      </c>
+      <c r="B638">
+        <v>6</v>
+      </c>
+      <c r="C638">
+        <v>37.799999999999997</v>
+      </c>
+      <c r="D638">
+        <v>22.4</v>
+      </c>
+      <c r="E638">
+        <v>4</v>
+      </c>
+      <c r="F638">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="639" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A639" t="s">
+        <v>110</v>
+      </c>
+      <c r="B639">
+        <v>6</v>
+      </c>
+      <c r="C639">
+        <v>42.2</v>
+      </c>
+      <c r="D639">
+        <v>19.600000000000001</v>
+      </c>
+      <c r="E639">
+        <v>5</v>
+      </c>
+      <c r="F639">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="640" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A640" t="s">
+        <v>53</v>
+      </c>
+      <c r="B640">
+        <v>6</v>
+      </c>
+      <c r="C640">
+        <v>42</v>
+      </c>
+      <c r="D640">
+        <v>14.4</v>
+      </c>
+      <c r="E640">
+        <v>4</v>
+      </c>
+      <c r="F640">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="641" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A641" t="s">
+        <v>58</v>
+      </c>
+      <c r="B641">
+        <v>6</v>
+      </c>
+      <c r="C641">
+        <v>17.600000000000001</v>
+      </c>
+      <c r="D641">
+        <v>36.4</v>
+      </c>
+      <c r="E641">
+        <v>1</v>
+      </c>
+      <c r="F641">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="642" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A642" t="s">
+        <v>48</v>
+      </c>
+      <c r="B642">
+        <v>6</v>
+      </c>
+      <c r="C642">
+        <v>20.7</v>
+      </c>
+      <c r="D642">
+        <v>26.8</v>
+      </c>
+      <c r="E642">
+        <v>3</v>
+      </c>
+      <c r="F642">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="643" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A643" t="s">
+        <v>45</v>
+      </c>
+      <c r="B643">
+        <v>6</v>
+      </c>
+      <c r="C643">
+        <v>38.6</v>
+      </c>
+      <c r="D643">
+        <v>34</v>
+      </c>
+      <c r="E643">
+        <v>3</v>
+      </c>
+      <c r="F643">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="644" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A644" t="s">
+        <v>177</v>
+      </c>
+      <c r="B644">
+        <v>6</v>
+      </c>
+      <c r="C644">
+        <v>34.200000000000003</v>
+      </c>
+      <c r="D644">
+        <v>33.799999999999997</v>
+      </c>
+      <c r="E644">
+        <v>3</v>
+      </c>
+      <c r="F644">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="645" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A645" t="s">
+        <v>178</v>
+      </c>
+      <c r="B645">
+        <v>6</v>
+      </c>
+      <c r="C645">
+        <v>18</v>
+      </c>
+      <c r="D645">
+        <v>23</v>
+      </c>
+      <c r="E645">
+        <v>2</v>
+      </c>
+      <c r="F645">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="646" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A646" t="s">
+        <v>179</v>
+      </c>
+      <c r="B646">
+        <v>6</v>
+      </c>
+      <c r="C646">
+        <v>18.2</v>
+      </c>
+      <c r="D646">
+        <v>22.2</v>
+      </c>
+      <c r="E646">
+        <v>2</v>
+      </c>
+      <c r="F646">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="647" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A647" t="s">
+        <v>180</v>
+      </c>
+      <c r="B647">
+        <v>6</v>
+      </c>
+      <c r="C647">
+        <v>40.4</v>
+      </c>
+      <c r="D647">
+        <v>28.6</v>
+      </c>
+      <c r="E647">
+        <v>4</v>
+      </c>
+      <c r="F647">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="648" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A648" t="s">
+        <v>181</v>
+      </c>
+      <c r="B648">
+        <v>6</v>
+      </c>
+      <c r="C648">
+        <v>41.6</v>
+      </c>
+      <c r="D648">
+        <v>23.2</v>
+      </c>
+      <c r="E648">
+        <v>4</v>
+      </c>
+      <c r="F648">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="649" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A649" t="s">
+        <v>105</v>
+      </c>
+      <c r="B649">
+        <v>6</v>
+      </c>
+      <c r="C649">
+        <v>29.6</v>
+      </c>
+      <c r="D649">
+        <v>18.2</v>
+      </c>
+      <c r="E649">
+        <v>4</v>
+      </c>
+      <c r="F649">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="650" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A650" t="s">
+        <v>39</v>
+      </c>
+      <c r="B650">
+        <v>6</v>
+      </c>
+      <c r="C650">
+        <v>38.200000000000003</v>
+      </c>
+      <c r="D650">
+        <v>29.6</v>
+      </c>
+      <c r="E650">
+        <v>2</v>
+      </c>
+      <c r="F650">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="651" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A651" t="s">
+        <v>182</v>
+      </c>
+      <c r="B651">
+        <v>6</v>
+      </c>
+      <c r="C651">
+        <v>43.4</v>
+      </c>
+      <c r="D651">
+        <v>22.2</v>
+      </c>
+      <c r="E651">
+        <v>3</v>
+      </c>
+      <c r="F651">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="652" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A652" t="s">
+        <v>37</v>
+      </c>
+      <c r="B652">
+        <v>6</v>
+      </c>
+      <c r="C652">
+        <v>22.6</v>
+      </c>
+      <c r="D652">
+        <v>28</v>
+      </c>
+      <c r="E652">
+        <v>2</v>
+      </c>
+      <c r="F652">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="653" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A653" t="s">
+        <v>35</v>
+      </c>
+      <c r="B653">
+        <v>6</v>
+      </c>
+      <c r="C653">
+        <v>29.8</v>
+      </c>
+      <c r="D653">
+        <v>22</v>
+      </c>
+      <c r="E653">
+        <v>2</v>
+      </c>
+      <c r="F653">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="654" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A654" t="s">
+        <v>62</v>
+      </c>
+      <c r="B654">
+        <v>6</v>
+      </c>
+      <c r="C654">
+        <v>22.7</v>
+      </c>
+      <c r="D654">
+        <v>28.3</v>
+      </c>
+      <c r="E654">
+        <v>3</v>
+      </c>
+      <c r="F654">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -20605,10 +23528,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01ABCD41-9594-F549-BC55-37725303300E}">
-  <dimension ref="A1:C101"/>
+  <dimension ref="A1:C126"/>
   <sheetViews>
-    <sheetView topLeftCell="A97" workbookViewId="0">
-      <selection activeCell="D75" sqref="D75"/>
+    <sheetView topLeftCell="A92" workbookViewId="0">
+      <selection activeCell="A102" sqref="A102:B126"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -21724,6 +24647,281 @@
         <v>93</v>
       </c>
     </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A102">
+        <v>6</v>
+      </c>
+      <c r="B102">
+        <v>1</v>
+      </c>
+      <c r="C102" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A103">
+        <v>6</v>
+      </c>
+      <c r="B103">
+        <v>2</v>
+      </c>
+      <c r="C103" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A104">
+        <v>6</v>
+      </c>
+      <c r="B104">
+        <v>3</v>
+      </c>
+      <c r="C104" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A105">
+        <v>6</v>
+      </c>
+      <c r="B105">
+        <v>4</v>
+      </c>
+      <c r="C105" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A106">
+        <v>6</v>
+      </c>
+      <c r="B106">
+        <v>5</v>
+      </c>
+      <c r="C106" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A107">
+        <v>6</v>
+      </c>
+      <c r="B107">
+        <v>6</v>
+      </c>
+      <c r="C107" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A108">
+        <v>6</v>
+      </c>
+      <c r="B108">
+        <v>7</v>
+      </c>
+      <c r="C108" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A109">
+        <v>6</v>
+      </c>
+      <c r="B109">
+        <v>8</v>
+      </c>
+      <c r="C109" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A110">
+        <v>6</v>
+      </c>
+      <c r="B110">
+        <v>9</v>
+      </c>
+      <c r="C110" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A111">
+        <v>6</v>
+      </c>
+      <c r="B111">
+        <v>10</v>
+      </c>
+      <c r="C111" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A112">
+        <v>6</v>
+      </c>
+      <c r="B112">
+        <v>11</v>
+      </c>
+      <c r="C112" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A113">
+        <v>6</v>
+      </c>
+      <c r="B113">
+        <v>12</v>
+      </c>
+      <c r="C113" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A114">
+        <v>6</v>
+      </c>
+      <c r="B114">
+        <v>13</v>
+      </c>
+      <c r="C114" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A115">
+        <v>6</v>
+      </c>
+      <c r="B115">
+        <v>14</v>
+      </c>
+      <c r="C115" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A116">
+        <v>6</v>
+      </c>
+      <c r="B116">
+        <v>15</v>
+      </c>
+      <c r="C116" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A117">
+        <v>6</v>
+      </c>
+      <c r="B117">
+        <v>16</v>
+      </c>
+      <c r="C117" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A118">
+        <v>6</v>
+      </c>
+      <c r="B118">
+        <v>17</v>
+      </c>
+      <c r="C118" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A119">
+        <v>6</v>
+      </c>
+      <c r="B119">
+        <v>18</v>
+      </c>
+      <c r="C119" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A120">
+        <v>6</v>
+      </c>
+      <c r="B120">
+        <v>19</v>
+      </c>
+      <c r="C120" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A121">
+        <v>6</v>
+      </c>
+      <c r="B121">
+        <v>20</v>
+      </c>
+      <c r="C121" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A122">
+        <v>6</v>
+      </c>
+      <c r="B122">
+        <v>21</v>
+      </c>
+      <c r="C122" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A123">
+        <v>6</v>
+      </c>
+      <c r="B123">
+        <v>22</v>
+      </c>
+      <c r="C123" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A124">
+        <v>6</v>
+      </c>
+      <c r="B124">
+        <v>23</v>
+      </c>
+      <c r="C124" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A125">
+        <v>6</v>
+      </c>
+      <c r="B125">
+        <v>24</v>
+      </c>
+      <c r="C125" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A126">
+        <v>6</v>
+      </c>
+      <c r="B126">
+        <v>25</v>
+      </c>
+      <c r="C126" t="s">
+        <v>114</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Week 5 viewership / week 6 predictions
</commit_message>
<xml_diff>
--- a/ratings-2022.xlsx
+++ b/ratings-2022.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mike/PycharmProjects/tvratings-ssac2023/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9714AA1-637B-3841-A1BF-8677594967B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64D018EC-5954-7143-985C-84A95CA1270F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="13360" windowWidth="40960" windowHeight="11000" xr2:uid="{BBDA95F9-3552-704A-ADE2-3350C5179C3F}"/>
   </bookViews>
@@ -992,8 +992,8 @@
   <dimension ref="A1:AA105"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="760" topLeftCell="A86" activePane="bottomLeft"/>
-      <selection pane="bottomLeft" activeCell="F90" sqref="F90"/>
+      <pane ySplit="760" topLeftCell="A89" activePane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="F102" sqref="F102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8953,7 +8953,7 @@
         <v>38</v>
       </c>
       <c r="F90">
-        <v>0</v>
+        <v>4198000</v>
       </c>
       <c r="G90">
         <v>2022</v>
@@ -9046,7 +9046,7 @@
         <v>108</v>
       </c>
       <c r="F91">
-        <v>0</v>
+        <v>2791000</v>
       </c>
       <c r="G91">
         <v>2022</v>
@@ -9139,7 +9139,7 @@
         <v>36</v>
       </c>
       <c r="F92">
-        <v>0</v>
+        <v>2468000</v>
       </c>
       <c r="G92">
         <v>2022</v>
@@ -9232,7 +9232,7 @@
         <v>43</v>
       </c>
       <c r="F93">
-        <v>0</v>
+        <v>829000</v>
       </c>
       <c r="G93">
         <v>2022</v>
@@ -9325,7 +9325,7 @@
         <v>152</v>
       </c>
       <c r="F94">
-        <v>0</v>
+        <v>1132000</v>
       </c>
       <c r="G94">
         <v>2022</v>
@@ -9418,7 +9418,7 @@
         <v>91</v>
       </c>
       <c r="F95">
-        <v>0</v>
+        <v>5828000</v>
       </c>
       <c r="G95">
         <v>2022</v>
@@ -9511,7 +9511,7 @@
         <v>56</v>
       </c>
       <c r="F96">
-        <v>0</v>
+        <v>2412000</v>
       </c>
       <c r="G96">
         <v>2022</v>
@@ -9604,7 +9604,7 @@
         <v>30</v>
       </c>
       <c r="F97">
-        <v>0</v>
+        <v>1615000</v>
       </c>
       <c r="G97">
         <v>2022</v>
@@ -9697,7 +9697,7 @@
         <v>180</v>
       </c>
       <c r="F98">
-        <v>0</v>
+        <v>2483000</v>
       </c>
       <c r="G98">
         <v>2022</v>
@@ -9790,7 +9790,7 @@
         <v>136</v>
       </c>
       <c r="F99">
-        <v>0</v>
+        <v>865000</v>
       </c>
       <c r="G99">
         <v>2022</v>
@@ -9883,7 +9883,7 @@
         <v>29</v>
       </c>
       <c r="F100">
-        <v>0</v>
+        <v>904000</v>
       </c>
       <c r="G100">
         <v>2022</v>
@@ -9976,7 +9976,7 @@
         <v>114</v>
       </c>
       <c r="F101">
-        <v>0</v>
+        <v>2787000</v>
       </c>
       <c r="G101">
         <v>2022</v>
@@ -10069,7 +10069,7 @@
         <v>84</v>
       </c>
       <c r="F102">
-        <v>0</v>
+        <v>4732000</v>
       </c>
       <c r="G102">
         <v>2022</v>
@@ -10162,7 +10162,7 @@
         <v>39</v>
       </c>
       <c r="F103">
-        <v>0</v>
+        <v>1187000</v>
       </c>
       <c r="G103">
         <v>2022</v>
@@ -10255,7 +10255,7 @@
         <v>96</v>
       </c>
       <c r="F104">
-        <v>0</v>
+        <v>1916000</v>
       </c>
       <c r="G104">
         <v>2022</v>
@@ -10348,7 +10348,7 @@
         <v>109</v>
       </c>
       <c r="F105">
-        <v>0</v>
+        <v>672000</v>
       </c>
       <c r="G105">
         <v>2022</v>

</xml_diff>

<commit_message>
Week 9 viewership / week 10 predictions
</commit_message>
<xml_diff>
--- a/ratings-2022.xlsx
+++ b/ratings-2022.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mike/PycharmProjects/tvratings-ssac2023/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CE71122-309B-1745-8585-6FBFE0749E7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7465F568-571F-D043-AB22-CAA409077C89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1600" yWindow="13400" windowWidth="37240" windowHeight="11000" xr2:uid="{BBDA95F9-3552-704A-ADE2-3350C5179C3F}"/>
+    <workbookView xWindow="1560" yWindow="13400" windowWidth="37240" windowHeight="11000" activeTab="2" xr2:uid="{BBDA95F9-3552-704A-ADE2-3350C5179C3F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2184" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2445" uniqueCount="189">
   <si>
     <t>Time</t>
   </si>
@@ -670,10 +670,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -988,11 +989,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78DF36B5-5368-0F4E-AE20-BC9ECC5E0688}">
-  <dimension ref="A1:AA179"/>
+  <dimension ref="A1:AA200"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="760" topLeftCell="A144" activePane="bottomLeft"/>
-      <selection pane="bottomLeft" activeCell="A154" sqref="A154:XFD154"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="760" topLeftCell="A179" activePane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="G167" sqref="G167"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -15219,7 +15220,7 @@
         <v>179</v>
       </c>
       <c r="F159">
-        <v>0</v>
+        <v>1233000</v>
       </c>
       <c r="G159">
         <v>2022</v>
@@ -15297,7 +15298,7 @@
         <v>142</v>
       </c>
       <c r="F160">
-        <v>0</v>
+        <v>190000</v>
       </c>
       <c r="G160">
         <v>2022</v>
@@ -15375,7 +15376,7 @@
         <v>53</v>
       </c>
       <c r="F161">
-        <v>0</v>
+        <v>470000</v>
       </c>
       <c r="G161">
         <v>2022</v>
@@ -15453,7 +15454,7 @@
         <v>28</v>
       </c>
       <c r="F162">
-        <v>0</v>
+        <v>823000</v>
       </c>
       <c r="G162">
         <v>2022</v>
@@ -15531,7 +15532,7 @@
         <v>26</v>
       </c>
       <c r="F163">
-        <v>0</v>
+        <v>8273000</v>
       </c>
       <c r="G163">
         <v>2022</v>
@@ -15609,7 +15610,7 @@
         <v>168</v>
       </c>
       <c r="F164">
-        <v>0</v>
+        <v>1507000</v>
       </c>
       <c r="G164">
         <v>2022</v>
@@ -15687,7 +15688,7 @@
         <v>46</v>
       </c>
       <c r="F165">
-        <v>0</v>
+        <v>2337000</v>
       </c>
       <c r="G165">
         <v>2022</v>
@@ -15765,7 +15766,7 @@
         <v>36</v>
       </c>
       <c r="F166">
-        <v>0</v>
+        <v>711000</v>
       </c>
       <c r="G166">
         <v>2022</v>
@@ -15843,7 +15844,7 @@
         <v>165</v>
       </c>
       <c r="F167">
-        <v>0</v>
+        <v>131000</v>
       </c>
       <c r="G167">
         <v>2022</v>
@@ -15921,7 +15922,7 @@
         <v>52</v>
       </c>
       <c r="F168">
-        <v>0</v>
+        <v>5620000</v>
       </c>
       <c r="G168">
         <v>2022</v>
@@ -15999,7 +16000,7 @@
         <v>49</v>
       </c>
       <c r="F169">
-        <v>0</v>
+        <v>738000</v>
       </c>
       <c r="G169">
         <v>2022</v>
@@ -16077,7 +16078,7 @@
         <v>56</v>
       </c>
       <c r="F170">
-        <v>0</v>
+        <v>3378000</v>
       </c>
       <c r="G170">
         <v>2022</v>
@@ -16155,7 +16156,7 @@
         <v>23</v>
       </c>
       <c r="F171">
-        <v>0</v>
+        <v>2488000</v>
       </c>
       <c r="G171">
         <v>2022</v>
@@ -16233,7 +16234,7 @@
         <v>57</v>
       </c>
       <c r="F172">
-        <v>0</v>
+        <v>1059000</v>
       </c>
       <c r="G172">
         <v>2022</v>
@@ -16311,7 +16312,7 @@
         <v>30</v>
       </c>
       <c r="F173">
-        <v>0</v>
+        <v>483000</v>
       </c>
       <c r="G173">
         <v>2022</v>
@@ -16389,7 +16390,7 @@
         <v>108</v>
       </c>
       <c r="F174">
-        <v>0</v>
+        <v>4042000</v>
       </c>
       <c r="G174">
         <v>2022</v>
@@ -16467,7 +16468,7 @@
         <v>59</v>
       </c>
       <c r="F175">
-        <v>0</v>
+        <v>269000</v>
       </c>
       <c r="G175">
         <v>2022</v>
@@ -16545,7 +16546,7 @@
         <v>29</v>
       </c>
       <c r="F176">
-        <v>0</v>
+        <v>5583000</v>
       </c>
       <c r="G176">
         <v>2022</v>
@@ -16623,7 +16624,7 @@
         <v>98</v>
       </c>
       <c r="F177">
-        <v>0</v>
+        <v>572000</v>
       </c>
       <c r="G177">
         <v>2022</v>
@@ -16701,7 +16702,7 @@
         <v>109</v>
       </c>
       <c r="F178">
-        <v>0</v>
+        <v>1263000</v>
       </c>
       <c r="G178">
         <v>2022</v>
@@ -16779,7 +16780,7 @@
         <v>161</v>
       </c>
       <c r="F179">
-        <v>0</v>
+        <v>219000</v>
       </c>
       <c r="G179">
         <v>2022</v>
@@ -16838,6 +16839,1644 @@
       <c r="AA179" cm="1">
         <f t="array" ref="AA179">_xlfn.XLOOKUP(E179&amp;I179,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!F$2:F$13000,"")</f>
         <v>3</v>
+      </c>
+    </row>
+    <row r="180" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A180" s="1">
+        <v>44866</v>
+      </c>
+      <c r="B180" s="2">
+        <v>0.8125</v>
+      </c>
+      <c r="C180" t="s">
+        <v>47</v>
+      </c>
+      <c r="D180" t="s">
+        <v>157</v>
+      </c>
+      <c r="E180" t="s">
+        <v>126</v>
+      </c>
+      <c r="F180">
+        <v>0</v>
+      </c>
+      <c r="G180">
+        <v>2022</v>
+      </c>
+      <c r="H180">
+        <v>0</v>
+      </c>
+      <c r="I180">
+        <v>10</v>
+      </c>
+      <c r="J180" t="str" cm="1">
+        <f t="array" ref="J180">_xlfn.XLOOKUP(D180&amp;I180,Ranking!C$2:C$500&amp;Ranking!A$2:A$500,Ranking!B$2:B$500,"")</f>
+        <v/>
+      </c>
+      <c r="K180" t="str" cm="1">
+        <f t="array" ref="K180">_xlfn.XLOOKUP(E180&amp;I180,Ranking!C$2:C$500&amp;Ranking!A$2:A$500,Ranking!B$2:B$500,"")</f>
+        <v/>
+      </c>
+      <c r="L180" t="s">
+        <v>72</v>
+      </c>
+      <c r="M180" t="s">
+        <v>72</v>
+      </c>
+      <c r="N180">
+        <v>1</v>
+      </c>
+      <c r="O180" cm="1">
+        <f t="array" ref="O180">_xlfn.XLOOKUP(D180&amp;I180,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!C$2:C$13000,"")</f>
+        <v>32</v>
+      </c>
+      <c r="P180" cm="1">
+        <f t="array" ref="P180">_xlfn.XLOOKUP(D180&amp;I180,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!D$2:D$13000,"")</f>
+        <v>34.4</v>
+      </c>
+      <c r="Q180" cm="1">
+        <f t="array" ref="Q180">_xlfn.XLOOKUP(E180&amp;I180,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!C$2:C$13000,"")</f>
+        <v>30.9</v>
+      </c>
+      <c r="R180" cm="1">
+        <f t="array" ref="R180">_xlfn.XLOOKUP(E180&amp;I180,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!D$2:D$13000,"")</f>
+        <v>24.8</v>
+      </c>
+      <c r="X180" cm="1">
+        <f t="array" ref="X180">_xlfn.XLOOKUP(D180&amp;I180,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!E$2:E$13000,"")</f>
+        <v>5</v>
+      </c>
+      <c r="Y180" cm="1">
+        <f t="array" ref="Y180">_xlfn.XLOOKUP(D180&amp;I180,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!F$2:F$13000,"")</f>
+        <v>3</v>
+      </c>
+      <c r="Z180" cm="1">
+        <f t="array" ref="Z180">_xlfn.XLOOKUP(E180&amp;I180,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!E$2:E$13000,"")</f>
+        <v>5</v>
+      </c>
+      <c r="AA180" cm="1">
+        <f t="array" ref="AA180">_xlfn.XLOOKUP(E180&amp;I180,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!F$2:F$13000,"")</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="181" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A181" s="1">
+        <v>44867</v>
+      </c>
+      <c r="B181" s="2">
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="C181" t="s">
+        <v>47</v>
+      </c>
+      <c r="D181" t="s">
+        <v>125</v>
+      </c>
+      <c r="E181" t="s">
+        <v>37</v>
+      </c>
+      <c r="F181">
+        <v>0</v>
+      </c>
+      <c r="G181">
+        <v>2022</v>
+      </c>
+      <c r="H181">
+        <v>0</v>
+      </c>
+      <c r="I181">
+        <v>10</v>
+      </c>
+      <c r="J181" t="str" cm="1">
+        <f t="array" ref="J181">_xlfn.XLOOKUP(D181&amp;I181,Ranking!C$2:C$500&amp;Ranking!A$2:A$500,Ranking!B$2:B$500,"")</f>
+        <v/>
+      </c>
+      <c r="K181" t="str" cm="1">
+        <f t="array" ref="K181">_xlfn.XLOOKUP(E181&amp;I181,Ranking!C$2:C$500&amp;Ranking!A$2:A$500,Ranking!B$2:B$500,"")</f>
+        <v/>
+      </c>
+      <c r="L181" t="s">
+        <v>72</v>
+      </c>
+      <c r="M181" t="s">
+        <v>72</v>
+      </c>
+      <c r="N181">
+        <v>1</v>
+      </c>
+      <c r="O181" cm="1">
+        <f t="array" ref="O181">_xlfn.XLOOKUP(D181&amp;I181,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!C$2:C$13000,"")</f>
+        <v>26.4</v>
+      </c>
+      <c r="P181" cm="1">
+        <f t="array" ref="P181">_xlfn.XLOOKUP(D181&amp;I181,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!D$2:D$13000,"")</f>
+        <v>34.6</v>
+      </c>
+      <c r="Q181" cm="1">
+        <f t="array" ref="Q181">_xlfn.XLOOKUP(E181&amp;I181,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!C$2:C$13000,"")</f>
+        <v>20.8</v>
+      </c>
+      <c r="R181" cm="1">
+        <f t="array" ref="R181">_xlfn.XLOOKUP(E181&amp;I181,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!D$2:D$13000,"")</f>
+        <v>28.5</v>
+      </c>
+      <c r="X181" cm="1">
+        <f t="array" ref="X181">_xlfn.XLOOKUP(D181&amp;I181,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!E$2:E$13000,"")</f>
+        <v>4</v>
+      </c>
+      <c r="Y181" cm="1">
+        <f t="array" ref="Y181">_xlfn.XLOOKUP(D181&amp;I181,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!F$2:F$13000,"")</f>
+        <v>4</v>
+      </c>
+      <c r="Z181" cm="1">
+        <f t="array" ref="Z181">_xlfn.XLOOKUP(E181&amp;I181,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!E$2:E$13000,"")</f>
+        <v>3</v>
+      </c>
+      <c r="AA181" cm="1">
+        <f t="array" ref="AA181">_xlfn.XLOOKUP(E181&amp;I181,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!F$2:F$13000,"")</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="182" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A182" s="1">
+        <v>44868</v>
+      </c>
+      <c r="B182" s="2">
+        <v>0.8125</v>
+      </c>
+      <c r="C182" t="s">
+        <v>25</v>
+      </c>
+      <c r="D182" t="s">
+        <v>128</v>
+      </c>
+      <c r="E182" t="s">
+        <v>102</v>
+      </c>
+      <c r="F182">
+        <v>0</v>
+      </c>
+      <c r="G182">
+        <v>2022</v>
+      </c>
+      <c r="H182">
+        <v>0</v>
+      </c>
+      <c r="I182">
+        <v>10</v>
+      </c>
+      <c r="J182" t="str" cm="1">
+        <f t="array" ref="J182">_xlfn.XLOOKUP(D182&amp;I182,Ranking!C$2:C$500&amp;Ranking!A$2:A$500,Ranking!B$2:B$500,"")</f>
+        <v/>
+      </c>
+      <c r="K182" t="str" cm="1">
+        <f t="array" ref="K182">_xlfn.XLOOKUP(E182&amp;I182,Ranking!C$2:C$500&amp;Ranking!A$2:A$500,Ranking!B$2:B$500,"")</f>
+        <v/>
+      </c>
+      <c r="L182" t="s">
+        <v>103</v>
+      </c>
+      <c r="M182" t="s">
+        <v>103</v>
+      </c>
+      <c r="N182">
+        <v>1</v>
+      </c>
+      <c r="O182" cm="1">
+        <f t="array" ref="O182">_xlfn.XLOOKUP(D182&amp;I182,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!C$2:C$13000,"")</f>
+        <v>31.9</v>
+      </c>
+      <c r="P182" cm="1">
+        <f t="array" ref="P182">_xlfn.XLOOKUP(D182&amp;I182,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!D$2:D$13000,"")</f>
+        <v>27.3</v>
+      </c>
+      <c r="Q182" cm="1">
+        <f t="array" ref="Q182">_xlfn.XLOOKUP(E182&amp;I182,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!C$2:C$13000,"")</f>
+        <v>36.9</v>
+      </c>
+      <c r="R182" cm="1">
+        <f t="array" ref="R182">_xlfn.XLOOKUP(E182&amp;I182,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!D$2:D$13000,"")</f>
+        <v>24.1</v>
+      </c>
+      <c r="X182" cm="1">
+        <f t="array" ref="X182">_xlfn.XLOOKUP(D182&amp;I182,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!E$2:E$13000,"")</f>
+        <v>7</v>
+      </c>
+      <c r="Y182" cm="1">
+        <f t="array" ref="Y182">_xlfn.XLOOKUP(D182&amp;I182,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!F$2:F$13000,"")</f>
+        <v>1</v>
+      </c>
+      <c r="Z182" cm="1">
+        <f t="array" ref="Z182">_xlfn.XLOOKUP(E182&amp;I182,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!E$2:E$13000,"")</f>
+        <v>5</v>
+      </c>
+      <c r="AA182" cm="1">
+        <f t="array" ref="AA182">_xlfn.XLOOKUP(E182&amp;I182,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!F$2:F$13000,"")</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="183" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A183" s="1">
+        <v>44869</v>
+      </c>
+      <c r="B183" s="2">
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="C183" t="s">
+        <v>47</v>
+      </c>
+      <c r="D183" t="s">
+        <v>124</v>
+      </c>
+      <c r="E183" t="s">
+        <v>129</v>
+      </c>
+      <c r="F183">
+        <v>0</v>
+      </c>
+      <c r="G183">
+        <v>2022</v>
+      </c>
+      <c r="H183">
+        <v>0</v>
+      </c>
+      <c r="I183">
+        <v>10</v>
+      </c>
+      <c r="J183" t="str" cm="1">
+        <f t="array" ref="J183">_xlfn.XLOOKUP(D183&amp;I183,Ranking!C$2:C$500&amp;Ranking!A$2:A$500,Ranking!B$2:B$500,"")</f>
+        <v/>
+      </c>
+      <c r="K183" t="str" cm="1">
+        <f t="array" ref="K183">_xlfn.XLOOKUP(E183&amp;I183,Ranking!C$2:C$500&amp;Ranking!A$2:A$500,Ranking!B$2:B$500,"")</f>
+        <v/>
+      </c>
+      <c r="L183" t="s">
+        <v>69</v>
+      </c>
+      <c r="M183" t="s">
+        <v>69</v>
+      </c>
+      <c r="N183">
+        <v>1</v>
+      </c>
+      <c r="O183" cm="1">
+        <f t="array" ref="O183">_xlfn.XLOOKUP(D183&amp;I183,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!C$2:C$13000,"")</f>
+        <v>17.3</v>
+      </c>
+      <c r="P183" cm="1">
+        <f t="array" ref="P183">_xlfn.XLOOKUP(D183&amp;I183,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!D$2:D$13000,"")</f>
+        <v>28.8</v>
+      </c>
+      <c r="Q183" cm="1">
+        <f t="array" ref="Q183">_xlfn.XLOOKUP(E183&amp;I183,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!C$2:C$13000,"")</f>
+        <v>34.4</v>
+      </c>
+      <c r="R183" cm="1">
+        <f t="array" ref="R183">_xlfn.XLOOKUP(E183&amp;I183,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!D$2:D$13000,"")</f>
+        <v>22.1</v>
+      </c>
+      <c r="X183" cm="1">
+        <f t="array" ref="X183">_xlfn.XLOOKUP(D183&amp;I183,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!E$2:E$13000,"")</f>
+        <v>2</v>
+      </c>
+      <c r="Y183" cm="1">
+        <f t="array" ref="Y183">_xlfn.XLOOKUP(D183&amp;I183,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!F$2:F$13000,"")</f>
+        <v>6</v>
+      </c>
+      <c r="Z183" cm="1">
+        <f t="array" ref="Z183">_xlfn.XLOOKUP(E183&amp;I183,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!E$2:E$13000,"")</f>
+        <v>5</v>
+      </c>
+      <c r="AA183" cm="1">
+        <f t="array" ref="AA183">_xlfn.XLOOKUP(E183&amp;I183,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!F$2:F$13000,"")</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="184" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A184" s="1">
+        <v>44869</v>
+      </c>
+      <c r="B184" s="2">
+        <v>0.9375</v>
+      </c>
+      <c r="C184" t="s">
+        <v>47</v>
+      </c>
+      <c r="D184" t="s">
+        <v>181</v>
+      </c>
+      <c r="E184" t="s">
+        <v>42</v>
+      </c>
+      <c r="F184">
+        <v>0</v>
+      </c>
+      <c r="G184">
+        <v>2022</v>
+      </c>
+      <c r="H184">
+        <v>0</v>
+      </c>
+      <c r="I184">
+        <v>10</v>
+      </c>
+      <c r="J184" t="str" cm="1">
+        <f t="array" ref="J184">_xlfn.XLOOKUP(D184&amp;I184,Ranking!C$2:C$500&amp;Ranking!A$2:A$500,Ranking!B$2:B$500,"")</f>
+        <v/>
+      </c>
+      <c r="K184" cm="1">
+        <f t="array" ref="K184">_xlfn.XLOOKUP(E184&amp;I184,Ranking!C$2:C$500&amp;Ranking!A$2:A$500,Ranking!B$2:B$500,"")</f>
+        <v>23</v>
+      </c>
+      <c r="L184" t="s">
+        <v>65</v>
+      </c>
+      <c r="M184" t="s">
+        <v>65</v>
+      </c>
+      <c r="N184">
+        <v>1</v>
+      </c>
+      <c r="O184" cm="1">
+        <f t="array" ref="O184">_xlfn.XLOOKUP(D184&amp;I184,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!C$2:C$13000,"")</f>
+        <v>40.4</v>
+      </c>
+      <c r="P184" cm="1">
+        <f t="array" ref="P184">_xlfn.XLOOKUP(D184&amp;I184,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!D$2:D$13000,"")</f>
+        <v>27.6</v>
+      </c>
+      <c r="Q184" cm="1">
+        <f t="array" ref="Q184">_xlfn.XLOOKUP(E184&amp;I184,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!C$2:C$13000,"")</f>
+        <v>32.6</v>
+      </c>
+      <c r="R184" cm="1">
+        <f t="array" ref="R184">_xlfn.XLOOKUP(E184&amp;I184,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!D$2:D$13000,"")</f>
+        <v>22.8</v>
+      </c>
+      <c r="X184" cm="1">
+        <f t="array" ref="X184">_xlfn.XLOOKUP(D184&amp;I184,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!E$2:E$13000,"")</f>
+        <v>6</v>
+      </c>
+      <c r="Y184" cm="1">
+        <f t="array" ref="Y184">_xlfn.XLOOKUP(D184&amp;I184,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!F$2:F$13000,"")</f>
+        <v>2</v>
+      </c>
+      <c r="Z184" cm="1">
+        <f t="array" ref="Z184">_xlfn.XLOOKUP(E184&amp;I184,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!E$2:E$13000,"")</f>
+        <v>6</v>
+      </c>
+      <c r="AA184" cm="1">
+        <f t="array" ref="AA184">_xlfn.XLOOKUP(E184&amp;I184,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!F$2:F$13000,"")</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="185" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A185" s="1">
+        <v>44870</v>
+      </c>
+      <c r="B185" s="2">
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="C185" t="s">
+        <v>54</v>
+      </c>
+      <c r="D185" t="s">
+        <v>121</v>
+      </c>
+      <c r="E185" t="s">
+        <v>106</v>
+      </c>
+      <c r="F185">
+        <v>0</v>
+      </c>
+      <c r="G185">
+        <v>2022</v>
+      </c>
+      <c r="H185">
+        <v>0</v>
+      </c>
+      <c r="I185">
+        <v>10</v>
+      </c>
+      <c r="J185" t="str" cm="1">
+        <f t="array" ref="J185">_xlfn.XLOOKUP(D185&amp;I185,Ranking!C$2:C$500&amp;Ranking!A$2:A$500,Ranking!B$2:B$500,"")</f>
+        <v/>
+      </c>
+      <c r="K185" t="str" cm="1">
+        <f t="array" ref="K185">_xlfn.XLOOKUP(E185&amp;I185,Ranking!C$2:C$500&amp;Ranking!A$2:A$500,Ranking!B$2:B$500,"")</f>
+        <v/>
+      </c>
+      <c r="L185" t="s">
+        <v>73</v>
+      </c>
+      <c r="M185" t="s">
+        <v>66</v>
+      </c>
+      <c r="N185">
+        <v>1</v>
+      </c>
+      <c r="O185" cm="1">
+        <f t="array" ref="O185">_xlfn.XLOOKUP(D185&amp;I185,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!C$2:C$13000,"")</f>
+        <v>32.700000000000003</v>
+      </c>
+      <c r="P185" cm="1">
+        <f t="array" ref="P185">_xlfn.XLOOKUP(D185&amp;I185,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!D$2:D$13000,"")</f>
+        <v>29.4</v>
+      </c>
+      <c r="Q185" cm="1">
+        <f t="array" ref="Q185">_xlfn.XLOOKUP(E185&amp;I185,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!C$2:C$13000,"")</f>
+        <v>30.9</v>
+      </c>
+      <c r="R185" cm="1">
+        <f t="array" ref="R185">_xlfn.XLOOKUP(E185&amp;I185,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!D$2:D$13000,"")</f>
+        <v>16.8</v>
+      </c>
+      <c r="X185" cm="1">
+        <f t="array" ref="X185">_xlfn.XLOOKUP(D185&amp;I185,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!E$2:E$13000,"")</f>
+        <v>3</v>
+      </c>
+      <c r="Y185" cm="1">
+        <f t="array" ref="Y185">_xlfn.XLOOKUP(D185&amp;I185,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!F$2:F$13000,"")</f>
+        <v>4</v>
+      </c>
+      <c r="Z185" cm="1">
+        <f t="array" ref="Z185">_xlfn.XLOOKUP(E185&amp;I185,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!E$2:E$13000,"")</f>
+        <v>5</v>
+      </c>
+      <c r="AA185" cm="1">
+        <f t="array" ref="AA185">_xlfn.XLOOKUP(E185&amp;I185,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!F$2:F$13000,"")</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="186" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A186" s="1">
+        <v>44870</v>
+      </c>
+      <c r="B186" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="C186" t="s">
+        <v>33</v>
+      </c>
+      <c r="D186" t="s">
+        <v>30</v>
+      </c>
+      <c r="E186" t="s">
+        <v>26</v>
+      </c>
+      <c r="F186">
+        <v>0</v>
+      </c>
+      <c r="G186">
+        <v>2022</v>
+      </c>
+      <c r="H186">
+        <v>0</v>
+      </c>
+      <c r="I186">
+        <v>10</v>
+      </c>
+      <c r="J186" t="str" cm="1">
+        <f t="array" ref="J186">_xlfn.XLOOKUP(D186&amp;I186,Ranking!C$2:C$500&amp;Ranking!A$2:A$500,Ranking!B$2:B$500,"")</f>
+        <v/>
+      </c>
+      <c r="K186" cm="1">
+        <f t="array" ref="K186">_xlfn.XLOOKUP(E186&amp;I186,Ranking!C$2:C$500&amp;Ranking!A$2:A$500,Ranking!B$2:B$500,"")</f>
+        <v>2</v>
+      </c>
+      <c r="L186" t="s">
+        <v>64</v>
+      </c>
+      <c r="M186" t="s">
+        <v>64</v>
+      </c>
+      <c r="N186">
+        <v>1</v>
+      </c>
+      <c r="O186" cm="1">
+        <f t="array" ref="O186">_xlfn.XLOOKUP(D186&amp;I186,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!C$2:C$13000,"")</f>
+        <v>17.899999999999999</v>
+      </c>
+      <c r="P186" cm="1">
+        <f t="array" ref="P186">_xlfn.XLOOKUP(D186&amp;I186,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!D$2:D$13000,"")</f>
+        <v>28.8</v>
+      </c>
+      <c r="Q186" cm="1">
+        <f t="array" ref="Q186">_xlfn.XLOOKUP(E186&amp;I186,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!C$2:C$13000,"")</f>
+        <v>48.9</v>
+      </c>
+      <c r="R186" cm="1">
+        <f t="array" ref="R186">_xlfn.XLOOKUP(E186&amp;I186,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!D$2:D$13000,"")</f>
+        <v>16.899999999999999</v>
+      </c>
+      <c r="X186" cm="1">
+        <f t="array" ref="X186">_xlfn.XLOOKUP(D186&amp;I186,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!E$2:E$13000,"")</f>
+        <v>1</v>
+      </c>
+      <c r="Y186" cm="1">
+        <f t="array" ref="Y186">_xlfn.XLOOKUP(D186&amp;I186,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!F$2:F$13000,"")</f>
+        <v>7</v>
+      </c>
+      <c r="Z186" cm="1">
+        <f t="array" ref="Z186">_xlfn.XLOOKUP(E186&amp;I186,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!E$2:E$13000,"")</f>
+        <v>8</v>
+      </c>
+      <c r="AA186" cm="1">
+        <f t="array" ref="AA186">_xlfn.XLOOKUP(E186&amp;I186,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!F$2:F$13000,"")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="187" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A187" s="1">
+        <v>44870</v>
+      </c>
+      <c r="B187" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="C187" t="s">
+        <v>24</v>
+      </c>
+      <c r="D187" t="s">
+        <v>168</v>
+      </c>
+      <c r="E187" t="s">
+        <v>95</v>
+      </c>
+      <c r="F187">
+        <v>0</v>
+      </c>
+      <c r="G187">
+        <v>2022</v>
+      </c>
+      <c r="H187">
+        <v>0</v>
+      </c>
+      <c r="I187">
+        <v>10</v>
+      </c>
+      <c r="J187" cm="1">
+        <f t="array" ref="J187">_xlfn.XLOOKUP(D187&amp;I187,Ranking!C$2:C$500&amp;Ranking!A$2:A$500,Ranking!B$2:B$500,"")</f>
+        <v>7</v>
+      </c>
+      <c r="K187" t="str" cm="1">
+        <f t="array" ref="K187">_xlfn.XLOOKUP(E187&amp;I187,Ranking!C$2:C$500&amp;Ranking!A$2:A$500,Ranking!B$2:B$500,"")</f>
+        <v/>
+      </c>
+      <c r="L187" t="s">
+        <v>71</v>
+      </c>
+      <c r="M187" t="s">
+        <v>71</v>
+      </c>
+      <c r="N187">
+        <v>1</v>
+      </c>
+      <c r="O187" cm="1">
+        <f t="array" ref="O187">_xlfn.XLOOKUP(D187&amp;I187,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!C$2:C$13000,"")</f>
+        <v>44.3</v>
+      </c>
+      <c r="P187" cm="1">
+        <f t="array" ref="P187">_xlfn.XLOOKUP(D187&amp;I187,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!D$2:D$13000,"")</f>
+        <v>27.3</v>
+      </c>
+      <c r="Q187" cm="1">
+        <f t="array" ref="Q187">_xlfn.XLOOKUP(E187&amp;I187,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!C$2:C$13000,"")</f>
+        <v>33.9</v>
+      </c>
+      <c r="R187" cm="1">
+        <f t="array" ref="R187">_xlfn.XLOOKUP(E187&amp;I187,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!D$2:D$13000,"")</f>
+        <v>29.3</v>
+      </c>
+      <c r="X187" cm="1">
+        <f t="array" ref="X187">_xlfn.XLOOKUP(D187&amp;I187,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!E$2:E$13000,"")</f>
+        <v>8</v>
+      </c>
+      <c r="Y187" cm="1">
+        <f t="array" ref="Y187">_xlfn.XLOOKUP(D187&amp;I187,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!F$2:F$13000,"")</f>
+        <v>0</v>
+      </c>
+      <c r="Z187" cm="1">
+        <f t="array" ref="Z187">_xlfn.XLOOKUP(E187&amp;I187,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!E$2:E$13000,"")</f>
+        <v>4</v>
+      </c>
+      <c r="AA187" cm="1">
+        <f t="array" ref="AA187">_xlfn.XLOOKUP(E187&amp;I187,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!F$2:F$13000,"")</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="188" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A188" s="1">
+        <v>44870</v>
+      </c>
+      <c r="B188" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="C188" t="s">
+        <v>25</v>
+      </c>
+      <c r="D188" t="s">
+        <v>101</v>
+      </c>
+      <c r="E188" t="s">
+        <v>52</v>
+      </c>
+      <c r="F188">
+        <v>0</v>
+      </c>
+      <c r="G188">
+        <v>2022</v>
+      </c>
+      <c r="H188">
+        <v>0</v>
+      </c>
+      <c r="I188">
+        <v>10</v>
+      </c>
+      <c r="J188" t="str" cm="1">
+        <f t="array" ref="J188">_xlfn.XLOOKUP(D188&amp;I188,Ranking!C$2:C$500&amp;Ranking!A$2:A$500,Ranking!B$2:B$500,"")</f>
+        <v/>
+      </c>
+      <c r="K188" t="str" cm="1">
+        <f t="array" ref="K188">_xlfn.XLOOKUP(E188&amp;I188,Ranking!C$2:C$500&amp;Ranking!A$2:A$500,Ranking!B$2:B$500,"")</f>
+        <v/>
+      </c>
+      <c r="L188" t="s">
+        <v>70</v>
+      </c>
+      <c r="M188" t="s">
+        <v>70</v>
+      </c>
+      <c r="N188">
+        <v>1</v>
+      </c>
+      <c r="O188" cm="1">
+        <f t="array" ref="O188">_xlfn.XLOOKUP(D188&amp;I188,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!C$2:C$13000,"")</f>
+        <v>22.6</v>
+      </c>
+      <c r="P188" cm="1">
+        <f t="array" ref="P188">_xlfn.XLOOKUP(D188&amp;I188,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!D$2:D$13000,"")</f>
+        <v>21.8</v>
+      </c>
+      <c r="Q188" cm="1">
+        <f t="array" ref="Q188">_xlfn.XLOOKUP(E188&amp;I188,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!C$2:C$13000,"")</f>
+        <v>30</v>
+      </c>
+      <c r="R188" cm="1">
+        <f t="array" ref="R188">_xlfn.XLOOKUP(E188&amp;I188,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!D$2:D$13000,"")</f>
+        <v>29.9</v>
+      </c>
+      <c r="X188" cm="1">
+        <f t="array" ref="X188">_xlfn.XLOOKUP(D188&amp;I188,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!E$2:E$13000,"")</f>
+        <v>3</v>
+      </c>
+      <c r="Y188" cm="1">
+        <f t="array" ref="Y188">_xlfn.XLOOKUP(D188&amp;I188,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!F$2:F$13000,"")</f>
+        <v>5</v>
+      </c>
+      <c r="Z188" cm="1">
+        <f t="array" ref="Z188">_xlfn.XLOOKUP(E188&amp;I188,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!E$2:E$13000,"")</f>
+        <v>4</v>
+      </c>
+      <c r="AA188" cm="1">
+        <f t="array" ref="AA188">_xlfn.XLOOKUP(E188&amp;I188,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!F$2:F$13000,"")</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="189" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A189" s="1">
+        <v>44870</v>
+      </c>
+      <c r="B189" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="C189" t="s">
+        <v>47</v>
+      </c>
+      <c r="D189" t="s">
+        <v>22</v>
+      </c>
+      <c r="E189" t="s">
+        <v>150</v>
+      </c>
+      <c r="F189">
+        <v>0</v>
+      </c>
+      <c r="G189">
+        <v>2022</v>
+      </c>
+      <c r="H189">
+        <v>0</v>
+      </c>
+      <c r="I189">
+        <v>10</v>
+      </c>
+      <c r="J189" t="str" cm="1">
+        <f t="array" ref="J189">_xlfn.XLOOKUP(D189&amp;I189,Ranking!C$2:C$500&amp;Ranking!A$2:A$500,Ranking!B$2:B$500,"")</f>
+        <v/>
+      </c>
+      <c r="K189" t="str" cm="1">
+        <f t="array" ref="K189">_xlfn.XLOOKUP(E189&amp;I189,Ranking!C$2:C$500&amp;Ranking!A$2:A$500,Ranking!B$2:B$500,"")</f>
+        <v/>
+      </c>
+      <c r="L189" t="s">
+        <v>64</v>
+      </c>
+      <c r="M189" t="s">
+        <v>64</v>
+      </c>
+      <c r="N189">
+        <v>1</v>
+      </c>
+      <c r="O189" cm="1">
+        <f t="array" ref="O189">_xlfn.XLOOKUP(D189&amp;I189,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!C$2:C$13000,"")</f>
+        <v>27.1</v>
+      </c>
+      <c r="P189" cm="1">
+        <f t="array" ref="P189">_xlfn.XLOOKUP(D189&amp;I189,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!D$2:D$13000,"")</f>
+        <v>30.6</v>
+      </c>
+      <c r="Q189" cm="1">
+        <f t="array" ref="Q189">_xlfn.XLOOKUP(E189&amp;I189,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!C$2:C$13000,"")</f>
+        <v>31.9</v>
+      </c>
+      <c r="R189" cm="1">
+        <f t="array" ref="R189">_xlfn.XLOOKUP(E189&amp;I189,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!D$2:D$13000,"")</f>
+        <v>14.4</v>
+      </c>
+      <c r="X189" cm="1">
+        <f t="array" ref="X189">_xlfn.XLOOKUP(D189&amp;I189,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!E$2:E$13000,"")</f>
+        <v>3</v>
+      </c>
+      <c r="Y189" cm="1">
+        <f t="array" ref="Y189">_xlfn.XLOOKUP(D189&amp;I189,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!F$2:F$13000,"")</f>
+        <v>5</v>
+      </c>
+      <c r="Z189" cm="1">
+        <f t="array" ref="Z189">_xlfn.XLOOKUP(E189&amp;I189,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!E$2:E$13000,"")</f>
+        <v>5</v>
+      </c>
+      <c r="AA189" cm="1">
+        <f t="array" ref="AA189">_xlfn.XLOOKUP(E189&amp;I189,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!F$2:F$13000,"")</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="190" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A190" s="1">
+        <v>44870</v>
+      </c>
+      <c r="B190" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="C190" t="s">
+        <v>31</v>
+      </c>
+      <c r="D190" t="s">
+        <v>43</v>
+      </c>
+      <c r="E190" t="s">
+        <v>135</v>
+      </c>
+      <c r="F190">
+        <v>0</v>
+      </c>
+      <c r="G190">
+        <v>2022</v>
+      </c>
+      <c r="H190">
+        <v>0</v>
+      </c>
+      <c r="I190">
+        <v>10</v>
+      </c>
+      <c r="J190" t="str" cm="1">
+        <f t="array" ref="J190">_xlfn.XLOOKUP(D190&amp;I190,Ranking!C$2:C$500&amp;Ranking!A$2:A$500,Ranking!B$2:B$500,"")</f>
+        <v/>
+      </c>
+      <c r="K190" t="str" cm="1">
+        <f t="array" ref="K190">_xlfn.XLOOKUP(E190&amp;I190,Ranking!C$2:C$500&amp;Ranking!A$2:A$500,Ranking!B$2:B$500,"")</f>
+        <v/>
+      </c>
+      <c r="L190" t="s">
+        <v>64</v>
+      </c>
+      <c r="M190" t="s">
+        <v>64</v>
+      </c>
+      <c r="N190">
+        <v>1</v>
+      </c>
+      <c r="O190" cm="1">
+        <f t="array" ref="O190">_xlfn.XLOOKUP(D190&amp;I190,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!C$2:C$13000,"")</f>
+        <v>32.799999999999997</v>
+      </c>
+      <c r="P190" cm="1">
+        <f t="array" ref="P190">_xlfn.XLOOKUP(D190&amp;I190,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!D$2:D$13000,"")</f>
+        <v>25.5</v>
+      </c>
+      <c r="Q190" cm="1">
+        <f t="array" ref="Q190">_xlfn.XLOOKUP(E190&amp;I190,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!C$2:C$13000,"")</f>
+        <v>16.399999999999999</v>
+      </c>
+      <c r="R190" cm="1">
+        <f t="array" ref="R190">_xlfn.XLOOKUP(E190&amp;I190,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!D$2:D$13000,"")</f>
+        <v>15.8</v>
+      </c>
+      <c r="X190" cm="1">
+        <f t="array" ref="X190">_xlfn.XLOOKUP(D190&amp;I190,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!E$2:E$13000,"")</f>
+        <v>5</v>
+      </c>
+      <c r="Y190" cm="1">
+        <f t="array" ref="Y190">_xlfn.XLOOKUP(D190&amp;I190,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!F$2:F$13000,"")</f>
+        <v>3</v>
+      </c>
+      <c r="Z190" cm="1">
+        <f t="array" ref="Z190">_xlfn.XLOOKUP(E190&amp;I190,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!E$2:E$13000,"")</f>
+        <v>4</v>
+      </c>
+      <c r="AA190" cm="1">
+        <f t="array" ref="AA190">_xlfn.XLOOKUP(E190&amp;I190,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!F$2:F$13000,"")</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="191" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A191" s="1">
+        <v>44870</v>
+      </c>
+      <c r="B191" s="2">
+        <v>0.64583333333333337</v>
+      </c>
+      <c r="C191" t="s">
+        <v>54</v>
+      </c>
+      <c r="D191" t="s">
+        <v>32</v>
+      </c>
+      <c r="E191" t="s">
+        <v>104</v>
+      </c>
+      <c r="F191">
+        <v>0</v>
+      </c>
+      <c r="G191">
+        <v>2022</v>
+      </c>
+      <c r="H191">
+        <v>0</v>
+      </c>
+      <c r="I191">
+        <v>10</v>
+      </c>
+      <c r="J191" cm="1">
+        <f t="array" ref="J191">_xlfn.XLOOKUP(D191&amp;I191,Ranking!C$2:C$500&amp;Ranking!A$2:A$500,Ranking!B$2:B$500,"")</f>
+        <v>3</v>
+      </c>
+      <c r="K191" cm="1">
+        <f t="array" ref="K191">_xlfn.XLOOKUP(E191&amp;I191,Ranking!C$2:C$500&amp;Ranking!A$2:A$500,Ranking!B$2:B$500,"")</f>
+        <v>1</v>
+      </c>
+      <c r="L191" t="s">
+        <v>70</v>
+      </c>
+      <c r="M191" t="s">
+        <v>70</v>
+      </c>
+      <c r="N191">
+        <v>1</v>
+      </c>
+      <c r="O191" cm="1">
+        <f t="array" ref="O191">_xlfn.XLOOKUP(D191&amp;I191,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!C$2:C$13000,"")</f>
+        <v>41.8</v>
+      </c>
+      <c r="P191" cm="1">
+        <f t="array" ref="P191">_xlfn.XLOOKUP(D191&amp;I191,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!D$2:D$13000,"")</f>
+        <v>10.5</v>
+      </c>
+      <c r="Q191" cm="1">
+        <f t="array" ref="Q191">_xlfn.XLOOKUP(E191&amp;I191,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!C$2:C$13000,"")</f>
+        <v>49.4</v>
+      </c>
+      <c r="R191" cm="1">
+        <f t="array" ref="R191">_xlfn.XLOOKUP(E191&amp;I191,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!D$2:D$13000,"")</f>
+        <v>21</v>
+      </c>
+      <c r="X191" cm="1">
+        <f t="array" ref="X191">_xlfn.XLOOKUP(D191&amp;I191,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!E$2:E$13000,"")</f>
+        <v>8</v>
+      </c>
+      <c r="Y191" cm="1">
+        <f t="array" ref="Y191">_xlfn.XLOOKUP(D191&amp;I191,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!F$2:F$13000,"")</f>
+        <v>0</v>
+      </c>
+      <c r="Z191" cm="1">
+        <f t="array" ref="Z191">_xlfn.XLOOKUP(E191&amp;I191,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!E$2:E$13000,"")</f>
+        <v>8</v>
+      </c>
+      <c r="AA191" cm="1">
+        <f t="array" ref="AA191">_xlfn.XLOOKUP(E191&amp;I191,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!F$2:F$13000,"")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="192" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A192" s="1">
+        <v>44870</v>
+      </c>
+      <c r="B192" s="2">
+        <v>0.64583333333333337</v>
+      </c>
+      <c r="C192" t="s">
+        <v>25</v>
+      </c>
+      <c r="D192" t="s">
+        <v>107</v>
+      </c>
+      <c r="E192" t="s">
+        <v>49</v>
+      </c>
+      <c r="F192">
+        <v>0</v>
+      </c>
+      <c r="G192">
+        <v>2022</v>
+      </c>
+      <c r="H192">
+        <v>0</v>
+      </c>
+      <c r="I192">
+        <v>10</v>
+      </c>
+      <c r="J192" t="str" cm="1">
+        <f t="array" ref="J192">_xlfn.XLOOKUP(D192&amp;I192,Ranking!C$2:C$500&amp;Ranking!A$2:A$500,Ranking!B$2:B$500,"")</f>
+        <v/>
+      </c>
+      <c r="K192" cm="1">
+        <f t="array" ref="K192">_xlfn.XLOOKUP(E192&amp;I192,Ranking!C$2:C$500&amp;Ranking!A$2:A$500,Ranking!B$2:B$500,"")</f>
+        <v>8</v>
+      </c>
+      <c r="L192" t="s">
+        <v>65</v>
+      </c>
+      <c r="M192" t="s">
+        <v>65</v>
+      </c>
+      <c r="N192">
+        <v>1</v>
+      </c>
+      <c r="O192" cm="1">
+        <f t="array" ref="O192">_xlfn.XLOOKUP(D192&amp;I192,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!C$2:C$13000,"")</f>
+        <v>16.3</v>
+      </c>
+      <c r="P192" cm="1">
+        <f t="array" ref="P192">_xlfn.XLOOKUP(D192&amp;I192,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!D$2:D$13000,"")</f>
+        <v>39.1</v>
+      </c>
+      <c r="Q192" cm="1">
+        <f t="array" ref="Q192">_xlfn.XLOOKUP(E192&amp;I192,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!C$2:C$13000,"")</f>
+        <v>42.4</v>
+      </c>
+      <c r="R192" cm="1">
+        <f t="array" ref="R192">_xlfn.XLOOKUP(E192&amp;I192,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!D$2:D$13000,"")</f>
+        <v>28.4</v>
+      </c>
+      <c r="X192" cm="1">
+        <f t="array" ref="X192">_xlfn.XLOOKUP(D192&amp;I192,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!E$2:E$13000,"")</f>
+        <v>1</v>
+      </c>
+      <c r="Y192" cm="1">
+        <f t="array" ref="Y192">_xlfn.XLOOKUP(D192&amp;I192,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!F$2:F$13000,"")</f>
+        <v>7</v>
+      </c>
+      <c r="Z192" cm="1">
+        <f t="array" ref="Z192">_xlfn.XLOOKUP(E192&amp;I192,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!E$2:E$13000,"")</f>
+        <v>7</v>
+      </c>
+      <c r="AA192" cm="1">
+        <f t="array" ref="AA192">_xlfn.XLOOKUP(E192&amp;I192,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!F$2:F$13000,"")</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="193" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A193" s="1">
+        <v>44870</v>
+      </c>
+      <c r="B193" s="2">
+        <v>0.64583333333333337</v>
+      </c>
+      <c r="C193" t="s">
+        <v>33</v>
+      </c>
+      <c r="D193" t="s">
+        <v>41</v>
+      </c>
+      <c r="E193" t="s">
+        <v>34</v>
+      </c>
+      <c r="F193">
+        <v>0</v>
+      </c>
+      <c r="G193">
+        <v>2022</v>
+      </c>
+      <c r="H193">
+        <v>0</v>
+      </c>
+      <c r="I193">
+        <v>10</v>
+      </c>
+      <c r="J193" t="str" cm="1">
+        <f t="array" ref="J193">_xlfn.XLOOKUP(D193&amp;I193,Ranking!C$2:C$500&amp;Ranking!A$2:A$500,Ranking!B$2:B$500,"")</f>
+        <v/>
+      </c>
+      <c r="K193" cm="1">
+        <f t="array" ref="K193">_xlfn.XLOOKUP(E193&amp;I193,Ranking!C$2:C$500&amp;Ranking!A$2:A$500,Ranking!B$2:B$500,"")</f>
+        <v>15</v>
+      </c>
+      <c r="L193" t="s">
+        <v>64</v>
+      </c>
+      <c r="M193" t="s">
+        <v>64</v>
+      </c>
+      <c r="N193">
+        <v>1</v>
+      </c>
+      <c r="O193" cm="1">
+        <f t="array" ref="O193">_xlfn.XLOOKUP(D193&amp;I193,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!C$2:C$13000,"")</f>
+        <v>24.5</v>
+      </c>
+      <c r="P193" cm="1">
+        <f t="array" ref="P193">_xlfn.XLOOKUP(D193&amp;I193,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!D$2:D$13000,"")</f>
+        <v>30.6</v>
+      </c>
+      <c r="Q193" cm="1">
+        <f t="array" ref="Q193">_xlfn.XLOOKUP(E193&amp;I193,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!C$2:C$13000,"")</f>
+        <v>33.1</v>
+      </c>
+      <c r="R193" cm="1">
+        <f t="array" ref="R193">_xlfn.XLOOKUP(E193&amp;I193,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!D$2:D$13000,"")</f>
+        <v>22</v>
+      </c>
+      <c r="X193" cm="1">
+        <f t="array" ref="X193">_xlfn.XLOOKUP(D193&amp;I193,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!E$2:E$13000,"")</f>
+        <v>3</v>
+      </c>
+      <c r="Y193" cm="1">
+        <f t="array" ref="Y193">_xlfn.XLOOKUP(D193&amp;I193,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!F$2:F$13000,"")</f>
+        <v>5</v>
+      </c>
+      <c r="Z193" cm="1">
+        <f t="array" ref="Z193">_xlfn.XLOOKUP(E193&amp;I193,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!E$2:E$13000,"")</f>
+        <v>6</v>
+      </c>
+      <c r="AA193" cm="1">
+        <f t="array" ref="AA193">_xlfn.XLOOKUP(E193&amp;I193,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!F$2:F$13000,"")</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="194" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A194" s="1">
+        <v>44870</v>
+      </c>
+      <c r="B194" s="2">
+        <v>0.64583333333333337</v>
+      </c>
+      <c r="C194" t="s">
+        <v>47</v>
+      </c>
+      <c r="D194" t="s">
+        <v>146</v>
+      </c>
+      <c r="E194" t="s">
+        <v>88</v>
+      </c>
+      <c r="F194">
+        <v>0</v>
+      </c>
+      <c r="G194">
+        <v>2022</v>
+      </c>
+      <c r="H194">
+        <v>0</v>
+      </c>
+      <c r="I194">
+        <v>10</v>
+      </c>
+      <c r="J194" t="str" cm="1">
+        <f t="array" ref="J194">_xlfn.XLOOKUP(D194&amp;I194,Ranking!C$2:C$500&amp;Ranking!A$2:A$500,Ranking!B$2:B$500,"")</f>
+        <v/>
+      </c>
+      <c r="K194" cm="1">
+        <f t="array" ref="K194">_xlfn.XLOOKUP(E194&amp;I194,Ranking!C$2:C$500&amp;Ranking!A$2:A$500,Ranking!B$2:B$500,"")</f>
+        <v>25</v>
+      </c>
+      <c r="L194" t="s">
+        <v>68</v>
+      </c>
+      <c r="M194" t="s">
+        <v>68</v>
+      </c>
+      <c r="N194">
+        <v>1</v>
+      </c>
+      <c r="O194" cm="1">
+        <f t="array" ref="O194">_xlfn.XLOOKUP(D194&amp;I194,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!C$2:C$13000,"")</f>
+        <v>34.6</v>
+      </c>
+      <c r="P194" cm="1">
+        <f t="array" ref="P194">_xlfn.XLOOKUP(D194&amp;I194,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!D$2:D$13000,"")</f>
+        <v>31.1</v>
+      </c>
+      <c r="Q194" cm="1">
+        <f t="array" ref="Q194">_xlfn.XLOOKUP(E194&amp;I194,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!C$2:C$13000,"")</f>
+        <v>35.799999999999997</v>
+      </c>
+      <c r="R194" cm="1">
+        <f t="array" ref="R194">_xlfn.XLOOKUP(E194&amp;I194,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!D$2:D$13000,"")</f>
+        <v>17.600000000000001</v>
+      </c>
+      <c r="X194" cm="1">
+        <f t="array" ref="X194">_xlfn.XLOOKUP(D194&amp;I194,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!E$2:E$13000,"")</f>
+        <v>4</v>
+      </c>
+      <c r="Y194" cm="1">
+        <f t="array" ref="Y194">_xlfn.XLOOKUP(D194&amp;I194,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!F$2:F$13000,"")</f>
+        <v>4</v>
+      </c>
+      <c r="Z194" cm="1">
+        <f t="array" ref="Z194">_xlfn.XLOOKUP(E194&amp;I194,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!E$2:E$13000,"")</f>
+        <v>6</v>
+      </c>
+      <c r="AA194" cm="1">
+        <f t="array" ref="AA194">_xlfn.XLOOKUP(E194&amp;I194,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!F$2:F$13000,"")</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="195" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A195" s="1">
+        <v>44870</v>
+      </c>
+      <c r="B195" s="3">
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="C195" t="s">
+        <v>25</v>
+      </c>
+      <c r="D195" t="s">
+        <v>114</v>
+      </c>
+      <c r="E195" t="s">
+        <v>91</v>
+      </c>
+      <c r="F195">
+        <v>0</v>
+      </c>
+      <c r="G195">
+        <v>2022</v>
+      </c>
+      <c r="H195">
+        <v>0</v>
+      </c>
+      <c r="I195">
+        <v>10</v>
+      </c>
+      <c r="J195" cm="1">
+        <f t="array" ref="J195">_xlfn.XLOOKUP(D195&amp;I195,Ranking!C$2:C$500&amp;Ranking!A$2:A$500,Ranking!B$2:B$500,"")</f>
+        <v>10</v>
+      </c>
+      <c r="K195" cm="1">
+        <f t="array" ref="K195">_xlfn.XLOOKUP(E195&amp;I195,Ranking!C$2:C$500&amp;Ranking!A$2:A$500,Ranking!B$2:B$500,"")</f>
+        <v>6</v>
+      </c>
+      <c r="L195" t="s">
+        <v>70</v>
+      </c>
+      <c r="M195" t="s">
+        <v>70</v>
+      </c>
+      <c r="N195">
+        <v>1</v>
+      </c>
+      <c r="O195" cm="1">
+        <f t="array" ref="O195">_xlfn.XLOOKUP(D195&amp;I195,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!C$2:C$13000,"")</f>
+        <v>35.1</v>
+      </c>
+      <c r="P195" cm="1">
+        <f t="array" ref="P195">_xlfn.XLOOKUP(D195&amp;I195,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!D$2:D$13000,"")</f>
+        <v>21.1</v>
+      </c>
+      <c r="Q195" cm="1">
+        <f t="array" ref="Q195">_xlfn.XLOOKUP(E195&amp;I195,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!C$2:C$13000,"")</f>
+        <v>43.1</v>
+      </c>
+      <c r="R195" cm="1">
+        <f t="array" ref="R195">_xlfn.XLOOKUP(E195&amp;I195,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!D$2:D$13000,"")</f>
+        <v>16.600000000000001</v>
+      </c>
+      <c r="X195" cm="1">
+        <f t="array" ref="X195">_xlfn.XLOOKUP(D195&amp;I195,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!E$2:E$13000,"")</f>
+        <v>6</v>
+      </c>
+      <c r="Y195" cm="1">
+        <f t="array" ref="Y195">_xlfn.XLOOKUP(D195&amp;I195,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!F$2:F$13000,"")</f>
+        <v>2</v>
+      </c>
+      <c r="Z195" cm="1">
+        <f t="array" ref="Z195">_xlfn.XLOOKUP(E195&amp;I195,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!E$2:E$13000,"")</f>
+        <v>7</v>
+      </c>
+      <c r="AA195" cm="1">
+        <f t="array" ref="AA195">_xlfn.XLOOKUP(E195&amp;I195,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!F$2:F$13000,"")</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="196" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A196" s="1">
+        <v>44870</v>
+      </c>
+      <c r="B196" s="2">
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="C196" t="s">
+        <v>31</v>
+      </c>
+      <c r="D196" t="s">
+        <v>93</v>
+      </c>
+      <c r="E196" t="s">
+        <v>90</v>
+      </c>
+      <c r="F196">
+        <v>0</v>
+      </c>
+      <c r="G196">
+        <v>2022</v>
+      </c>
+      <c r="H196">
+        <v>0</v>
+      </c>
+      <c r="I196">
+        <v>10</v>
+      </c>
+      <c r="J196" cm="1">
+        <f t="array" ref="J196">_xlfn.XLOOKUP(D196&amp;I196,Ranking!C$2:C$500&amp;Ranking!A$2:A$500,Ranking!B$2:B$500,"")</f>
+        <v>13</v>
+      </c>
+      <c r="K196" cm="1">
+        <f t="array" ref="K196">_xlfn.XLOOKUP(E196&amp;I196,Ranking!C$2:C$500&amp;Ranking!A$2:A$500,Ranking!B$2:B$500,"")</f>
+        <v>24</v>
+      </c>
+      <c r="L196" t="s">
+        <v>71</v>
+      </c>
+      <c r="M196" t="s">
+        <v>71</v>
+      </c>
+      <c r="N196">
+        <v>1</v>
+      </c>
+      <c r="O196" cm="1">
+        <f t="array" ref="O196">_xlfn.XLOOKUP(D196&amp;I196,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!C$2:C$13000,"")</f>
+        <v>31</v>
+      </c>
+      <c r="P196" cm="1">
+        <f t="array" ref="P196">_xlfn.XLOOKUP(D196&amp;I196,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!D$2:D$13000,"")</f>
+        <v>17.3</v>
+      </c>
+      <c r="Q196" cm="1">
+        <f t="array" ref="Q196">_xlfn.XLOOKUP(E196&amp;I196,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!C$2:C$13000,"")</f>
+        <v>36.4</v>
+      </c>
+      <c r="R196" cm="1">
+        <f t="array" ref="R196">_xlfn.XLOOKUP(E196&amp;I196,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!D$2:D$13000,"")</f>
+        <v>21.1</v>
+      </c>
+      <c r="X196" cm="1">
+        <f t="array" ref="X196">_xlfn.XLOOKUP(D196&amp;I196,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!E$2:E$13000,"")</f>
+        <v>6</v>
+      </c>
+      <c r="Y196" cm="1">
+        <f t="array" ref="Y196">_xlfn.XLOOKUP(D196&amp;I196,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!F$2:F$13000,"")</f>
+        <v>2</v>
+      </c>
+      <c r="Z196" cm="1">
+        <f t="array" ref="Z196">_xlfn.XLOOKUP(E196&amp;I196,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!E$2:E$13000,"")</f>
+        <v>5</v>
+      </c>
+      <c r="AA196" cm="1">
+        <f t="array" ref="AA196">_xlfn.XLOOKUP(E196&amp;I196,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!F$2:F$13000,"")</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="197" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A197" s="1">
+        <v>44870</v>
+      </c>
+      <c r="B197" s="2">
+        <v>0.8125</v>
+      </c>
+      <c r="C197" t="s">
+        <v>47</v>
+      </c>
+      <c r="D197" t="s">
+        <v>113</v>
+      </c>
+      <c r="E197" t="s">
+        <v>122</v>
+      </c>
+      <c r="F197">
+        <v>0</v>
+      </c>
+      <c r="G197">
+        <v>2022</v>
+      </c>
+      <c r="H197">
+        <v>0</v>
+      </c>
+      <c r="I197">
+        <v>10</v>
+      </c>
+      <c r="J197" t="str" cm="1">
+        <f t="array" ref="J197">_xlfn.XLOOKUP(D197&amp;I197,Ranking!C$2:C$500&amp;Ranking!A$2:A$500,Ranking!B$2:B$500,"")</f>
+        <v/>
+      </c>
+      <c r="K197" t="str" cm="1">
+        <f t="array" ref="K197">_xlfn.XLOOKUP(E197&amp;I197,Ranking!C$2:C$500&amp;Ranking!A$2:A$500,Ranking!B$2:B$500,"")</f>
+        <v/>
+      </c>
+      <c r="L197" t="s">
+        <v>70</v>
+      </c>
+      <c r="M197" t="s">
+        <v>70</v>
+      </c>
+      <c r="N197">
+        <v>1</v>
+      </c>
+      <c r="O197" cm="1">
+        <f t="array" ref="O197">_xlfn.XLOOKUP(D197&amp;I197,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!C$2:C$13000,"")</f>
+        <v>31.8</v>
+      </c>
+      <c r="P197" cm="1">
+        <f t="array" ref="P197">_xlfn.XLOOKUP(D197&amp;I197,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!D$2:D$13000,"")</f>
+        <v>22.9</v>
+      </c>
+      <c r="Q197" cm="1">
+        <f t="array" ref="Q197">_xlfn.XLOOKUP(E197&amp;I197,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!C$2:C$13000,"")</f>
+        <v>22.9</v>
+      </c>
+      <c r="R197" cm="1">
+        <f t="array" ref="R197">_xlfn.XLOOKUP(E197&amp;I197,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!D$2:D$13000,"")</f>
+        <v>29.9</v>
+      </c>
+      <c r="X197" cm="1">
+        <f t="array" ref="X197">_xlfn.XLOOKUP(D197&amp;I197,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!E$2:E$13000,"")</f>
+        <v>5</v>
+      </c>
+      <c r="Y197" cm="1">
+        <f t="array" ref="Y197">_xlfn.XLOOKUP(D197&amp;I197,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!F$2:F$13000,"")</f>
+        <v>3</v>
+      </c>
+      <c r="Z197" cm="1">
+        <f t="array" ref="Z197">_xlfn.XLOOKUP(E197&amp;I197,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!E$2:E$13000,"")</f>
+        <v>3</v>
+      </c>
+      <c r="AA197" cm="1">
+        <f t="array" ref="AA197">_xlfn.XLOOKUP(E197&amp;I197,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!F$2:F$13000,"")</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="198" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A198" s="1">
+        <v>44870</v>
+      </c>
+      <c r="B198" s="2">
+        <v>0.8125</v>
+      </c>
+      <c r="C198" t="s">
+        <v>33</v>
+      </c>
+      <c r="D198" t="s">
+        <v>147</v>
+      </c>
+      <c r="E198" t="s">
+        <v>115</v>
+      </c>
+      <c r="F198">
+        <v>0</v>
+      </c>
+      <c r="G198">
+        <v>2022</v>
+      </c>
+      <c r="H198">
+        <v>0</v>
+      </c>
+      <c r="I198">
+        <v>10</v>
+      </c>
+      <c r="J198" t="str" cm="1">
+        <f t="array" ref="J198">_xlfn.XLOOKUP(D198&amp;I198,Ranking!C$2:C$500&amp;Ranking!A$2:A$500,Ranking!B$2:B$500,"")</f>
+        <v/>
+      </c>
+      <c r="K198" t="str" cm="1">
+        <f t="array" ref="K198">_xlfn.XLOOKUP(E198&amp;I198,Ranking!C$2:C$500&amp;Ranking!A$2:A$500,Ranking!B$2:B$500,"")</f>
+        <v/>
+      </c>
+      <c r="L198" t="s">
+        <v>69</v>
+      </c>
+      <c r="M198" t="s">
+        <v>69</v>
+      </c>
+      <c r="N198">
+        <v>1</v>
+      </c>
+      <c r="O198" cm="1">
+        <f t="array" ref="O198">_xlfn.XLOOKUP(D198&amp;I198,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!C$2:C$13000,"")</f>
+        <v>27.4</v>
+      </c>
+      <c r="P198" cm="1">
+        <f t="array" ref="P198">_xlfn.XLOOKUP(D198&amp;I198,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!D$2:D$13000,"")</f>
+        <v>22.5</v>
+      </c>
+      <c r="Q198" cm="1">
+        <f t="array" ref="Q198">_xlfn.XLOOKUP(E198&amp;I198,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!C$2:C$13000,"")</f>
+        <v>32.1</v>
+      </c>
+      <c r="R198" cm="1">
+        <f t="array" ref="R198">_xlfn.XLOOKUP(E198&amp;I198,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!D$2:D$13000,"")</f>
+        <v>21.9</v>
+      </c>
+      <c r="X198" cm="1">
+        <f t="array" ref="X198">_xlfn.XLOOKUP(D198&amp;I198,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!E$2:E$13000,"")</f>
+        <v>4</v>
+      </c>
+      <c r="Y198" cm="1">
+        <f t="array" ref="Y198">_xlfn.XLOOKUP(D198&amp;I198,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!F$2:F$13000,"")</f>
+        <v>4</v>
+      </c>
+      <c r="Z198" cm="1">
+        <f t="array" ref="Z198">_xlfn.XLOOKUP(E198&amp;I198,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!E$2:E$13000,"")</f>
+        <v>5</v>
+      </c>
+      <c r="AA198" cm="1">
+        <f t="array" ref="AA198">_xlfn.XLOOKUP(E198&amp;I198,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!F$2:F$13000,"")</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="199" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A199" s="1">
+        <v>44870</v>
+      </c>
+      <c r="B199" s="2">
+        <v>0.89583333333333337</v>
+      </c>
+      <c r="C199" t="s">
+        <v>31</v>
+      </c>
+      <c r="D199" t="s">
+        <v>96</v>
+      </c>
+      <c r="E199" t="s">
+        <v>175</v>
+      </c>
+      <c r="F199">
+        <v>0</v>
+      </c>
+      <c r="G199">
+        <v>2022</v>
+      </c>
+      <c r="H199">
+        <v>0</v>
+      </c>
+      <c r="I199">
+        <v>10</v>
+      </c>
+      <c r="J199" t="str" cm="1">
+        <f t="array" ref="J199">_xlfn.XLOOKUP(D199&amp;I199,Ranking!C$2:C$500&amp;Ranking!A$2:A$500,Ranking!B$2:B$500,"")</f>
+        <v/>
+      </c>
+      <c r="K199" cm="1">
+        <f t="array" ref="K199">_xlfn.XLOOKUP(E199&amp;I199,Ranking!C$2:C$500&amp;Ranking!A$2:A$500,Ranking!B$2:B$500,"")</f>
+        <v>12</v>
+      </c>
+      <c r="L199" t="s">
+        <v>65</v>
+      </c>
+      <c r="M199" t="s">
+        <v>65</v>
+      </c>
+      <c r="N199">
+        <v>1</v>
+      </c>
+      <c r="O199" cm="1">
+        <f t="array" ref="O199">_xlfn.XLOOKUP(D199&amp;I199,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!C$2:C$13000,"")</f>
+        <v>27.1</v>
+      </c>
+      <c r="P199" cm="1">
+        <f t="array" ref="P199">_xlfn.XLOOKUP(D199&amp;I199,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!D$2:D$13000,"")</f>
+        <v>28.8</v>
+      </c>
+      <c r="Q199" cm="1">
+        <f t="array" ref="Q199">_xlfn.XLOOKUP(E199&amp;I199,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!C$2:C$13000,"")</f>
+        <v>39.6</v>
+      </c>
+      <c r="R199" cm="1">
+        <f t="array" ref="R199">_xlfn.XLOOKUP(E199&amp;I199,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!D$2:D$13000,"")</f>
+        <v>24.3</v>
+      </c>
+      <c r="X199" cm="1">
+        <f t="array" ref="X199">_xlfn.XLOOKUP(D199&amp;I199,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!E$2:E$13000,"")</f>
+        <v>3</v>
+      </c>
+      <c r="Y199" cm="1">
+        <f t="array" ref="Y199">_xlfn.XLOOKUP(D199&amp;I199,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!F$2:F$13000,"")</f>
+        <v>5</v>
+      </c>
+      <c r="Z199" cm="1">
+        <f t="array" ref="Z199">_xlfn.XLOOKUP(E199&amp;I199,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!E$2:E$13000,"")</f>
+        <v>7</v>
+      </c>
+      <c r="AA199" cm="1">
+        <f t="array" ref="AA199">_xlfn.XLOOKUP(E199&amp;I199,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!F$2:F$13000,"")</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="200" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A200" s="1">
+        <v>44870</v>
+      </c>
+      <c r="B200" s="2">
+        <v>0.9375</v>
+      </c>
+      <c r="C200" t="s">
+        <v>25</v>
+      </c>
+      <c r="D200" t="s">
+        <v>110</v>
+      </c>
+      <c r="E200" t="s">
+        <v>127</v>
+      </c>
+      <c r="F200">
+        <v>0</v>
+      </c>
+      <c r="G200">
+        <v>2022</v>
+      </c>
+      <c r="H200">
+        <v>0</v>
+      </c>
+      <c r="I200">
+        <v>10</v>
+      </c>
+      <c r="J200" cm="1">
+        <f t="array" ref="J200">_xlfn.XLOOKUP(D200&amp;I200,Ranking!C$2:C$500&amp;Ranking!A$2:A$500,Ranking!B$2:B$500,"")</f>
+        <v>9</v>
+      </c>
+      <c r="K200" t="str" cm="1">
+        <f t="array" ref="K200">_xlfn.XLOOKUP(E200&amp;I200,Ranking!C$2:C$500&amp;Ranking!A$2:A$500,Ranking!B$2:B$500,"")</f>
+        <v/>
+      </c>
+      <c r="L200" t="s">
+        <v>65</v>
+      </c>
+      <c r="M200" t="s">
+        <v>65</v>
+      </c>
+      <c r="N200">
+        <v>1</v>
+      </c>
+      <c r="O200" cm="1">
+        <f t="array" ref="O200">_xlfn.XLOOKUP(D200&amp;I200,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!C$2:C$13000,"")</f>
+        <v>41</v>
+      </c>
+      <c r="P200" cm="1">
+        <f t="array" ref="P200">_xlfn.XLOOKUP(D200&amp;I200,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!D$2:D$13000,"")</f>
+        <v>24</v>
+      </c>
+      <c r="Q200" cm="1">
+        <f t="array" ref="Q200">_xlfn.XLOOKUP(E200&amp;I200,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!C$2:C$13000,"")</f>
+        <v>23.4</v>
+      </c>
+      <c r="R200" cm="1">
+        <f t="array" ref="R200">_xlfn.XLOOKUP(E200&amp;I200,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!D$2:D$13000,"")</f>
+        <v>25</v>
+      </c>
+      <c r="X200" cm="1">
+        <f t="array" ref="X200">_xlfn.XLOOKUP(D200&amp;I200,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!E$2:E$13000,"")</f>
+        <v>7</v>
+      </c>
+      <c r="Y200" cm="1">
+        <f t="array" ref="Y200">_xlfn.XLOOKUP(D200&amp;I200,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!F$2:F$13000,"")</f>
+        <v>1</v>
+      </c>
+      <c r="Z200" cm="1">
+        <f t="array" ref="Z200">_xlfn.XLOOKUP(E200&amp;I200,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!E$2:E$13000,"")</f>
+        <v>3</v>
+      </c>
+      <c r="AA200" cm="1">
+        <f t="array" ref="AA200">_xlfn.XLOOKUP(E200&amp;I200,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!F$2:F$13000,"")</f>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -16849,10 +18488,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF262906-C2E8-EB40-9ABF-94137CE271DB}">
-  <dimension ref="A1:F1047"/>
+  <dimension ref="A1:F1178"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G747" sqref="G747"/>
+    <sheetView topLeftCell="A1151" workbookViewId="0">
+      <selection activeCell="D1141" sqref="D1141"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -37794,6 +39433,2626 @@
         <v>5</v>
       </c>
       <c r="F1047">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1048" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1048" t="s">
+        <v>106</v>
+      </c>
+      <c r="B1048">
+        <v>10</v>
+      </c>
+      <c r="C1048">
+        <v>30.9</v>
+      </c>
+      <c r="D1048">
+        <v>16.8</v>
+      </c>
+      <c r="E1048">
+        <v>5</v>
+      </c>
+      <c r="F1048">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1049" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1049" t="s">
+        <v>119</v>
+      </c>
+      <c r="B1049">
+        <v>10</v>
+      </c>
+      <c r="C1049">
+        <v>18.600000000000001</v>
+      </c>
+      <c r="D1049">
+        <v>37</v>
+      </c>
+      <c r="E1049">
+        <v>1</v>
+      </c>
+      <c r="F1049">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="1050" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1050" t="s">
+        <v>91</v>
+      </c>
+      <c r="B1050">
+        <v>10</v>
+      </c>
+      <c r="C1050">
+        <v>43.1</v>
+      </c>
+      <c r="D1050">
+        <v>16.600000000000001</v>
+      </c>
+      <c r="E1050">
+        <v>7</v>
+      </c>
+      <c r="F1050">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1051" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1051" t="s">
+        <v>102</v>
+      </c>
+      <c r="B1051">
+        <v>10</v>
+      </c>
+      <c r="C1051">
+        <v>36.9</v>
+      </c>
+      <c r="D1051">
+        <v>24.1</v>
+      </c>
+      <c r="E1051">
+        <v>5</v>
+      </c>
+      <c r="F1051">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1052" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1052" t="s">
+        <v>112</v>
+      </c>
+      <c r="B1052">
+        <v>10</v>
+      </c>
+      <c r="C1052">
+        <v>32.299999999999997</v>
+      </c>
+      <c r="D1052">
+        <v>37.4</v>
+      </c>
+      <c r="E1052">
+        <v>3</v>
+      </c>
+      <c r="F1052">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1053" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1053" t="s">
+        <v>96</v>
+      </c>
+      <c r="B1053">
+        <v>10</v>
+      </c>
+      <c r="C1053">
+        <v>27.1</v>
+      </c>
+      <c r="D1053">
+        <v>28.8</v>
+      </c>
+      <c r="E1053">
+        <v>3</v>
+      </c>
+      <c r="F1053">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1054" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1054" t="s">
+        <v>50</v>
+      </c>
+      <c r="B1054">
+        <v>10</v>
+      </c>
+      <c r="C1054">
+        <v>33.799999999999997</v>
+      </c>
+      <c r="D1054">
+        <v>31.9</v>
+      </c>
+      <c r="E1054">
+        <v>5</v>
+      </c>
+      <c r="F1054">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1055" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1055" t="s">
+        <v>120</v>
+      </c>
+      <c r="B1055">
+        <v>10</v>
+      </c>
+      <c r="C1055">
+        <v>25.9</v>
+      </c>
+      <c r="D1055">
+        <v>31.1</v>
+      </c>
+      <c r="E1055">
+        <v>2</v>
+      </c>
+      <c r="F1055">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1056" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1056" t="s">
+        <v>121</v>
+      </c>
+      <c r="B1056">
+        <v>10</v>
+      </c>
+      <c r="C1056">
+        <v>32.700000000000003</v>
+      </c>
+      <c r="D1056">
+        <v>29.4</v>
+      </c>
+      <c r="E1056">
+        <v>3</v>
+      </c>
+      <c r="F1056">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1057" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1057" t="s">
+        <v>122</v>
+      </c>
+      <c r="B1057">
+        <v>10</v>
+      </c>
+      <c r="C1057">
+        <v>22.9</v>
+      </c>
+      <c r="D1057">
+        <v>29.9</v>
+      </c>
+      <c r="E1057">
+        <v>3</v>
+      </c>
+      <c r="F1057">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1058" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1058" t="s">
+        <v>123</v>
+      </c>
+      <c r="B1058">
+        <v>10</v>
+      </c>
+      <c r="C1058">
+        <v>24.5</v>
+      </c>
+      <c r="D1058">
+        <v>28.1</v>
+      </c>
+      <c r="E1058">
+        <v>4</v>
+      </c>
+      <c r="F1058">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1059" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1059" t="s">
+        <v>98</v>
+      </c>
+      <c r="B1059">
+        <v>10</v>
+      </c>
+      <c r="C1059">
+        <v>38.4</v>
+      </c>
+      <c r="D1059">
+        <v>23.3</v>
+      </c>
+      <c r="E1059">
+        <v>5</v>
+      </c>
+      <c r="F1059">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1060" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1060" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1060">
+        <v>10</v>
+      </c>
+      <c r="C1060">
+        <v>28.9</v>
+      </c>
+      <c r="D1060">
+        <v>17.399999999999999</v>
+      </c>
+      <c r="E1060">
+        <v>6</v>
+      </c>
+      <c r="F1060">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1061" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1061" t="s">
+        <v>124</v>
+      </c>
+      <c r="B1061">
+        <v>10</v>
+      </c>
+      <c r="C1061">
+        <v>17.3</v>
+      </c>
+      <c r="D1061">
+        <v>28.8</v>
+      </c>
+      <c r="E1061">
+        <v>2</v>
+      </c>
+      <c r="F1061">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1062" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1062" t="s">
+        <v>125</v>
+      </c>
+      <c r="B1062">
+        <v>10</v>
+      </c>
+      <c r="C1062">
+        <v>26.4</v>
+      </c>
+      <c r="D1062">
+        <v>34.6</v>
+      </c>
+      <c r="E1062">
+        <v>4</v>
+      </c>
+      <c r="F1062">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1063" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1063" t="s">
+        <v>126</v>
+      </c>
+      <c r="B1063">
+        <v>10</v>
+      </c>
+      <c r="C1063">
+        <v>30.9</v>
+      </c>
+      <c r="D1063">
+        <v>24.8</v>
+      </c>
+      <c r="E1063">
+        <v>5</v>
+      </c>
+      <c r="F1063">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1064" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1064" t="s">
+        <v>97</v>
+      </c>
+      <c r="B1064">
+        <v>10</v>
+      </c>
+      <c r="C1064">
+        <v>29.4</v>
+      </c>
+      <c r="D1064">
+        <v>31.1</v>
+      </c>
+      <c r="E1064">
+        <v>4</v>
+      </c>
+      <c r="F1064">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1065" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1065" t="s">
+        <v>127</v>
+      </c>
+      <c r="B1065">
+        <v>10</v>
+      </c>
+      <c r="C1065">
+        <v>23.4</v>
+      </c>
+      <c r="D1065">
+        <v>25</v>
+      </c>
+      <c r="E1065">
+        <v>3</v>
+      </c>
+      <c r="F1065">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1066" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1066" t="s">
+        <v>61</v>
+      </c>
+      <c r="B1066">
+        <v>10</v>
+      </c>
+      <c r="C1066">
+        <v>25.3</v>
+      </c>
+      <c r="D1066">
+        <v>29.9</v>
+      </c>
+      <c r="E1066">
+        <v>2</v>
+      </c>
+      <c r="F1066">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1067" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1067" t="s">
+        <v>82</v>
+      </c>
+      <c r="B1067">
+        <v>10</v>
+      </c>
+      <c r="C1067">
+        <v>27.3</v>
+      </c>
+      <c r="D1067">
+        <v>41</v>
+      </c>
+      <c r="E1067">
+        <v>2</v>
+      </c>
+      <c r="F1067">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1068" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1068" t="s">
+        <v>57</v>
+      </c>
+      <c r="B1068">
+        <v>10</v>
+      </c>
+      <c r="C1068">
+        <v>34.9</v>
+      </c>
+      <c r="D1068">
+        <v>22.4</v>
+      </c>
+      <c r="E1068">
+        <v>6</v>
+      </c>
+      <c r="F1068">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1069" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1069" t="s">
+        <v>87</v>
+      </c>
+      <c r="B1069">
+        <v>10</v>
+      </c>
+      <c r="C1069">
+        <v>37.1</v>
+      </c>
+      <c r="D1069">
+        <v>19.899999999999999</v>
+      </c>
+      <c r="E1069">
+        <v>8</v>
+      </c>
+      <c r="F1069">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1070" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1070" t="s">
+        <v>128</v>
+      </c>
+      <c r="B1070">
+        <v>10</v>
+      </c>
+      <c r="C1070">
+        <v>31.9</v>
+      </c>
+      <c r="D1070">
+        <v>27.3</v>
+      </c>
+      <c r="E1070">
+        <v>7</v>
+      </c>
+      <c r="F1070">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1071" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1071" t="s">
+        <v>107</v>
+      </c>
+      <c r="B1071">
+        <v>10</v>
+      </c>
+      <c r="C1071">
+        <v>16.3</v>
+      </c>
+      <c r="D1071">
+        <v>39.1</v>
+      </c>
+      <c r="E1071">
+        <v>1</v>
+      </c>
+      <c r="F1071">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1072" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1072" t="s">
+        <v>59</v>
+      </c>
+      <c r="B1072">
+        <v>10</v>
+      </c>
+      <c r="C1072">
+        <v>12.5</v>
+      </c>
+      <c r="D1072">
+        <v>32.1</v>
+      </c>
+      <c r="E1072">
+        <v>2</v>
+      </c>
+      <c r="F1072">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1073" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1073" t="s">
+        <v>80</v>
+      </c>
+      <c r="B1073">
+        <v>10</v>
+      </c>
+      <c r="C1073">
+        <v>17.600000000000001</v>
+      </c>
+      <c r="D1073">
+        <v>26.2</v>
+      </c>
+      <c r="E1073">
+        <v>4</v>
+      </c>
+      <c r="F1073">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1074" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1074" t="s">
+        <v>129</v>
+      </c>
+      <c r="B1074">
+        <v>10</v>
+      </c>
+      <c r="C1074">
+        <v>34.4</v>
+      </c>
+      <c r="D1074">
+        <v>22.1</v>
+      </c>
+      <c r="E1074">
+        <v>5</v>
+      </c>
+      <c r="F1074">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1075" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1075" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1075">
+        <v>10</v>
+      </c>
+      <c r="C1075">
+        <v>32.6</v>
+      </c>
+      <c r="D1075">
+        <v>23.2</v>
+      </c>
+      <c r="E1075">
+        <v>6</v>
+      </c>
+      <c r="F1075">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1076" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1076" t="s">
+        <v>130</v>
+      </c>
+      <c r="B1076">
+        <v>10</v>
+      </c>
+      <c r="C1076">
+        <v>27</v>
+      </c>
+      <c r="D1076">
+        <v>30.2</v>
+      </c>
+      <c r="E1076">
+        <v>5</v>
+      </c>
+      <c r="F1076">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1077" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1077" t="s">
+        <v>52</v>
+      </c>
+      <c r="B1077">
+        <v>10</v>
+      </c>
+      <c r="C1077">
+        <v>30</v>
+      </c>
+      <c r="D1077">
+        <v>29.9</v>
+      </c>
+      <c r="E1077">
+        <v>4</v>
+      </c>
+      <c r="F1077">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1078" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1078" t="s">
+        <v>81</v>
+      </c>
+      <c r="B1078">
+        <v>10</v>
+      </c>
+      <c r="C1078">
+        <v>28.1</v>
+      </c>
+      <c r="D1078">
+        <v>25.7</v>
+      </c>
+      <c r="E1078">
+        <v>4</v>
+      </c>
+      <c r="F1078">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1079" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1079" t="s">
+        <v>131</v>
+      </c>
+      <c r="B1079">
+        <v>10</v>
+      </c>
+      <c r="C1079">
+        <v>21.1</v>
+      </c>
+      <c r="D1079">
+        <v>33.799999999999997</v>
+      </c>
+      <c r="E1079">
+        <v>4</v>
+      </c>
+      <c r="F1079">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1080" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1080" t="s">
+        <v>115</v>
+      </c>
+      <c r="B1080">
+        <v>10</v>
+      </c>
+      <c r="C1080">
+        <v>32.1</v>
+      </c>
+      <c r="D1080">
+        <v>21.9</v>
+      </c>
+      <c r="E1080">
+        <v>5</v>
+      </c>
+      <c r="F1080">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1081" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1081" t="s">
+        <v>132</v>
+      </c>
+      <c r="B1081">
+        <v>10</v>
+      </c>
+      <c r="C1081">
+        <v>26</v>
+      </c>
+      <c r="D1081">
+        <v>24.1</v>
+      </c>
+      <c r="E1081">
+        <v>4</v>
+      </c>
+      <c r="F1081">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1082" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1082" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1082">
+        <v>10</v>
+      </c>
+      <c r="C1082">
+        <v>41.8</v>
+      </c>
+      <c r="D1082">
+        <v>10.5</v>
+      </c>
+      <c r="E1082">
+        <v>8</v>
+      </c>
+      <c r="F1082">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1083" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1083" t="s">
+        <v>111</v>
+      </c>
+      <c r="B1083">
+        <v>10</v>
+      </c>
+      <c r="C1083">
+        <v>36.9</v>
+      </c>
+      <c r="D1083">
+        <v>30.4</v>
+      </c>
+      <c r="E1083">
+        <v>5</v>
+      </c>
+      <c r="F1083">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1084" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1084" t="s">
+        <v>133</v>
+      </c>
+      <c r="B1084">
+        <v>10</v>
+      </c>
+      <c r="C1084">
+        <v>28.4</v>
+      </c>
+      <c r="D1084">
+        <v>32.4</v>
+      </c>
+      <c r="E1084">
+        <v>3</v>
+      </c>
+      <c r="F1084">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1085" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1085" t="s">
+        <v>86</v>
+      </c>
+      <c r="B1085">
+        <v>10</v>
+      </c>
+      <c r="C1085">
+        <v>16.100000000000001</v>
+      </c>
+      <c r="D1085">
+        <v>28.1</v>
+      </c>
+      <c r="E1085">
+        <v>3</v>
+      </c>
+      <c r="F1085">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1086" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1086" t="s">
+        <v>134</v>
+      </c>
+      <c r="B1086">
+        <v>10</v>
+      </c>
+      <c r="C1086">
+        <v>18.3</v>
+      </c>
+      <c r="D1086">
+        <v>33.700000000000003</v>
+      </c>
+      <c r="E1086">
+        <v>2</v>
+      </c>
+      <c r="F1086">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1087" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1087" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1087">
+        <v>10</v>
+      </c>
+      <c r="C1087">
+        <v>33.5</v>
+      </c>
+      <c r="D1087">
+        <v>31.1</v>
+      </c>
+      <c r="E1087">
+        <v>5</v>
+      </c>
+      <c r="F1087">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1088" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1088" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1088">
+        <v>10</v>
+      </c>
+      <c r="C1088">
+        <v>26</v>
+      </c>
+      <c r="D1088">
+        <v>8.9</v>
+      </c>
+      <c r="E1088">
+        <v>7</v>
+      </c>
+      <c r="F1088">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1089" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1089" t="s">
+        <v>41</v>
+      </c>
+      <c r="B1089">
+        <v>10</v>
+      </c>
+      <c r="C1089">
+        <v>24.5</v>
+      </c>
+      <c r="D1089">
+        <v>30.6</v>
+      </c>
+      <c r="E1089">
+        <v>3</v>
+      </c>
+      <c r="F1089">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1090" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1090" t="s">
+        <v>135</v>
+      </c>
+      <c r="B1090">
+        <v>10</v>
+      </c>
+      <c r="C1090">
+        <v>16.399999999999999</v>
+      </c>
+      <c r="D1090">
+        <v>15.8</v>
+      </c>
+      <c r="E1090">
+        <v>4</v>
+      </c>
+      <c r="F1090">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1091" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1091" t="s">
+        <v>136</v>
+      </c>
+      <c r="B1091">
+        <v>10</v>
+      </c>
+      <c r="C1091">
+        <v>21.6</v>
+      </c>
+      <c r="D1091">
+        <v>16.600000000000001</v>
+      </c>
+      <c r="E1091">
+        <v>3</v>
+      </c>
+      <c r="F1091">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1092" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1092" t="s">
+        <v>137</v>
+      </c>
+      <c r="B1092">
+        <v>10</v>
+      </c>
+      <c r="C1092">
+        <v>38.700000000000003</v>
+      </c>
+      <c r="D1092">
+        <v>20.9</v>
+      </c>
+      <c r="E1092">
+        <v>5</v>
+      </c>
+      <c r="F1092">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1093" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1093" t="s">
+        <v>138</v>
+      </c>
+      <c r="B1093">
+        <v>10</v>
+      </c>
+      <c r="C1093">
+        <v>38</v>
+      </c>
+      <c r="D1093">
+        <v>30.6</v>
+      </c>
+      <c r="E1093">
+        <v>5</v>
+      </c>
+      <c r="F1093">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1094" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1094" t="s">
+        <v>93</v>
+      </c>
+      <c r="B1094">
+        <v>10</v>
+      </c>
+      <c r="C1094">
+        <v>31</v>
+      </c>
+      <c r="D1094">
+        <v>17.3</v>
+      </c>
+      <c r="E1094">
+        <v>6</v>
+      </c>
+      <c r="F1094">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1095" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1095" t="s">
+        <v>139</v>
+      </c>
+      <c r="B1095">
+        <v>10</v>
+      </c>
+      <c r="C1095">
+        <v>28.4</v>
+      </c>
+      <c r="D1095">
+        <v>32.1</v>
+      </c>
+      <c r="E1095">
+        <v>3</v>
+      </c>
+      <c r="F1095">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1096" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1096" t="s">
+        <v>108</v>
+      </c>
+      <c r="B1096">
+        <v>10</v>
+      </c>
+      <c r="C1096">
+        <v>23.9</v>
+      </c>
+      <c r="D1096">
+        <v>19.899999999999999</v>
+      </c>
+      <c r="E1096">
+        <v>5</v>
+      </c>
+      <c r="F1096">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1097" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1097" t="s">
+        <v>140</v>
+      </c>
+      <c r="B1097">
+        <v>10</v>
+      </c>
+      <c r="C1097">
+        <v>31.1</v>
+      </c>
+      <c r="D1097">
+        <v>21.5</v>
+      </c>
+      <c r="E1097">
+        <v>7</v>
+      </c>
+      <c r="F1097">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1098" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1098" t="s">
+        <v>141</v>
+      </c>
+      <c r="B1098">
+        <v>10</v>
+      </c>
+      <c r="C1098">
+        <v>31.6</v>
+      </c>
+      <c r="D1098">
+        <v>39.6</v>
+      </c>
+      <c r="E1098">
+        <v>2</v>
+      </c>
+      <c r="F1098">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1099" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1099" t="s">
+        <v>142</v>
+      </c>
+      <c r="B1099">
+        <v>10</v>
+      </c>
+      <c r="C1099">
+        <v>26.6</v>
+      </c>
+      <c r="D1099">
+        <v>21.5</v>
+      </c>
+      <c r="E1099">
+        <v>4</v>
+      </c>
+      <c r="F1099">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1100" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1100" t="s">
+        <v>143</v>
+      </c>
+      <c r="B1100">
+        <v>10</v>
+      </c>
+      <c r="C1100">
+        <v>22.5</v>
+      </c>
+      <c r="D1100">
+        <v>37.6</v>
+      </c>
+      <c r="E1100">
+        <v>2</v>
+      </c>
+      <c r="F1100">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1101" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1101" t="s">
+        <v>89</v>
+      </c>
+      <c r="B1101">
+        <v>10</v>
+      </c>
+      <c r="C1101">
+        <v>29.8</v>
+      </c>
+      <c r="D1101">
+        <v>20.6</v>
+      </c>
+      <c r="E1101">
+        <v>5</v>
+      </c>
+      <c r="F1101">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1102" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1102" t="s">
+        <v>114</v>
+      </c>
+      <c r="B1102">
+        <v>10</v>
+      </c>
+      <c r="C1102">
+        <v>35.1</v>
+      </c>
+      <c r="D1102">
+        <v>21.1</v>
+      </c>
+      <c r="E1102">
+        <v>6</v>
+      </c>
+      <c r="F1102">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1103" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1103" t="s">
+        <v>100</v>
+      </c>
+      <c r="B1103">
+        <v>10</v>
+      </c>
+      <c r="C1103">
+        <v>24.9</v>
+      </c>
+      <c r="D1103">
+        <v>17.5</v>
+      </c>
+      <c r="E1103">
+        <v>4</v>
+      </c>
+      <c r="F1103">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1104" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1104" t="s">
+        <v>144</v>
+      </c>
+      <c r="B1104">
+        <v>10</v>
+      </c>
+      <c r="C1104">
+        <v>34.1</v>
+      </c>
+      <c r="D1104">
+        <v>24.1</v>
+      </c>
+      <c r="E1104">
+        <v>6</v>
+      </c>
+      <c r="F1104">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1105" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1105" t="s">
+        <v>145</v>
+      </c>
+      <c r="B1105">
+        <v>10</v>
+      </c>
+      <c r="C1105">
+        <v>12.1</v>
+      </c>
+      <c r="D1105">
+        <v>30.9</v>
+      </c>
+      <c r="E1105">
+        <v>1</v>
+      </c>
+      <c r="F1105">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1106" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1106" t="s">
+        <v>146</v>
+      </c>
+      <c r="B1106">
+        <v>10</v>
+      </c>
+      <c r="C1106">
+        <v>34.6</v>
+      </c>
+      <c r="D1106">
+        <v>31.1</v>
+      </c>
+      <c r="E1106">
+        <v>4</v>
+      </c>
+      <c r="F1106">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1107" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1107" t="s">
+        <v>147</v>
+      </c>
+      <c r="B1107">
+        <v>10</v>
+      </c>
+      <c r="C1107">
+        <v>27.4</v>
+      </c>
+      <c r="D1107">
+        <v>22.5</v>
+      </c>
+      <c r="E1107">
+        <v>4</v>
+      </c>
+      <c r="F1107">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1108" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1108" t="s">
+        <v>148</v>
+      </c>
+      <c r="B1108">
+        <v>10</v>
+      </c>
+      <c r="C1108">
+        <v>19.399999999999999</v>
+      </c>
+      <c r="D1108">
+        <v>21.4</v>
+      </c>
+      <c r="E1108">
+        <v>4</v>
+      </c>
+      <c r="F1108">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1109" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1109" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1109">
+        <v>10</v>
+      </c>
+      <c r="C1109">
+        <v>41</v>
+      </c>
+      <c r="D1109">
+        <v>11.5</v>
+      </c>
+      <c r="E1109">
+        <v>8</v>
+      </c>
+      <c r="F1109">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1110" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1110" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1110">
+        <v>10</v>
+      </c>
+      <c r="C1110">
+        <v>24.5</v>
+      </c>
+      <c r="D1110">
+        <v>27.4</v>
+      </c>
+      <c r="E1110">
+        <v>3</v>
+      </c>
+      <c r="F1110">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1111" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1111" t="s">
+        <v>149</v>
+      </c>
+      <c r="B1111">
+        <v>10</v>
+      </c>
+      <c r="C1111">
+        <v>27.5</v>
+      </c>
+      <c r="D1111">
+        <v>29.3</v>
+      </c>
+      <c r="E1111">
+        <v>4</v>
+      </c>
+      <c r="F1111">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1112" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1112" t="s">
+        <v>150</v>
+      </c>
+      <c r="B1112">
+        <v>10</v>
+      </c>
+      <c r="C1112">
+        <v>31.9</v>
+      </c>
+      <c r="D1112">
+        <v>14.4</v>
+      </c>
+      <c r="E1112">
+        <v>5</v>
+      </c>
+      <c r="F1112">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1113" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1113" t="s">
+        <v>151</v>
+      </c>
+      <c r="B1113">
+        <v>10</v>
+      </c>
+      <c r="C1113">
+        <v>37.4</v>
+      </c>
+      <c r="D1113">
+        <v>21.6</v>
+      </c>
+      <c r="E1113">
+        <v>8</v>
+      </c>
+      <c r="F1113">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1114" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1114" t="s">
+        <v>113</v>
+      </c>
+      <c r="B1114">
+        <v>10</v>
+      </c>
+      <c r="C1114">
+        <v>31.8</v>
+      </c>
+      <c r="D1114">
+        <v>22.9</v>
+      </c>
+      <c r="E1114">
+        <v>5</v>
+      </c>
+      <c r="F1114">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1115" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1115" t="s">
+        <v>94</v>
+      </c>
+      <c r="B1115">
+        <v>10</v>
+      </c>
+      <c r="C1115">
+        <v>23.9</v>
+      </c>
+      <c r="D1115">
+        <v>21.5</v>
+      </c>
+      <c r="E1115">
+        <v>4</v>
+      </c>
+      <c r="F1115">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1116" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1116" t="s">
+        <v>152</v>
+      </c>
+      <c r="B1116">
+        <v>10</v>
+      </c>
+      <c r="C1116">
+        <v>23.4</v>
+      </c>
+      <c r="D1116">
+        <v>25.4</v>
+      </c>
+      <c r="E1116">
+        <v>3</v>
+      </c>
+      <c r="F1116">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1117" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1117" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1117">
+        <v>10</v>
+      </c>
+      <c r="C1117">
+        <v>27.1</v>
+      </c>
+      <c r="D1117">
+        <v>30.6</v>
+      </c>
+      <c r="E1117">
+        <v>3</v>
+      </c>
+      <c r="F1117">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1118" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1118" t="s">
+        <v>44</v>
+      </c>
+      <c r="B1118">
+        <v>10</v>
+      </c>
+      <c r="C1118">
+        <v>20.8</v>
+      </c>
+      <c r="D1118">
+        <v>29.1</v>
+      </c>
+      <c r="E1118">
+        <v>2</v>
+      </c>
+      <c r="F1118">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1119" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1119" t="s">
+        <v>153</v>
+      </c>
+      <c r="B1119">
+        <v>10</v>
+      </c>
+      <c r="C1119">
+        <v>16.8</v>
+      </c>
+      <c r="D1119">
+        <v>24.9</v>
+      </c>
+      <c r="E1119">
+        <v>2</v>
+      </c>
+      <c r="F1119">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1120" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1120" t="s">
+        <v>83</v>
+      </c>
+      <c r="B1120">
+        <v>10</v>
+      </c>
+      <c r="C1120">
+        <v>16</v>
+      </c>
+      <c r="D1120">
+        <v>27</v>
+      </c>
+      <c r="E1120">
+        <v>3</v>
+      </c>
+      <c r="F1120">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1121" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1121" t="s">
+        <v>154</v>
+      </c>
+      <c r="B1121">
+        <v>10</v>
+      </c>
+      <c r="C1121">
+        <v>41.8</v>
+      </c>
+      <c r="D1121">
+        <v>31.4</v>
+      </c>
+      <c r="E1121">
+        <v>7</v>
+      </c>
+      <c r="F1121">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1122" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1122" t="s">
+        <v>84</v>
+      </c>
+      <c r="B1122">
+        <v>10</v>
+      </c>
+      <c r="C1122">
+        <v>26.8</v>
+      </c>
+      <c r="D1122">
+        <v>17.399999999999999</v>
+      </c>
+      <c r="E1122">
+        <v>6</v>
+      </c>
+      <c r="F1122">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1123" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1123" t="s">
+        <v>155</v>
+      </c>
+      <c r="B1123">
+        <v>10</v>
+      </c>
+      <c r="C1123">
+        <v>35.6</v>
+      </c>
+      <c r="D1123">
+        <v>32.1</v>
+      </c>
+      <c r="E1123">
+        <v>5</v>
+      </c>
+      <c r="F1123">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1124" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1124" t="s">
+        <v>156</v>
+      </c>
+      <c r="B1124">
+        <v>10</v>
+      </c>
+      <c r="C1124">
+        <v>30.8</v>
+      </c>
+      <c r="D1124">
+        <v>33</v>
+      </c>
+      <c r="E1124">
+        <v>2</v>
+      </c>
+      <c r="F1124">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1125" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1125" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1125">
+        <v>10</v>
+      </c>
+      <c r="C1125">
+        <v>17.899999999999999</v>
+      </c>
+      <c r="D1125">
+        <v>28.8</v>
+      </c>
+      <c r="E1125">
+        <v>1</v>
+      </c>
+      <c r="F1125">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1126" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1126" t="s">
+        <v>46</v>
+      </c>
+      <c r="B1126">
+        <v>10</v>
+      </c>
+      <c r="C1126">
+        <v>28.4</v>
+      </c>
+      <c r="D1126">
+        <v>22.1</v>
+      </c>
+      <c r="E1126">
+        <v>5</v>
+      </c>
+      <c r="F1126">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1127" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1127" t="s">
+        <v>157</v>
+      </c>
+      <c r="B1127">
+        <v>10</v>
+      </c>
+      <c r="C1127">
+        <v>32</v>
+      </c>
+      <c r="D1127">
+        <v>34.4</v>
+      </c>
+      <c r="E1127">
+        <v>5</v>
+      </c>
+      <c r="F1127">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1128" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1128" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1128">
+        <v>10</v>
+      </c>
+      <c r="C1128">
+        <v>48.9</v>
+      </c>
+      <c r="D1128">
+        <v>16.899999999999999</v>
+      </c>
+      <c r="E1128">
+        <v>8</v>
+      </c>
+      <c r="F1128">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1129" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1129" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1129">
+        <v>10</v>
+      </c>
+      <c r="C1129">
+        <v>33</v>
+      </c>
+      <c r="D1129">
+        <v>28.8</v>
+      </c>
+      <c r="E1129">
+        <v>5</v>
+      </c>
+      <c r="F1129">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1130" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1130" t="s">
+        <v>56</v>
+      </c>
+      <c r="B1130">
+        <v>10</v>
+      </c>
+      <c r="C1130">
+        <v>39.1</v>
+      </c>
+      <c r="D1130">
+        <v>31.1</v>
+      </c>
+      <c r="E1130">
+        <v>6</v>
+      </c>
+      <c r="F1130">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1131" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1131" t="s">
+        <v>158</v>
+      </c>
+      <c r="B1131">
+        <v>10</v>
+      </c>
+      <c r="C1131">
+        <v>24.6</v>
+      </c>
+      <c r="D1131">
+        <v>27</v>
+      </c>
+      <c r="E1131">
+        <v>3</v>
+      </c>
+      <c r="F1131">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1132" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1132" t="s">
+        <v>49</v>
+      </c>
+      <c r="B1132">
+        <v>10</v>
+      </c>
+      <c r="C1132">
+        <v>42.4</v>
+      </c>
+      <c r="D1132">
+        <v>28.4</v>
+      </c>
+      <c r="E1132">
+        <v>7</v>
+      </c>
+      <c r="F1132">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1133" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1133" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1133">
+        <v>10</v>
+      </c>
+      <c r="C1133">
+        <v>32.6</v>
+      </c>
+      <c r="D1133">
+        <v>22.8</v>
+      </c>
+      <c r="E1133">
+        <v>6</v>
+      </c>
+      <c r="F1133">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1134" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1134" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1134">
+        <v>10</v>
+      </c>
+      <c r="C1134">
+        <v>33.1</v>
+      </c>
+      <c r="D1134">
+        <v>22</v>
+      </c>
+      <c r="E1134">
+        <v>6</v>
+      </c>
+      <c r="F1134">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1135" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1135" t="s">
+        <v>51</v>
+      </c>
+      <c r="B1135">
+        <v>10</v>
+      </c>
+      <c r="C1135">
+        <v>30.5</v>
+      </c>
+      <c r="D1135">
+        <v>27.9</v>
+      </c>
+      <c r="E1135">
+        <v>4</v>
+      </c>
+      <c r="F1135">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1136" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1136" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1136">
+        <v>10</v>
+      </c>
+      <c r="C1136">
+        <v>32.799999999999997</v>
+      </c>
+      <c r="D1136">
+        <v>25.5</v>
+      </c>
+      <c r="E1136">
+        <v>5</v>
+      </c>
+      <c r="F1136">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1137" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1137" t="s">
+        <v>159</v>
+      </c>
+      <c r="B1137">
+        <v>10</v>
+      </c>
+      <c r="C1137">
+        <v>29.1</v>
+      </c>
+      <c r="D1137">
+        <v>33.6</v>
+      </c>
+      <c r="E1137">
+        <v>4</v>
+      </c>
+      <c r="F1137">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1138" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1138" t="s">
+        <v>160</v>
+      </c>
+      <c r="B1138">
+        <v>10</v>
+      </c>
+      <c r="C1138">
+        <v>20.100000000000001</v>
+      </c>
+      <c r="D1138">
+        <v>22.5</v>
+      </c>
+      <c r="E1138">
+        <v>4</v>
+      </c>
+      <c r="F1138">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1139" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1139" t="s">
+        <v>161</v>
+      </c>
+      <c r="B1139">
+        <v>10</v>
+      </c>
+      <c r="C1139">
+        <v>20.3</v>
+      </c>
+      <c r="D1139">
+        <v>22.8</v>
+      </c>
+      <c r="E1139">
+        <v>4</v>
+      </c>
+      <c r="F1139">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1140" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1140" t="s">
+        <v>162</v>
+      </c>
+      <c r="B1140">
+        <v>10</v>
+      </c>
+      <c r="C1140">
+        <v>27</v>
+      </c>
+      <c r="D1140">
+        <v>16.399999999999999</v>
+      </c>
+      <c r="E1140">
+        <v>5</v>
+      </c>
+      <c r="F1140">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1141" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1141" t="s">
+        <v>163</v>
+      </c>
+      <c r="B1141">
+        <v>10</v>
+      </c>
+      <c r="C1141">
+        <v>35.6</v>
+      </c>
+      <c r="D1141">
+        <v>30</v>
+      </c>
+      <c r="E1141">
+        <v>4</v>
+      </c>
+      <c r="F1141">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1142" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1142" t="s">
+        <v>164</v>
+      </c>
+      <c r="B1142">
+        <v>10</v>
+      </c>
+      <c r="C1142">
+        <v>31.6</v>
+      </c>
+      <c r="D1142">
+        <v>17.600000000000001</v>
+      </c>
+      <c r="E1142">
+        <v>6</v>
+      </c>
+      <c r="F1142">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1143" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1143" t="s">
+        <v>92</v>
+      </c>
+      <c r="B1143">
+        <v>10</v>
+      </c>
+      <c r="C1143">
+        <v>30.3</v>
+      </c>
+      <c r="D1143">
+        <v>24.6</v>
+      </c>
+      <c r="E1143">
+        <v>5</v>
+      </c>
+      <c r="F1143">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1144" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1144" t="s">
+        <v>165</v>
+      </c>
+      <c r="B1144">
+        <v>10</v>
+      </c>
+      <c r="C1144">
+        <v>25.5</v>
+      </c>
+      <c r="D1144">
+        <v>38.1</v>
+      </c>
+      <c r="E1144">
+        <v>1</v>
+      </c>
+      <c r="F1144">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1145" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1145" t="s">
+        <v>166</v>
+      </c>
+      <c r="B1145">
+        <v>10</v>
+      </c>
+      <c r="C1145">
+        <v>26.8</v>
+      </c>
+      <c r="D1145">
+        <v>22.1</v>
+      </c>
+      <c r="E1145">
+        <v>5</v>
+      </c>
+      <c r="F1145">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1146" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1146" t="s">
+        <v>109</v>
+      </c>
+      <c r="B1146">
+        <v>10</v>
+      </c>
+      <c r="C1146">
+        <v>23.6</v>
+      </c>
+      <c r="D1146">
+        <v>28.8</v>
+      </c>
+      <c r="E1146">
+        <v>3</v>
+      </c>
+      <c r="F1146">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1147" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1147" t="s">
+        <v>167</v>
+      </c>
+      <c r="B1147">
+        <v>10</v>
+      </c>
+      <c r="C1147">
+        <v>32.6</v>
+      </c>
+      <c r="D1147">
+        <v>18.399999999999999</v>
+      </c>
+      <c r="E1147">
+        <v>6</v>
+      </c>
+      <c r="F1147">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1148" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1148" t="s">
+        <v>168</v>
+      </c>
+      <c r="B1148">
+        <v>10</v>
+      </c>
+      <c r="C1148">
+        <v>44.3</v>
+      </c>
+      <c r="D1148">
+        <v>27.3</v>
+      </c>
+      <c r="E1148">
+        <v>8</v>
+      </c>
+      <c r="F1148">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1149" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1149" t="s">
+        <v>169</v>
+      </c>
+      <c r="B1149">
+        <v>10</v>
+      </c>
+      <c r="C1149">
+        <v>15.5</v>
+      </c>
+      <c r="D1149">
+        <v>26</v>
+      </c>
+      <c r="E1149">
+        <v>2</v>
+      </c>
+      <c r="F1149">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1150" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1150" t="s">
+        <v>104</v>
+      </c>
+      <c r="B1150">
+        <v>10</v>
+      </c>
+      <c r="C1150">
+        <v>49.4</v>
+      </c>
+      <c r="D1150">
+        <v>21</v>
+      </c>
+      <c r="E1150">
+        <v>8</v>
+      </c>
+      <c r="F1150">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1151" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1151" t="s">
+        <v>90</v>
+      </c>
+      <c r="B1151">
+        <v>10</v>
+      </c>
+      <c r="C1151">
+        <v>36.4</v>
+      </c>
+      <c r="D1151">
+        <v>21.1</v>
+      </c>
+      <c r="E1151">
+        <v>5</v>
+      </c>
+      <c r="F1151">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1152" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1152" t="s">
+        <v>101</v>
+      </c>
+      <c r="B1152">
+        <v>10</v>
+      </c>
+      <c r="C1152">
+        <v>22.6</v>
+      </c>
+      <c r="D1152">
+        <v>21.8</v>
+      </c>
+      <c r="E1152">
+        <v>3</v>
+      </c>
+      <c r="F1152">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1153" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1153" t="s">
+        <v>170</v>
+      </c>
+      <c r="B1153">
+        <v>10</v>
+      </c>
+      <c r="C1153">
+        <v>21.6</v>
+      </c>
+      <c r="D1153">
+        <v>24.1</v>
+      </c>
+      <c r="E1153">
+        <v>3</v>
+      </c>
+      <c r="F1153">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1154" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1154" t="s">
+        <v>95</v>
+      </c>
+      <c r="B1154">
+        <v>10</v>
+      </c>
+      <c r="C1154">
+        <v>33.9</v>
+      </c>
+      <c r="D1154">
+        <v>29.3</v>
+      </c>
+      <c r="E1154">
+        <v>4</v>
+      </c>
+      <c r="F1154">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1155" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1155" t="s">
+        <v>171</v>
+      </c>
+      <c r="B1155">
+        <v>10</v>
+      </c>
+      <c r="C1155">
+        <v>35.9</v>
+      </c>
+      <c r="D1155">
+        <v>26.9</v>
+      </c>
+      <c r="E1155">
+        <v>6</v>
+      </c>
+      <c r="F1155">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1156" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1156" t="s">
+        <v>172</v>
+      </c>
+      <c r="B1156">
+        <v>10</v>
+      </c>
+      <c r="C1156">
+        <v>22.5</v>
+      </c>
+      <c r="D1156">
+        <v>17.600000000000001</v>
+      </c>
+      <c r="E1156">
+        <v>6</v>
+      </c>
+      <c r="F1156">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1157" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1157" t="s">
+        <v>173</v>
+      </c>
+      <c r="B1157">
+        <v>10</v>
+      </c>
+      <c r="C1157">
+        <v>33.6</v>
+      </c>
+      <c r="D1157">
+        <v>17.399999999999999</v>
+      </c>
+      <c r="E1157">
+        <v>7</v>
+      </c>
+      <c r="F1157">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1158" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1158" t="s">
+        <v>55</v>
+      </c>
+      <c r="B1158">
+        <v>10</v>
+      </c>
+      <c r="C1158">
+        <v>32.4</v>
+      </c>
+      <c r="D1158">
+        <v>34</v>
+      </c>
+      <c r="E1158">
+        <v>3</v>
+      </c>
+      <c r="F1158">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1159" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1159" t="s">
+        <v>174</v>
+      </c>
+      <c r="B1159">
+        <v>10</v>
+      </c>
+      <c r="C1159">
+        <v>30.1</v>
+      </c>
+      <c r="D1159">
+        <v>18.5</v>
+      </c>
+      <c r="E1159">
+        <v>4</v>
+      </c>
+      <c r="F1159">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1160" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1160" t="s">
+        <v>88</v>
+      </c>
+      <c r="B1160">
+        <v>10</v>
+      </c>
+      <c r="C1160">
+        <v>35.799999999999997</v>
+      </c>
+      <c r="D1160">
+        <v>17.600000000000001</v>
+      </c>
+      <c r="E1160">
+        <v>6</v>
+      </c>
+      <c r="F1160">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1161" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1161" t="s">
+        <v>175</v>
+      </c>
+      <c r="B1161">
+        <v>10</v>
+      </c>
+      <c r="C1161">
+        <v>39.6</v>
+      </c>
+      <c r="D1161">
+        <v>24.3</v>
+      </c>
+      <c r="E1161">
+        <v>7</v>
+      </c>
+      <c r="F1161">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1162" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1162" t="s">
+        <v>176</v>
+      </c>
+      <c r="B1162">
+        <v>10</v>
+      </c>
+      <c r="C1162">
+        <v>28</v>
+      </c>
+      <c r="D1162">
+        <v>29.8</v>
+      </c>
+      <c r="E1162">
+        <v>4</v>
+      </c>
+      <c r="F1162">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1163" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1163" t="s">
+        <v>110</v>
+      </c>
+      <c r="B1163">
+        <v>10</v>
+      </c>
+      <c r="C1163">
+        <v>41</v>
+      </c>
+      <c r="D1163">
+        <v>24</v>
+      </c>
+      <c r="E1163">
+        <v>7</v>
+      </c>
+      <c r="F1163">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1164" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1164" t="s">
+        <v>53</v>
+      </c>
+      <c r="B1164">
+        <v>10</v>
+      </c>
+      <c r="C1164">
+        <v>38.299999999999997</v>
+      </c>
+      <c r="D1164">
+        <v>21.6</v>
+      </c>
+      <c r="E1164">
+        <v>6</v>
+      </c>
+      <c r="F1164">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1165" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1165" t="s">
+        <v>58</v>
+      </c>
+      <c r="B1165">
+        <v>10</v>
+      </c>
+      <c r="C1165">
+        <v>19.100000000000001</v>
+      </c>
+      <c r="D1165">
+        <v>31.3</v>
+      </c>
+      <c r="E1165">
+        <v>3</v>
+      </c>
+      <c r="F1165">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1166" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1166" t="s">
+        <v>48</v>
+      </c>
+      <c r="B1166">
+        <v>10</v>
+      </c>
+      <c r="C1166">
+        <v>21.3</v>
+      </c>
+      <c r="D1166">
+        <v>27.4</v>
+      </c>
+      <c r="E1166">
+        <v>4</v>
+      </c>
+      <c r="F1166">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1167" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1167" t="s">
+        <v>45</v>
+      </c>
+      <c r="B1167">
+        <v>10</v>
+      </c>
+      <c r="C1167">
+        <v>35.6</v>
+      </c>
+      <c r="D1167">
+        <v>29.4</v>
+      </c>
+      <c r="E1167">
+        <v>6</v>
+      </c>
+      <c r="F1167">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1168" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1168" t="s">
+        <v>177</v>
+      </c>
+      <c r="B1168">
+        <v>10</v>
+      </c>
+      <c r="C1168">
+        <v>26.6</v>
+      </c>
+      <c r="D1168">
+        <v>36.6</v>
+      </c>
+      <c r="E1168">
+        <v>3</v>
+      </c>
+      <c r="F1168">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1169" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1169" t="s">
+        <v>178</v>
+      </c>
+      <c r="B1169">
+        <v>10</v>
+      </c>
+      <c r="C1169">
+        <v>16.899999999999999</v>
+      </c>
+      <c r="D1169">
+        <v>21.5</v>
+      </c>
+      <c r="E1169">
+        <v>3</v>
+      </c>
+      <c r="F1169">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1170" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1170" t="s">
+        <v>179</v>
+      </c>
+      <c r="B1170">
+        <v>10</v>
+      </c>
+      <c r="C1170">
+        <v>19.399999999999999</v>
+      </c>
+      <c r="D1170">
+        <v>24.8</v>
+      </c>
+      <c r="E1170">
+        <v>2</v>
+      </c>
+      <c r="F1170">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1171" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1171" t="s">
+        <v>180</v>
+      </c>
+      <c r="B1171">
+        <v>10</v>
+      </c>
+      <c r="C1171">
+        <v>38.9</v>
+      </c>
+      <c r="D1171">
+        <v>27</v>
+      </c>
+      <c r="E1171">
+        <v>6</v>
+      </c>
+      <c r="F1171">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1172" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1172" t="s">
+        <v>181</v>
+      </c>
+      <c r="B1172">
+        <v>10</v>
+      </c>
+      <c r="C1172">
+        <v>40.4</v>
+      </c>
+      <c r="D1172">
+        <v>27.6</v>
+      </c>
+      <c r="E1172">
+        <v>6</v>
+      </c>
+      <c r="F1172">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1173" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1173" t="s">
+        <v>105</v>
+      </c>
+      <c r="B1173">
+        <v>10</v>
+      </c>
+      <c r="C1173">
+        <v>23.6</v>
+      </c>
+      <c r="D1173">
+        <v>20.8</v>
+      </c>
+      <c r="E1173">
+        <v>4</v>
+      </c>
+      <c r="F1173">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1174" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1174" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1174">
+        <v>10</v>
+      </c>
+      <c r="C1174">
+        <v>34.4</v>
+      </c>
+      <c r="D1174">
+        <v>34.6</v>
+      </c>
+      <c r="E1174">
+        <v>3</v>
+      </c>
+      <c r="F1174">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1175" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1175" t="s">
+        <v>182</v>
+      </c>
+      <c r="B1175">
+        <v>10</v>
+      </c>
+      <c r="C1175">
+        <v>34.799999999999997</v>
+      </c>
+      <c r="D1175">
+        <v>24</v>
+      </c>
+      <c r="E1175">
+        <v>5</v>
+      </c>
+      <c r="F1175">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1176" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1176" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1176">
+        <v>10</v>
+      </c>
+      <c r="C1176">
+        <v>20.8</v>
+      </c>
+      <c r="D1176">
+        <v>28.5</v>
+      </c>
+      <c r="E1176">
+        <v>3</v>
+      </c>
+      <c r="F1176">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1177" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1177" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1177">
+        <v>10</v>
+      </c>
+      <c r="C1177">
+        <v>31.8</v>
+      </c>
+      <c r="D1177">
+        <v>21.9</v>
+      </c>
+      <c r="E1177">
+        <v>4</v>
+      </c>
+      <c r="F1177">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1178" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1178" t="s">
+        <v>62</v>
+      </c>
+      <c r="B1178">
+        <v>10</v>
+      </c>
+      <c r="C1178">
+        <v>24.2</v>
+      </c>
+      <c r="D1178">
+        <v>24.2</v>
+      </c>
+      <c r="E1178">
+        <v>6</v>
+      </c>
+      <c r="F1178">
         <v>3</v>
       </c>
     </row>
@@ -37805,10 +42064,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01ABCD41-9594-F549-BC55-37725303300E}">
-  <dimension ref="A1:C201"/>
+  <dimension ref="A1:C226"/>
   <sheetViews>
-    <sheetView topLeftCell="A185" workbookViewId="0">
-      <selection activeCell="A177" sqref="A177:B201"/>
+    <sheetView tabSelected="1" topLeftCell="A219" workbookViewId="0">
+      <selection activeCell="A202" sqref="A202:B226"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -40022,6 +44281,281 @@
       </c>
       <c r="C201" t="s">
         <v>92</v>
+      </c>
+    </row>
+    <row r="202" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A202">
+        <v>10</v>
+      </c>
+      <c r="B202">
+        <v>1</v>
+      </c>
+      <c r="C202" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="203" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A203">
+        <v>10</v>
+      </c>
+      <c r="B203">
+        <v>2</v>
+      </c>
+      <c r="C203" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="204" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A204">
+        <v>10</v>
+      </c>
+      <c r="B204">
+        <v>3</v>
+      </c>
+      <c r="C204" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="205" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A205">
+        <v>10</v>
+      </c>
+      <c r="B205">
+        <v>4</v>
+      </c>
+      <c r="C205" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="206" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A206">
+        <v>10</v>
+      </c>
+      <c r="B206">
+        <v>5</v>
+      </c>
+      <c r="C206" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="207" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A207">
+        <v>10</v>
+      </c>
+      <c r="B207">
+        <v>6</v>
+      </c>
+      <c r="C207" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="208" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A208">
+        <v>10</v>
+      </c>
+      <c r="B208">
+        <v>7</v>
+      </c>
+      <c r="C208" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="209" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A209">
+        <v>10</v>
+      </c>
+      <c r="B209">
+        <v>8</v>
+      </c>
+      <c r="C209" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="210" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A210">
+        <v>10</v>
+      </c>
+      <c r="B210">
+        <v>9</v>
+      </c>
+      <c r="C210" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="211" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A211">
+        <v>10</v>
+      </c>
+      <c r="B211">
+        <v>10</v>
+      </c>
+      <c r="C211" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="212" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A212">
+        <v>10</v>
+      </c>
+      <c r="B212">
+        <v>11</v>
+      </c>
+      <c r="C212" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="213" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A213">
+        <v>10</v>
+      </c>
+      <c r="B213">
+        <v>12</v>
+      </c>
+      <c r="C213" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="214" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A214">
+        <v>10</v>
+      </c>
+      <c r="B214">
+        <v>13</v>
+      </c>
+      <c r="C214" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="215" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A215">
+        <v>10</v>
+      </c>
+      <c r="B215">
+        <v>14</v>
+      </c>
+      <c r="C215" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="216" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A216">
+        <v>10</v>
+      </c>
+      <c r="B216">
+        <v>15</v>
+      </c>
+      <c r="C216" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="217" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A217">
+        <v>10</v>
+      </c>
+      <c r="B217">
+        <v>16</v>
+      </c>
+      <c r="C217" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="218" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A218">
+        <v>10</v>
+      </c>
+      <c r="B218">
+        <v>17</v>
+      </c>
+      <c r="C218" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="219" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A219">
+        <v>10</v>
+      </c>
+      <c r="B219">
+        <v>18</v>
+      </c>
+      <c r="C219" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="220" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A220">
+        <v>10</v>
+      </c>
+      <c r="B220">
+        <v>19</v>
+      </c>
+      <c r="C220" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="221" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A221">
+        <v>10</v>
+      </c>
+      <c r="B221">
+        <v>20</v>
+      </c>
+      <c r="C221" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="222" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A222">
+        <v>10</v>
+      </c>
+      <c r="B222">
+        <v>21</v>
+      </c>
+      <c r="C222" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="223" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A223">
+        <v>10</v>
+      </c>
+      <c r="B223">
+        <v>22</v>
+      </c>
+      <c r="C223" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="224" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A224">
+        <v>10</v>
+      </c>
+      <c r="B224">
+        <v>23</v>
+      </c>
+      <c r="C224" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="225" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A225">
+        <v>10</v>
+      </c>
+      <c r="B225">
+        <v>24</v>
+      </c>
+      <c r="C225" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="226" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A226">
+        <v>10</v>
+      </c>
+      <c r="B226">
+        <v>25</v>
+      </c>
+      <c r="C226" t="s">
+        <v>88</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Week 10 viewership / week 11 predictions
</commit_message>
<xml_diff>
--- a/ratings-2022.xlsx
+++ b/ratings-2022.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mike/PycharmProjects/tvratings-ssac2023/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EF89696-5EB2-FB49-9E95-7719B213587B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19D3EEEE-71F3-2C45-8D7C-F29D029C816B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1200" yWindow="14680" windowWidth="37240" windowHeight="10280" activeTab="2" xr2:uid="{BBDA95F9-3552-704A-ADE2-3350C5179C3F}"/>
+    <workbookView xWindow="1200" yWindow="14680" windowWidth="37240" windowHeight="10280" xr2:uid="{BBDA95F9-3552-704A-ADE2-3350C5179C3F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -991,9 +991,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78DF36B5-5368-0F4E-AE20-BC9ECC5E0688}">
   <dimension ref="A1:AA226"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="760" topLeftCell="A184" activePane="bottomLeft"/>
-      <selection pane="bottomLeft" activeCell="F201" sqref="F201"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="760" topLeftCell="A183" activePane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="F186" sqref="F186"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -17248,7 +17248,7 @@
         <v>106</v>
       </c>
       <c r="F185">
-        <v>0</v>
+        <v>1230000</v>
       </c>
       <c r="G185">
         <v>2022</v>
@@ -46714,7 +46714,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01ABCD41-9594-F549-BC55-37725303300E}">
   <dimension ref="A1:C251"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A240" workbookViewId="0">
+    <sheetView topLeftCell="A240" workbookViewId="0">
       <selection activeCell="A227" sqref="A227:B251"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Week 12 viewership / week 14 predictions
</commit_message>
<xml_diff>
--- a/ratings-2022.xlsx
+++ b/ratings-2022.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mike/PycharmProjects/tvratings-ssac2023/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C96950E9-36D7-814E-87C7-FBAE59A5C372}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{037FD951-D6FB-3549-A0DE-06C4EFC1BF97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1940" yWindow="14160" windowWidth="37240" windowHeight="10280" xr2:uid="{BBDA95F9-3552-704A-ADE2-3350C5179C3F}"/>
+    <workbookView xWindow="820" yWindow="14080" windowWidth="37240" windowHeight="10280" xr2:uid="{BBDA95F9-3552-704A-ADE2-3350C5179C3F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3303" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3504" uniqueCount="190">
   <si>
     <t>Time</t>
   </si>
@@ -632,6 +632,9 @@
   <si>
     <t>North Dakota State</t>
   </si>
+  <si>
+    <t>North Carolina State</t>
+  </si>
 </sst>
 </file>
 
@@ -988,12 +991,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78DF36B5-5368-0F4E-AE20-BC9ECC5E0688}">
-  <dimension ref="A1:AA278"/>
+  <dimension ref="A1:AA287"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="760" topLeftCell="A265" activePane="bottomLeft"/>
+      <pane ySplit="760" topLeftCell="A280" activePane="bottomLeft"/>
       <selection sqref="A1:AA1"/>
-      <selection pane="bottomLeft" activeCell="O278" sqref="O278"/>
+      <selection pane="bottomLeft" activeCell="F253" sqref="F253"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -22474,7 +22477,7 @@
         <v>113</v>
       </c>
       <c r="F252">
-        <v>0</v>
+        <v>2231000</v>
       </c>
       <c r="G252">
         <v>2022</v>
@@ -24561,6 +24564,708 @@
       <c r="AA278" cm="1">
         <f t="array" ref="AA278">_xlfn.XLOOKUP(E278&amp;I278,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!F$2:F$13000,"")</f>
         <v>5</v>
+      </c>
+    </row>
+    <row r="279" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A279" s="1">
+        <v>44897</v>
+      </c>
+      <c r="B279" s="2">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="C279" t="s">
+        <v>24</v>
+      </c>
+      <c r="D279" t="s">
+        <v>110</v>
+      </c>
+      <c r="E279" t="s">
+        <v>53</v>
+      </c>
+      <c r="F279">
+        <v>0</v>
+      </c>
+      <c r="G279">
+        <v>2022</v>
+      </c>
+      <c r="H279">
+        <v>0</v>
+      </c>
+      <c r="I279">
+        <v>14</v>
+      </c>
+      <c r="J279" cm="1">
+        <f t="array" ref="J279">_xlfn.XLOOKUP(D279&amp;I279,Ranking!C$2:C$500&amp;Ranking!A$2:A$500,Ranking!B$2:B$500,"")</f>
+        <v>4</v>
+      </c>
+      <c r="K279" cm="1">
+        <f t="array" ref="K279">_xlfn.XLOOKUP(E279&amp;I279,Ranking!C$2:C$500&amp;Ranking!A$2:A$500,Ranking!B$2:B$500,"")</f>
+        <v>11</v>
+      </c>
+      <c r="L279" t="s">
+        <v>65</v>
+      </c>
+      <c r="M279" t="s">
+        <v>65</v>
+      </c>
+      <c r="N279">
+        <v>1</v>
+      </c>
+      <c r="O279" cm="1">
+        <f t="array" ref="O279">_xlfn.XLOOKUP(D279&amp;I279,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!C$2:C$13000,"")</f>
+        <v>42.5</v>
+      </c>
+      <c r="P279" cm="1">
+        <f t="array" ref="P279">_xlfn.XLOOKUP(D279&amp;I279,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!D$2:D$13000,"")</f>
+        <v>26.3</v>
+      </c>
+      <c r="Q279" cm="1">
+        <f t="array" ref="Q279">_xlfn.XLOOKUP(E279&amp;I279,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!C$2:C$13000,"")</f>
+        <v>39.4</v>
+      </c>
+      <c r="R279" cm="1">
+        <f t="array" ref="R279">_xlfn.XLOOKUP(E279&amp;I279,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!D$2:D$13000,"")</f>
+        <v>20.100000000000001</v>
+      </c>
+      <c r="X279" cm="1">
+        <f t="array" ref="X279">_xlfn.XLOOKUP(D279&amp;I279,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!E$2:E$13000,"")</f>
+        <v>11</v>
+      </c>
+      <c r="Y279" cm="1">
+        <f t="array" ref="Y279">_xlfn.XLOOKUP(D279&amp;I279,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!F$2:F$13000,"")</f>
+        <v>1</v>
+      </c>
+      <c r="Z279" cm="1">
+        <f t="array" ref="Z279">_xlfn.XLOOKUP(E279&amp;I279,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!E$2:E$13000,"")</f>
+        <v>9</v>
+      </c>
+      <c r="AA279" cm="1">
+        <f t="array" ref="AA279">_xlfn.XLOOKUP(E279&amp;I279,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!F$2:F$13000,"")</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="280" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A280" s="1">
+        <v>44898</v>
+      </c>
+      <c r="B280" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="C280" t="s">
+        <v>33</v>
+      </c>
+      <c r="D280" t="s">
+        <v>168</v>
+      </c>
+      <c r="E280" t="s">
+        <v>93</v>
+      </c>
+      <c r="F280">
+        <v>0</v>
+      </c>
+      <c r="G280">
+        <v>2022</v>
+      </c>
+      <c r="H280">
+        <v>0</v>
+      </c>
+      <c r="I280">
+        <v>14</v>
+      </c>
+      <c r="J280" cm="1">
+        <f t="array" ref="J280">_xlfn.XLOOKUP(D280&amp;I280,Ranking!C$2:C$500&amp;Ranking!A$2:A$500,Ranking!B$2:B$500,"")</f>
+        <v>3</v>
+      </c>
+      <c r="K280" cm="1">
+        <f t="array" ref="K280">_xlfn.XLOOKUP(E280&amp;I280,Ranking!C$2:C$500&amp;Ranking!A$2:A$500,Ranking!B$2:B$500,"")</f>
+        <v>10</v>
+      </c>
+      <c r="L280" t="s">
+        <v>71</v>
+      </c>
+      <c r="M280" t="s">
+        <v>71</v>
+      </c>
+      <c r="N280">
+        <v>1</v>
+      </c>
+      <c r="O280" cm="1">
+        <f t="array" ref="O280">_xlfn.XLOOKUP(D280&amp;I280,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!C$2:C$13000,"")</f>
+        <v>41.3</v>
+      </c>
+      <c r="P280" cm="1">
+        <f t="array" ref="P280">_xlfn.XLOOKUP(D280&amp;I280,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!D$2:D$13000,"")</f>
+        <v>24.5</v>
+      </c>
+      <c r="Q280" cm="1">
+        <f t="array" ref="Q280">_xlfn.XLOOKUP(E280&amp;I280,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!C$2:C$13000,"")</f>
+        <v>33.4</v>
+      </c>
+      <c r="R280" cm="1">
+        <f t="array" ref="R280">_xlfn.XLOOKUP(E280&amp;I280,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!D$2:D$13000,"")</f>
+        <v>19.399999999999999</v>
+      </c>
+      <c r="X280" cm="1">
+        <f t="array" ref="X280">_xlfn.XLOOKUP(D280&amp;I280,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!E$2:E$13000,"")</f>
+        <v>12</v>
+      </c>
+      <c r="Y280" cm="1">
+        <f t="array" ref="Y280">_xlfn.XLOOKUP(D280&amp;I280,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!F$2:F$13000,"")</f>
+        <v>0</v>
+      </c>
+      <c r="Z280" cm="1">
+        <f t="array" ref="Z280">_xlfn.XLOOKUP(E280&amp;I280,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!E$2:E$13000,"")</f>
+        <v>9</v>
+      </c>
+      <c r="AA280" cm="1">
+        <f t="array" ref="AA280">_xlfn.XLOOKUP(E280&amp;I280,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!F$2:F$13000,"")</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="281" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A281" s="1">
+        <v>44898</v>
+      </c>
+      <c r="B281" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="C281" t="s">
+        <v>25</v>
+      </c>
+      <c r="D281" t="s">
+        <v>157</v>
+      </c>
+      <c r="E281" t="s">
+        <v>171</v>
+      </c>
+      <c r="F281">
+        <v>0</v>
+      </c>
+      <c r="G281">
+        <v>2022</v>
+      </c>
+      <c r="H281">
+        <v>0</v>
+      </c>
+      <c r="I281">
+        <v>14</v>
+      </c>
+      <c r="J281" t="str" cm="1">
+        <f t="array" ref="J281">_xlfn.XLOOKUP(D281&amp;I281,Ranking!C$2:C$500&amp;Ranking!A$2:A$500,Ranking!B$2:B$500,"")</f>
+        <v/>
+      </c>
+      <c r="K281" t="str" cm="1">
+        <f t="array" ref="K281">_xlfn.XLOOKUP(E281&amp;I281,Ranking!C$2:C$500&amp;Ranking!A$2:A$500,Ranking!B$2:B$500,"")</f>
+        <v/>
+      </c>
+      <c r="L281" t="s">
+        <v>72</v>
+      </c>
+      <c r="M281" t="s">
+        <v>72</v>
+      </c>
+      <c r="N281">
+        <v>1</v>
+      </c>
+      <c r="O281" cm="1">
+        <f t="array" ref="O281">_xlfn.XLOOKUP(D281&amp;I281,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!C$2:C$13000,"")</f>
+        <v>34</v>
+      </c>
+      <c r="P281" cm="1">
+        <f t="array" ref="P281">_xlfn.XLOOKUP(D281&amp;I281,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!D$2:D$13000,"")</f>
+        <v>29.3</v>
+      </c>
+      <c r="Q281" cm="1">
+        <f t="array" ref="Q281">_xlfn.XLOOKUP(E281&amp;I281,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!C$2:C$13000,"")</f>
+        <v>33.299999999999997</v>
+      </c>
+      <c r="R281" cm="1">
+        <f t="array" ref="R281">_xlfn.XLOOKUP(E281&amp;I281,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!D$2:D$13000,"")</f>
+        <v>27.1</v>
+      </c>
+      <c r="X281" cm="1">
+        <f t="array" ref="X281">_xlfn.XLOOKUP(D281&amp;I281,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!E$2:E$13000,"")</f>
+        <v>9</v>
+      </c>
+      <c r="Y281" cm="1">
+        <f t="array" ref="Y281">_xlfn.XLOOKUP(D281&amp;I281,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!F$2:F$13000,"")</f>
+        <v>3</v>
+      </c>
+      <c r="Z281" cm="1">
+        <f t="array" ref="Z281">_xlfn.XLOOKUP(E281&amp;I281,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!E$2:E$13000,"")</f>
+        <v>7</v>
+      </c>
+      <c r="AA281" cm="1">
+        <f t="array" ref="AA281">_xlfn.XLOOKUP(E281&amp;I281,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!F$2:F$13000,"")</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="282" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A282" s="1">
+        <v>44898</v>
+      </c>
+      <c r="B282" s="2">
+        <v>0.64583333333333337</v>
+      </c>
+      <c r="C282" t="s">
+        <v>25</v>
+      </c>
+      <c r="D282" t="s">
+        <v>172</v>
+      </c>
+      <c r="E282" t="s">
+        <v>128</v>
+      </c>
+      <c r="F282">
+        <v>0</v>
+      </c>
+      <c r="G282">
+        <v>2022</v>
+      </c>
+      <c r="H282">
+        <v>0</v>
+      </c>
+      <c r="I282">
+        <v>14</v>
+      </c>
+      <c r="J282" t="str" cm="1">
+        <f t="array" ref="J282">_xlfn.XLOOKUP(D282&amp;I282,Ranking!C$2:C$500&amp;Ranking!A$2:A$500,Ranking!B$2:B$500,"")</f>
+        <v/>
+      </c>
+      <c r="K282" t="str" cm="1">
+        <f t="array" ref="K282">_xlfn.XLOOKUP(E282&amp;I282,Ranking!C$2:C$500&amp;Ranking!A$2:A$500,Ranking!B$2:B$500,"")</f>
+        <v/>
+      </c>
+      <c r="L282" t="s">
+        <v>103</v>
+      </c>
+      <c r="M282" t="s">
+        <v>103</v>
+      </c>
+      <c r="N282">
+        <v>1</v>
+      </c>
+      <c r="O282" cm="1">
+        <f t="array" ref="O282">_xlfn.XLOOKUP(D282&amp;I282,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!C$2:C$13000,"")</f>
+        <v>24.6</v>
+      </c>
+      <c r="P282" cm="1">
+        <f t="array" ref="P282">_xlfn.XLOOKUP(D282&amp;I282,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!D$2:D$13000,"")</f>
+        <v>16.8</v>
+      </c>
+      <c r="Q282" cm="1">
+        <f t="array" ref="Q282">_xlfn.XLOOKUP(E282&amp;I282,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!C$2:C$13000,"")</f>
+        <v>29.4</v>
+      </c>
+      <c r="R282" cm="1">
+        <f t="array" ref="R282">_xlfn.XLOOKUP(E282&amp;I282,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!D$2:D$13000,"")</f>
+        <v>28.7</v>
+      </c>
+      <c r="X282" cm="1">
+        <f t="array" ref="X282">_xlfn.XLOOKUP(D282&amp;I282,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!E$2:E$13000,"")</f>
+        <v>10</v>
+      </c>
+      <c r="Y282" cm="1">
+        <f t="array" ref="Y282">_xlfn.XLOOKUP(D282&amp;I282,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!F$2:F$13000,"")</f>
+        <v>2</v>
+      </c>
+      <c r="Z282" cm="1">
+        <f t="array" ref="Z282">_xlfn.XLOOKUP(E282&amp;I282,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!E$2:E$13000,"")</f>
+        <v>9</v>
+      </c>
+      <c r="AA282" cm="1">
+        <f t="array" ref="AA282">_xlfn.XLOOKUP(E282&amp;I282,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!F$2:F$13000,"")</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="283" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A283" s="1">
+        <v>44898</v>
+      </c>
+      <c r="B283" s="2">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="C283" t="s">
+        <v>54</v>
+      </c>
+      <c r="D283" t="s">
+        <v>32</v>
+      </c>
+      <c r="E283" t="s">
+        <v>114</v>
+      </c>
+      <c r="F283">
+        <v>0</v>
+      </c>
+      <c r="G283">
+        <v>2022</v>
+      </c>
+      <c r="H283">
+        <v>0</v>
+      </c>
+      <c r="I283">
+        <v>14</v>
+      </c>
+      <c r="J283" cm="1">
+        <f t="array" ref="J283">_xlfn.XLOOKUP(D283&amp;I283,Ranking!C$2:C$500&amp;Ranking!A$2:A$500,Ranking!B$2:B$500,"")</f>
+        <v>1</v>
+      </c>
+      <c r="K283" cm="1">
+        <f t="array" ref="K283">_xlfn.XLOOKUP(E283&amp;I283,Ranking!C$2:C$500&amp;Ranking!A$2:A$500,Ranking!B$2:B$500,"")</f>
+        <v>14</v>
+      </c>
+      <c r="L283" t="s">
+        <v>70</v>
+      </c>
+      <c r="M283" t="s">
+        <v>70</v>
+      </c>
+      <c r="N283">
+        <v>1</v>
+      </c>
+      <c r="O283" cm="1">
+        <f t="array" ref="O283">_xlfn.XLOOKUP(D283&amp;I283,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!C$2:C$13000,"")</f>
+        <v>38.299999999999997</v>
+      </c>
+      <c r="P283" cm="1">
+        <f t="array" ref="P283">_xlfn.XLOOKUP(D283&amp;I283,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!D$2:D$13000,"")</f>
+        <v>11.3</v>
+      </c>
+      <c r="Q283" cm="1">
+        <f t="array" ref="Q283">_xlfn.XLOOKUP(E283&amp;I283,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!C$2:C$13000,"")</f>
+        <v>32.5</v>
+      </c>
+      <c r="R283" cm="1">
+        <f t="array" ref="R283">_xlfn.XLOOKUP(E283&amp;I283,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!D$2:D$13000,"")</f>
+        <v>21.5</v>
+      </c>
+      <c r="X283" cm="1">
+        <f t="array" ref="X283">_xlfn.XLOOKUP(D283&amp;I283,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!E$2:E$13000,"")</f>
+        <v>12</v>
+      </c>
+      <c r="Y283" cm="1">
+        <f t="array" ref="Y283">_xlfn.XLOOKUP(D283&amp;I283,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!F$2:F$13000,"")</f>
+        <v>0</v>
+      </c>
+      <c r="Z283" cm="1">
+        <f t="array" ref="Z283">_xlfn.XLOOKUP(E283&amp;I283,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!E$2:E$13000,"")</f>
+        <v>9</v>
+      </c>
+      <c r="AA283" cm="1">
+        <f t="array" ref="AA283">_xlfn.XLOOKUP(E283&amp;I283,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!F$2:F$13000,"")</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="284" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A284" s="1">
+        <v>44898</v>
+      </c>
+      <c r="B284" s="2">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="C284" t="s">
+        <v>33</v>
+      </c>
+      <c r="D284" t="s">
+        <v>173</v>
+      </c>
+      <c r="E284" t="s">
+        <v>88</v>
+      </c>
+      <c r="F284">
+        <v>0</v>
+      </c>
+      <c r="G284">
+        <v>2022</v>
+      </c>
+      <c r="H284">
+        <v>0</v>
+      </c>
+      <c r="I284">
+        <v>14</v>
+      </c>
+      <c r="J284" cm="1">
+        <f t="array" ref="J284">_xlfn.XLOOKUP(D284&amp;I284,Ranking!C$2:C$500&amp;Ranking!A$2:A$500,Ranking!B$2:B$500,"")</f>
+        <v>18</v>
+      </c>
+      <c r="K284" cm="1">
+        <f t="array" ref="K284">_xlfn.XLOOKUP(E284&amp;I284,Ranking!C$2:C$500&amp;Ranking!A$2:A$500,Ranking!B$2:B$500,"")</f>
+        <v>22</v>
+      </c>
+      <c r="L284" t="s">
+        <v>68</v>
+      </c>
+      <c r="M284" t="s">
+        <v>68</v>
+      </c>
+      <c r="N284">
+        <v>1</v>
+      </c>
+      <c r="O284" cm="1">
+        <f t="array" ref="O284">_xlfn.XLOOKUP(D284&amp;I284,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!C$2:C$13000,"")</f>
+        <v>34.4</v>
+      </c>
+      <c r="P284" cm="1">
+        <f t="array" ref="P284">_xlfn.XLOOKUP(D284&amp;I284,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!D$2:D$13000,"")</f>
+        <v>19.8</v>
+      </c>
+      <c r="Q284" cm="1">
+        <f t="array" ref="Q284">_xlfn.XLOOKUP(E284&amp;I284,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!C$2:C$13000,"")</f>
+        <v>34.9</v>
+      </c>
+      <c r="R284" cm="1">
+        <f t="array" ref="R284">_xlfn.XLOOKUP(E284&amp;I284,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!D$2:D$13000,"")</f>
+        <v>21.3</v>
+      </c>
+      <c r="X284" cm="1">
+        <f t="array" ref="X284">_xlfn.XLOOKUP(D284&amp;I284,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!E$2:E$13000,"")</f>
+        <v>10</v>
+      </c>
+      <c r="Y284" cm="1">
+        <f t="array" ref="Y284">_xlfn.XLOOKUP(D284&amp;I284,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!F$2:F$13000,"")</f>
+        <v>2</v>
+      </c>
+      <c r="Z284" cm="1">
+        <f t="array" ref="Z284">_xlfn.XLOOKUP(E284&amp;I284,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!E$2:E$13000,"")</f>
+        <v>9</v>
+      </c>
+      <c r="AA284" cm="1">
+        <f t="array" ref="AA284">_xlfn.XLOOKUP(E284&amp;I284,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!F$2:F$13000,"")</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="285" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A285" s="1">
+        <v>44898</v>
+      </c>
+      <c r="B285" s="2">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="C285" t="s">
+        <v>24</v>
+      </c>
+      <c r="D285" t="s">
+        <v>27</v>
+      </c>
+      <c r="E285" t="s">
+        <v>132</v>
+      </c>
+      <c r="F285">
+        <v>0</v>
+      </c>
+      <c r="G285">
+        <v>2022</v>
+      </c>
+      <c r="H285">
+        <v>0</v>
+      </c>
+      <c r="I285">
+        <v>14</v>
+      </c>
+      <c r="J285" t="str" cm="1">
+        <f t="array" ref="J285">_xlfn.XLOOKUP(D285&amp;I285,Ranking!C$2:C$500&amp;Ranking!A$2:A$500,Ranking!B$2:B$500,"")</f>
+        <v/>
+      </c>
+      <c r="K285" t="str" cm="1">
+        <f t="array" ref="K285">_xlfn.XLOOKUP(E285&amp;I285,Ranking!C$2:C$500&amp;Ranking!A$2:A$500,Ranking!B$2:B$500,"")</f>
+        <v/>
+      </c>
+      <c r="L285" t="s">
+        <v>66</v>
+      </c>
+      <c r="M285" t="s">
+        <v>66</v>
+      </c>
+      <c r="N285">
+        <v>1</v>
+      </c>
+      <c r="O285" cm="1">
+        <f t="array" ref="O285">_xlfn.XLOOKUP(D285&amp;I285,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!C$2:C$13000,"")</f>
+        <v>30.2</v>
+      </c>
+      <c r="P285" cm="1">
+        <f t="array" ref="P285">_xlfn.XLOOKUP(D285&amp;I285,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!D$2:D$13000,"")</f>
+        <v>17.8</v>
+      </c>
+      <c r="Q285" cm="1">
+        <f t="array" ref="Q285">_xlfn.XLOOKUP(E285&amp;I285,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!C$2:C$13000,"")</f>
+        <v>30.9</v>
+      </c>
+      <c r="R285" cm="1">
+        <f t="array" ref="R285">_xlfn.XLOOKUP(E285&amp;I285,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!D$2:D$13000,"")</f>
+        <v>20.8</v>
+      </c>
+      <c r="X285" cm="1">
+        <f t="array" ref="X285">_xlfn.XLOOKUP(D285&amp;I285,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!E$2:E$13000,"")</f>
+        <v>9</v>
+      </c>
+      <c r="Y285" cm="1">
+        <f t="array" ref="Y285">_xlfn.XLOOKUP(D285&amp;I285,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!F$2:F$13000,"")</f>
+        <v>3</v>
+      </c>
+      <c r="Z285" cm="1">
+        <f t="array" ref="Z285">_xlfn.XLOOKUP(E285&amp;I285,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!E$2:E$13000,"")</f>
+        <v>8</v>
+      </c>
+      <c r="AA285" cm="1">
+        <f t="array" ref="AA285">_xlfn.XLOOKUP(E285&amp;I285,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!F$2:F$13000,"")</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="286" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A286" s="1">
+        <v>44898</v>
+      </c>
+      <c r="B286" s="2">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="C286" t="s">
+        <v>24</v>
+      </c>
+      <c r="D286" t="s">
+        <v>38</v>
+      </c>
+      <c r="E286" t="s">
+        <v>43</v>
+      </c>
+      <c r="F286">
+        <v>0</v>
+      </c>
+      <c r="G286">
+        <v>2022</v>
+      </c>
+      <c r="H286">
+        <v>0</v>
+      </c>
+      <c r="I286">
+        <v>14</v>
+      </c>
+      <c r="J286" cm="1">
+        <f t="array" ref="J286">_xlfn.XLOOKUP(D286&amp;I286,Ranking!C$2:C$500&amp;Ranking!A$2:A$500,Ranking!B$2:B$500,"")</f>
+        <v>2</v>
+      </c>
+      <c r="K286" t="str" cm="1">
+        <f t="array" ref="K286">_xlfn.XLOOKUP(E286&amp;I286,Ranking!C$2:C$500&amp;Ranking!A$2:A$500,Ranking!B$2:B$500,"")</f>
+        <v/>
+      </c>
+      <c r="L286" t="s">
+        <v>64</v>
+      </c>
+      <c r="M286" t="s">
+        <v>64</v>
+      </c>
+      <c r="N286">
+        <v>1</v>
+      </c>
+      <c r="O286" cm="1">
+        <f t="array" ref="O286">_xlfn.XLOOKUP(D286&amp;I286,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!C$2:C$13000,"")</f>
+        <v>39.799999999999997</v>
+      </c>
+      <c r="P286" cm="1">
+        <f t="array" ref="P286">_xlfn.XLOOKUP(D286&amp;I286,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!D$2:D$13000,"")</f>
+        <v>12.7</v>
+      </c>
+      <c r="Q286" cm="1">
+        <f t="array" ref="Q286">_xlfn.XLOOKUP(E286&amp;I286,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!C$2:C$13000,"")</f>
+        <v>28.6</v>
+      </c>
+      <c r="R286" cm="1">
+        <f t="array" ref="R286">_xlfn.XLOOKUP(E286&amp;I286,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!D$2:D$13000,"")</f>
+        <v>23.1</v>
+      </c>
+      <c r="X286" cm="1">
+        <f t="array" ref="X286">_xlfn.XLOOKUP(D286&amp;I286,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!E$2:E$13000,"")</f>
+        <v>12</v>
+      </c>
+      <c r="Y286" cm="1">
+        <f t="array" ref="Y286">_xlfn.XLOOKUP(D286&amp;I286,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!F$2:F$13000,"")</f>
+        <v>0</v>
+      </c>
+      <c r="Z286" cm="1">
+        <f t="array" ref="Z286">_xlfn.XLOOKUP(E286&amp;I286,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!E$2:E$13000,"")</f>
+        <v>8</v>
+      </c>
+      <c r="AA286" cm="1">
+        <f t="array" ref="AA286">_xlfn.XLOOKUP(E286&amp;I286,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!F$2:F$13000,"")</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="287" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A287" s="1">
+        <v>44898</v>
+      </c>
+      <c r="B287" s="2">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="C287" t="s">
+        <v>33</v>
+      </c>
+      <c r="D287" t="s">
+        <v>154</v>
+      </c>
+      <c r="E287" t="s">
+        <v>87</v>
+      </c>
+      <c r="F287">
+        <v>0</v>
+      </c>
+      <c r="G287">
+        <v>2022</v>
+      </c>
+      <c r="H287">
+        <v>0</v>
+      </c>
+      <c r="I287">
+        <v>14</v>
+      </c>
+      <c r="J287" cm="1">
+        <f t="array" ref="J287">_xlfn.XLOOKUP(D287&amp;I287,Ranking!C$2:C$500&amp;Ranking!A$2:A$500,Ranking!B$2:B$500,"")</f>
+        <v>23</v>
+      </c>
+      <c r="K287" cm="1">
+        <f t="array" ref="K287">_xlfn.XLOOKUP(E287&amp;I287,Ranking!C$2:C$500&amp;Ranking!A$2:A$500,Ranking!B$2:B$500,"")</f>
+        <v>9</v>
+      </c>
+      <c r="L287" t="s">
+        <v>69</v>
+      </c>
+      <c r="M287" t="s">
+        <v>69</v>
+      </c>
+      <c r="N287">
+        <v>1</v>
+      </c>
+      <c r="O287" cm="1">
+        <f t="array" ref="O287">_xlfn.XLOOKUP(D287&amp;I287,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!C$2:C$13000,"")</f>
+        <v>37.1</v>
+      </c>
+      <c r="P287" cm="1">
+        <f t="array" ref="P287">_xlfn.XLOOKUP(D287&amp;I287,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!D$2:D$13000,"")</f>
+        <v>30.3</v>
+      </c>
+      <c r="Q287" cm="1">
+        <f t="array" ref="Q287">_xlfn.XLOOKUP(E287&amp;I287,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!C$2:C$13000,"")</f>
+        <v>34.299999999999997</v>
+      </c>
+      <c r="R287" cm="1">
+        <f t="array" ref="R287">_xlfn.XLOOKUP(E287&amp;I287,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!D$2:D$13000,"")</f>
+        <v>20.9</v>
+      </c>
+      <c r="X287" cm="1">
+        <f t="array" ref="X287">_xlfn.XLOOKUP(D287&amp;I287,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!E$2:E$13000,"")</f>
+        <v>9</v>
+      </c>
+      <c r="Y287" cm="1">
+        <f t="array" ref="Y287">_xlfn.XLOOKUP(D287&amp;I287,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!F$2:F$13000,"")</f>
+        <v>3</v>
+      </c>
+      <c r="Z287" cm="1">
+        <f t="array" ref="Z287">_xlfn.XLOOKUP(E287&amp;I287,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!E$2:E$13000,"")</f>
+        <v>10</v>
+      </c>
+      <c r="AA287" cm="1">
+        <f t="array" ref="AA287">_xlfn.XLOOKUP(E287&amp;I287,Sheet2!A$2:A$13000&amp;Sheet2!B$2:B$13000,Sheet2!F$2:F$13000,"")</f>
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -24572,10 +25277,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF262906-C2E8-EB40-9ABF-94137CE271DB}">
-  <dimension ref="A1:F1571"/>
+  <dimension ref="A1:F1702"/>
   <sheetViews>
-    <sheetView topLeftCell="A1509" workbookViewId="0">
-      <selection activeCell="A1516" sqref="A1516"/>
+    <sheetView topLeftCell="A1614" workbookViewId="0">
+      <selection activeCell="B1624" sqref="B1624"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -55998,6 +56703,2626 @@
       </c>
       <c r="F1571">
         <v>4</v>
+      </c>
+    </row>
+    <row r="1572" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1572" t="s">
+        <v>106</v>
+      </c>
+      <c r="B1572">
+        <v>14</v>
+      </c>
+      <c r="C1572">
+        <v>27.7</v>
+      </c>
+      <c r="D1572">
+        <v>13.3</v>
+      </c>
+      <c r="E1572">
+        <v>9</v>
+      </c>
+      <c r="F1572">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1573" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1573" t="s">
+        <v>119</v>
+      </c>
+      <c r="B1573">
+        <v>14</v>
+      </c>
+      <c r="C1573">
+        <v>21.7</v>
+      </c>
+      <c r="D1573">
+        <v>34.5</v>
+      </c>
+      <c r="E1573">
+        <v>2</v>
+      </c>
+      <c r="F1573">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="1574" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1574" t="s">
+        <v>91</v>
+      </c>
+      <c r="B1574">
+        <v>14</v>
+      </c>
+      <c r="C1574">
+        <v>40.799999999999997</v>
+      </c>
+      <c r="D1574">
+        <v>18</v>
+      </c>
+      <c r="E1574">
+        <v>10</v>
+      </c>
+      <c r="F1574">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1575" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1575" t="s">
+        <v>102</v>
+      </c>
+      <c r="B1575">
+        <v>14</v>
+      </c>
+      <c r="C1575">
+        <v>34.9</v>
+      </c>
+      <c r="D1575">
+        <v>26.8</v>
+      </c>
+      <c r="E1575">
+        <v>6</v>
+      </c>
+      <c r="F1575">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1576" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1576" t="s">
+        <v>112</v>
+      </c>
+      <c r="B1576">
+        <v>14</v>
+      </c>
+      <c r="C1576">
+        <v>30.8</v>
+      </c>
+      <c r="D1576">
+        <v>36.5</v>
+      </c>
+      <c r="E1576">
+        <v>5</v>
+      </c>
+      <c r="F1576">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1577" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1577" t="s">
+        <v>96</v>
+      </c>
+      <c r="B1577">
+        <v>14</v>
+      </c>
+      <c r="C1577">
+        <v>26.1</v>
+      </c>
+      <c r="D1577">
+        <v>31.4</v>
+      </c>
+      <c r="E1577">
+        <v>3</v>
+      </c>
+      <c r="F1577">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="1578" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1578" t="s">
+        <v>50</v>
+      </c>
+      <c r="B1578">
+        <v>14</v>
+      </c>
+      <c r="C1578">
+        <v>30.7</v>
+      </c>
+      <c r="D1578">
+        <v>28.8</v>
+      </c>
+      <c r="E1578">
+        <v>6</v>
+      </c>
+      <c r="F1578">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1579" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1579" t="s">
+        <v>120</v>
+      </c>
+      <c r="B1579">
+        <v>14</v>
+      </c>
+      <c r="C1579">
+        <v>25</v>
+      </c>
+      <c r="D1579">
+        <v>31.4</v>
+      </c>
+      <c r="E1579">
+        <v>3</v>
+      </c>
+      <c r="F1579">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="1580" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1580" t="s">
+        <v>121</v>
+      </c>
+      <c r="B1580">
+        <v>14</v>
+      </c>
+      <c r="C1580">
+        <v>29.4</v>
+      </c>
+      <c r="D1580">
+        <v>23</v>
+      </c>
+      <c r="E1580">
+        <v>5</v>
+      </c>
+      <c r="F1580">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1581" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1581" t="s">
+        <v>122</v>
+      </c>
+      <c r="B1581">
+        <v>14</v>
+      </c>
+      <c r="C1581">
+        <v>24.8</v>
+      </c>
+      <c r="D1581">
+        <v>29.5</v>
+      </c>
+      <c r="E1581">
+        <v>5</v>
+      </c>
+      <c r="F1581">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1582" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1582" t="s">
+        <v>123</v>
+      </c>
+      <c r="B1582">
+        <v>14</v>
+      </c>
+      <c r="C1582">
+        <v>23.3</v>
+      </c>
+      <c r="D1582">
+        <v>26.9</v>
+      </c>
+      <c r="E1582">
+        <v>5</v>
+      </c>
+      <c r="F1582">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1583" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1583" t="s">
+        <v>98</v>
+      </c>
+      <c r="B1583">
+        <v>14</v>
+      </c>
+      <c r="C1583">
+        <v>33.6</v>
+      </c>
+      <c r="D1583">
+        <v>26.6</v>
+      </c>
+      <c r="E1583">
+        <v>6</v>
+      </c>
+      <c r="F1583">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1584" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1584" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1584">
+        <v>14</v>
+      </c>
+      <c r="C1584">
+        <v>30.2</v>
+      </c>
+      <c r="D1584">
+        <v>17.8</v>
+      </c>
+      <c r="E1584">
+        <v>9</v>
+      </c>
+      <c r="F1584">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1585" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1585" t="s">
+        <v>124</v>
+      </c>
+      <c r="B1585">
+        <v>14</v>
+      </c>
+      <c r="C1585">
+        <v>17.8</v>
+      </c>
+      <c r="D1585">
+        <v>30.3</v>
+      </c>
+      <c r="E1585">
+        <v>3</v>
+      </c>
+      <c r="F1585">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="1586" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1586" t="s">
+        <v>125</v>
+      </c>
+      <c r="B1586">
+        <v>14</v>
+      </c>
+      <c r="C1586">
+        <v>23.8</v>
+      </c>
+      <c r="D1586">
+        <v>33.299999999999997</v>
+      </c>
+      <c r="E1586">
+        <v>6</v>
+      </c>
+      <c r="F1586">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1587" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1587" t="s">
+        <v>126</v>
+      </c>
+      <c r="B1587">
+        <v>14</v>
+      </c>
+      <c r="C1587">
+        <v>29.5</v>
+      </c>
+      <c r="D1587">
+        <v>27.6</v>
+      </c>
+      <c r="E1587">
+        <v>5</v>
+      </c>
+      <c r="F1587">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1588" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1588" t="s">
+        <v>97</v>
+      </c>
+      <c r="B1588">
+        <v>14</v>
+      </c>
+      <c r="C1588">
+        <v>31.9</v>
+      </c>
+      <c r="D1588">
+        <v>30</v>
+      </c>
+      <c r="E1588">
+        <v>7</v>
+      </c>
+      <c r="F1588">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1589" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1589" t="s">
+        <v>127</v>
+      </c>
+      <c r="B1589">
+        <v>14</v>
+      </c>
+      <c r="C1589">
+        <v>23.9</v>
+      </c>
+      <c r="D1589">
+        <v>27.8</v>
+      </c>
+      <c r="E1589">
+        <v>4</v>
+      </c>
+      <c r="F1589">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="1590" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1590" t="s">
+        <v>61</v>
+      </c>
+      <c r="B1590">
+        <v>14</v>
+      </c>
+      <c r="C1590">
+        <v>24.8</v>
+      </c>
+      <c r="D1590">
+        <v>28.2</v>
+      </c>
+      <c r="E1590">
+        <v>4</v>
+      </c>
+      <c r="F1590">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="1591" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1591" t="s">
+        <v>82</v>
+      </c>
+      <c r="B1591">
+        <v>14</v>
+      </c>
+      <c r="C1591">
+        <v>24.4</v>
+      </c>
+      <c r="D1591">
+        <v>39.4</v>
+      </c>
+      <c r="E1591">
+        <v>3</v>
+      </c>
+      <c r="F1591">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="1592" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1592" t="s">
+        <v>57</v>
+      </c>
+      <c r="B1592">
+        <v>14</v>
+      </c>
+      <c r="C1592">
+        <v>31.1</v>
+      </c>
+      <c r="D1592">
+        <v>20.3</v>
+      </c>
+      <c r="E1592">
+        <v>9</v>
+      </c>
+      <c r="F1592">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1593" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1593" t="s">
+        <v>87</v>
+      </c>
+      <c r="B1593">
+        <v>14</v>
+      </c>
+      <c r="C1593">
+        <v>34.299999999999997</v>
+      </c>
+      <c r="D1593">
+        <v>20.9</v>
+      </c>
+      <c r="E1593">
+        <v>10</v>
+      </c>
+      <c r="F1593">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1594" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1594" t="s">
+        <v>128</v>
+      </c>
+      <c r="B1594">
+        <v>14</v>
+      </c>
+      <c r="C1594">
+        <v>29.4</v>
+      </c>
+      <c r="D1594">
+        <v>28.7</v>
+      </c>
+      <c r="E1594">
+        <v>9</v>
+      </c>
+      <c r="F1594">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1595" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1595" t="s">
+        <v>107</v>
+      </c>
+      <c r="B1595">
+        <v>14</v>
+      </c>
+      <c r="C1595">
+        <v>15.4</v>
+      </c>
+      <c r="D1595">
+        <v>44.5</v>
+      </c>
+      <c r="E1595">
+        <v>1</v>
+      </c>
+      <c r="F1595">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1596" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1596" t="s">
+        <v>59</v>
+      </c>
+      <c r="B1596">
+        <v>14</v>
+      </c>
+      <c r="C1596">
+        <v>13.2</v>
+      </c>
+      <c r="D1596">
+        <v>26.9</v>
+      </c>
+      <c r="E1596">
+        <v>3</v>
+      </c>
+      <c r="F1596">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="1597" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1597" t="s">
+        <v>80</v>
+      </c>
+      <c r="B1597">
+        <v>14</v>
+      </c>
+      <c r="C1597">
+        <v>19.8</v>
+      </c>
+      <c r="D1597">
+        <v>26.1</v>
+      </c>
+      <c r="E1597">
+        <v>6</v>
+      </c>
+      <c r="F1597">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1598" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1598" t="s">
+        <v>129</v>
+      </c>
+      <c r="B1598">
+        <v>14</v>
+      </c>
+      <c r="C1598">
+        <v>33.1</v>
+      </c>
+      <c r="D1598">
+        <v>22.8</v>
+      </c>
+      <c r="E1598">
+        <v>8</v>
+      </c>
+      <c r="F1598">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1599" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1599" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1599">
+        <v>14</v>
+      </c>
+      <c r="C1599">
+        <v>30.8</v>
+      </c>
+      <c r="D1599">
+        <v>27</v>
+      </c>
+      <c r="E1599">
+        <v>7</v>
+      </c>
+      <c r="F1599">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1600" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1600" t="s">
+        <v>130</v>
+      </c>
+      <c r="B1600">
+        <v>14</v>
+      </c>
+      <c r="C1600">
+        <v>28.8</v>
+      </c>
+      <c r="D1600">
+        <v>28.6</v>
+      </c>
+      <c r="E1600">
+        <v>8</v>
+      </c>
+      <c r="F1600">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1601" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1601" t="s">
+        <v>52</v>
+      </c>
+      <c r="B1601">
+        <v>14</v>
+      </c>
+      <c r="C1601">
+        <v>31.8</v>
+      </c>
+      <c r="D1601">
+        <v>28.8</v>
+      </c>
+      <c r="E1601">
+        <v>6</v>
+      </c>
+      <c r="F1601">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1602" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1602" t="s">
+        <v>81</v>
+      </c>
+      <c r="B1602">
+        <v>14</v>
+      </c>
+      <c r="C1602">
+        <v>29.8</v>
+      </c>
+      <c r="D1602">
+        <v>26.6</v>
+      </c>
+      <c r="E1602">
+        <v>5</v>
+      </c>
+      <c r="F1602">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1603" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1603" t="s">
+        <v>131</v>
+      </c>
+      <c r="B1603">
+        <v>14</v>
+      </c>
+      <c r="C1603">
+        <v>18.7</v>
+      </c>
+      <c r="D1603">
+        <v>37.299999999999997</v>
+      </c>
+      <c r="E1603">
+        <v>4</v>
+      </c>
+      <c r="F1603">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="1604" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1604" t="s">
+        <v>115</v>
+      </c>
+      <c r="B1604">
+        <v>14</v>
+      </c>
+      <c r="C1604">
+        <v>36.200000000000003</v>
+      </c>
+      <c r="D1604">
+        <v>19.7</v>
+      </c>
+      <c r="E1604">
+        <v>9</v>
+      </c>
+      <c r="F1604">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1605" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1605" t="s">
+        <v>132</v>
+      </c>
+      <c r="B1605">
+        <v>14</v>
+      </c>
+      <c r="C1605">
+        <v>30.9</v>
+      </c>
+      <c r="D1605">
+        <v>20.8</v>
+      </c>
+      <c r="E1605">
+        <v>8</v>
+      </c>
+      <c r="F1605">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1606" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1606" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1606">
+        <v>14</v>
+      </c>
+      <c r="C1606">
+        <v>38.299999999999997</v>
+      </c>
+      <c r="D1606">
+        <v>11.3</v>
+      </c>
+      <c r="E1606">
+        <v>12</v>
+      </c>
+      <c r="F1606">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1607" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1607" t="s">
+        <v>111</v>
+      </c>
+      <c r="B1607">
+        <v>14</v>
+      </c>
+      <c r="C1607">
+        <v>33.700000000000003</v>
+      </c>
+      <c r="D1607">
+        <v>32.299999999999997</v>
+      </c>
+      <c r="E1607">
+        <v>6</v>
+      </c>
+      <c r="F1607">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1608" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1608" t="s">
+        <v>133</v>
+      </c>
+      <c r="B1608">
+        <v>14</v>
+      </c>
+      <c r="C1608">
+        <v>30</v>
+      </c>
+      <c r="D1608">
+        <v>31.2</v>
+      </c>
+      <c r="E1608">
+        <v>4</v>
+      </c>
+      <c r="F1608">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="1609" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1609" t="s">
+        <v>86</v>
+      </c>
+      <c r="B1609">
+        <v>14</v>
+      </c>
+      <c r="C1609">
+        <v>17.2</v>
+      </c>
+      <c r="D1609">
+        <v>28.4</v>
+      </c>
+      <c r="E1609">
+        <v>5</v>
+      </c>
+      <c r="F1609">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1610" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1610" t="s">
+        <v>134</v>
+      </c>
+      <c r="B1610">
+        <v>14</v>
+      </c>
+      <c r="C1610">
+        <v>19.8</v>
+      </c>
+      <c r="D1610">
+        <v>34.700000000000003</v>
+      </c>
+      <c r="E1610">
+        <v>3</v>
+      </c>
+      <c r="F1610">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="1611" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1611" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1611">
+        <v>14</v>
+      </c>
+      <c r="C1611">
+        <v>37.200000000000003</v>
+      </c>
+      <c r="D1611">
+        <v>33.5</v>
+      </c>
+      <c r="E1611">
+        <v>7</v>
+      </c>
+      <c r="F1611">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1612" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1612" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1612">
+        <v>14</v>
+      </c>
+      <c r="C1612">
+        <v>25.4</v>
+      </c>
+      <c r="D1612">
+        <v>12.3</v>
+      </c>
+      <c r="E1612">
+        <v>8</v>
+      </c>
+      <c r="F1612">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1613" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1613" t="s">
+        <v>41</v>
+      </c>
+      <c r="B1613">
+        <v>14</v>
+      </c>
+      <c r="C1613">
+        <v>23.3</v>
+      </c>
+      <c r="D1613">
+        <v>33.9</v>
+      </c>
+      <c r="E1613">
+        <v>4</v>
+      </c>
+      <c r="F1613">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="1614" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1614" t="s">
+        <v>135</v>
+      </c>
+      <c r="B1614">
+        <v>14</v>
+      </c>
+      <c r="C1614">
+        <v>17.399999999999999</v>
+      </c>
+      <c r="D1614">
+        <v>14.4</v>
+      </c>
+      <c r="E1614">
+        <v>7</v>
+      </c>
+      <c r="F1614">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1615" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1615" t="s">
+        <v>136</v>
+      </c>
+      <c r="B1615">
+        <v>14</v>
+      </c>
+      <c r="C1615">
+        <v>20.2</v>
+      </c>
+      <c r="D1615">
+        <v>20.3</v>
+      </c>
+      <c r="E1615">
+        <v>4</v>
+      </c>
+      <c r="F1615">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="1616" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1616" t="s">
+        <v>137</v>
+      </c>
+      <c r="B1616">
+        <v>14</v>
+      </c>
+      <c r="C1616">
+        <v>37</v>
+      </c>
+      <c r="D1616">
+        <v>20.9</v>
+      </c>
+      <c r="E1616">
+        <v>8</v>
+      </c>
+      <c r="F1616">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1617" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1617" t="s">
+        <v>138</v>
+      </c>
+      <c r="B1617">
+        <v>14</v>
+      </c>
+      <c r="C1617">
+        <v>34.200000000000003</v>
+      </c>
+      <c r="D1617">
+        <v>33.799999999999997</v>
+      </c>
+      <c r="E1617">
+        <v>6</v>
+      </c>
+      <c r="F1617">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1618" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1618" t="s">
+        <v>93</v>
+      </c>
+      <c r="B1618">
+        <v>14</v>
+      </c>
+      <c r="C1618">
+        <v>33.4</v>
+      </c>
+      <c r="D1618">
+        <v>19.399999999999999</v>
+      </c>
+      <c r="E1618">
+        <v>9</v>
+      </c>
+      <c r="F1618">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1619" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1619" t="s">
+        <v>139</v>
+      </c>
+      <c r="B1619">
+        <v>14</v>
+      </c>
+      <c r="C1619">
+        <v>28.4</v>
+      </c>
+      <c r="D1619">
+        <v>29</v>
+      </c>
+      <c r="E1619">
+        <v>5</v>
+      </c>
+      <c r="F1619">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1620" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1620" t="s">
+        <v>108</v>
+      </c>
+      <c r="B1620">
+        <v>14</v>
+      </c>
+      <c r="C1620">
+        <v>22.1</v>
+      </c>
+      <c r="D1620">
+        <v>19.100000000000001</v>
+      </c>
+      <c r="E1620">
+        <v>7</v>
+      </c>
+      <c r="F1620">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1621" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1621" t="s">
+        <v>140</v>
+      </c>
+      <c r="B1621">
+        <v>14</v>
+      </c>
+      <c r="C1621">
+        <v>28.3</v>
+      </c>
+      <c r="D1621">
+        <v>24.9</v>
+      </c>
+      <c r="E1621">
+        <v>8</v>
+      </c>
+      <c r="F1621">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1622" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1622" t="s">
+        <v>141</v>
+      </c>
+      <c r="B1622">
+        <v>14</v>
+      </c>
+      <c r="C1622">
+        <v>29</v>
+      </c>
+      <c r="D1622">
+        <v>37.9</v>
+      </c>
+      <c r="E1622">
+        <v>3</v>
+      </c>
+      <c r="F1622">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="1623" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1623" t="s">
+        <v>142</v>
+      </c>
+      <c r="B1623">
+        <v>14</v>
+      </c>
+      <c r="C1623">
+        <v>27</v>
+      </c>
+      <c r="D1623">
+        <v>22.8</v>
+      </c>
+      <c r="E1623">
+        <v>6</v>
+      </c>
+      <c r="F1623">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1624" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1624" t="s">
+        <v>143</v>
+      </c>
+      <c r="B1624">
+        <v>14</v>
+      </c>
+      <c r="C1624">
+        <v>22.3</v>
+      </c>
+      <c r="D1624">
+        <v>34.4</v>
+      </c>
+      <c r="E1624">
+        <v>4</v>
+      </c>
+      <c r="F1624">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="1625" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1625" t="s">
+        <v>89</v>
+      </c>
+      <c r="B1625">
+        <v>14</v>
+      </c>
+      <c r="C1625">
+        <v>27.2</v>
+      </c>
+      <c r="D1625">
+        <v>20.2</v>
+      </c>
+      <c r="E1625">
+        <v>7</v>
+      </c>
+      <c r="F1625">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1626" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1626" t="s">
+        <v>114</v>
+      </c>
+      <c r="B1626">
+        <v>14</v>
+      </c>
+      <c r="C1626">
+        <v>32.5</v>
+      </c>
+      <c r="D1626">
+        <v>21.5</v>
+      </c>
+      <c r="E1626">
+        <v>9</v>
+      </c>
+      <c r="F1626">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1627" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1627" t="s">
+        <v>100</v>
+      </c>
+      <c r="B1627">
+        <v>14</v>
+      </c>
+      <c r="C1627">
+        <v>24.2</v>
+      </c>
+      <c r="D1627">
+        <v>16.2</v>
+      </c>
+      <c r="E1627">
+        <v>8</v>
+      </c>
+      <c r="F1627">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1628" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1628" t="s">
+        <v>144</v>
+      </c>
+      <c r="B1628">
+        <v>14</v>
+      </c>
+      <c r="C1628">
+        <v>29.2</v>
+      </c>
+      <c r="D1628">
+        <v>24.1</v>
+      </c>
+      <c r="E1628">
+        <v>7</v>
+      </c>
+      <c r="F1628">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1629" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1629" t="s">
+        <v>145</v>
+      </c>
+      <c r="B1629">
+        <v>14</v>
+      </c>
+      <c r="C1629">
+        <v>12.5</v>
+      </c>
+      <c r="D1629">
+        <v>31.1</v>
+      </c>
+      <c r="E1629">
+        <v>1</v>
+      </c>
+      <c r="F1629">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1630" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1630" t="s">
+        <v>146</v>
+      </c>
+      <c r="B1630">
+        <v>14</v>
+      </c>
+      <c r="C1630">
+        <v>35.1</v>
+      </c>
+      <c r="D1630">
+        <v>27.3</v>
+      </c>
+      <c r="E1630">
+        <v>6</v>
+      </c>
+      <c r="F1630">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1631" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1631" t="s">
+        <v>147</v>
+      </c>
+      <c r="B1631">
+        <v>14</v>
+      </c>
+      <c r="C1631">
+        <v>23.6</v>
+      </c>
+      <c r="D1631">
+        <v>26.8</v>
+      </c>
+      <c r="E1631">
+        <v>5</v>
+      </c>
+      <c r="F1631">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1632" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1632" t="s">
+        <v>148</v>
+      </c>
+      <c r="B1632">
+        <v>14</v>
+      </c>
+      <c r="C1632">
+        <v>20.3</v>
+      </c>
+      <c r="D1632">
+        <v>22.5</v>
+      </c>
+      <c r="E1632">
+        <v>6</v>
+      </c>
+      <c r="F1632">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1633" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1633" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1633">
+        <v>14</v>
+      </c>
+      <c r="C1633">
+        <v>39.799999999999997</v>
+      </c>
+      <c r="D1633">
+        <v>12.7</v>
+      </c>
+      <c r="E1633">
+        <v>12</v>
+      </c>
+      <c r="F1633">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1634" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1634" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1634">
+        <v>14</v>
+      </c>
+      <c r="C1634">
+        <v>24.4</v>
+      </c>
+      <c r="D1634">
+        <v>27.4</v>
+      </c>
+      <c r="E1634">
+        <v>5</v>
+      </c>
+      <c r="F1634">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1635" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1635" t="s">
+        <v>149</v>
+      </c>
+      <c r="B1635">
+        <v>14</v>
+      </c>
+      <c r="C1635">
+        <v>29.2</v>
+      </c>
+      <c r="D1635">
+        <v>28.1</v>
+      </c>
+      <c r="E1635">
+        <v>7</v>
+      </c>
+      <c r="F1635">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1636" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1636" t="s">
+        <v>150</v>
+      </c>
+      <c r="B1636">
+        <v>14</v>
+      </c>
+      <c r="C1636">
+        <v>28.3</v>
+      </c>
+      <c r="D1636">
+        <v>13.3</v>
+      </c>
+      <c r="E1636">
+        <v>8</v>
+      </c>
+      <c r="F1636">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1637" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1637" t="s">
+        <v>151</v>
+      </c>
+      <c r="B1637">
+        <v>14</v>
+      </c>
+      <c r="C1637">
+        <v>34.200000000000003</v>
+      </c>
+      <c r="D1637">
+        <v>24.2</v>
+      </c>
+      <c r="E1637">
+        <v>8</v>
+      </c>
+      <c r="F1637">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1638" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1638" t="s">
+        <v>113</v>
+      </c>
+      <c r="B1638">
+        <v>14</v>
+      </c>
+      <c r="C1638">
+        <v>32.700000000000003</v>
+      </c>
+      <c r="D1638">
+        <v>24.2</v>
+      </c>
+      <c r="E1638">
+        <v>8</v>
+      </c>
+      <c r="F1638">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1639" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1639" t="s">
+        <v>94</v>
+      </c>
+      <c r="B1639">
+        <v>14</v>
+      </c>
+      <c r="C1639">
+        <v>25.5</v>
+      </c>
+      <c r="D1639">
+        <v>25</v>
+      </c>
+      <c r="E1639">
+        <v>6</v>
+      </c>
+      <c r="F1639">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1640" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1640" t="s">
+        <v>152</v>
+      </c>
+      <c r="B1640">
+        <v>14</v>
+      </c>
+      <c r="C1640">
+        <v>22.4</v>
+      </c>
+      <c r="D1640">
+        <v>24.7</v>
+      </c>
+      <c r="E1640">
+        <v>4</v>
+      </c>
+      <c r="F1640">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1641" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1641" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1641">
+        <v>14</v>
+      </c>
+      <c r="C1641">
+        <v>22.6</v>
+      </c>
+      <c r="D1641">
+        <v>27.6</v>
+      </c>
+      <c r="E1641">
+        <v>4</v>
+      </c>
+      <c r="F1641">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="1642" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1642" t="s">
+        <v>44</v>
+      </c>
+      <c r="B1642">
+        <v>14</v>
+      </c>
+      <c r="C1642">
+        <v>18.8</v>
+      </c>
+      <c r="D1642">
+        <v>30.9</v>
+      </c>
+      <c r="E1642">
+        <v>2</v>
+      </c>
+      <c r="F1642">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="1643" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1643" t="s">
+        <v>153</v>
+      </c>
+      <c r="B1643">
+        <v>14</v>
+      </c>
+      <c r="C1643">
+        <v>13.1</v>
+      </c>
+      <c r="D1643">
+        <v>26</v>
+      </c>
+      <c r="E1643">
+        <v>2</v>
+      </c>
+      <c r="F1643">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="1644" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1644" t="s">
+        <v>83</v>
+      </c>
+      <c r="B1644">
+        <v>14</v>
+      </c>
+      <c r="C1644">
+        <v>22</v>
+      </c>
+      <c r="D1644">
+        <v>26.3</v>
+      </c>
+      <c r="E1644">
+        <v>5</v>
+      </c>
+      <c r="F1644">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1645" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1645" t="s">
+        <v>154</v>
+      </c>
+      <c r="B1645">
+        <v>14</v>
+      </c>
+      <c r="C1645">
+        <v>37.1</v>
+      </c>
+      <c r="D1645">
+        <v>30.3</v>
+      </c>
+      <c r="E1645">
+        <v>9</v>
+      </c>
+      <c r="F1645">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1646" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1646" t="s">
+        <v>189</v>
+      </c>
+      <c r="B1646">
+        <v>14</v>
+      </c>
+      <c r="C1646">
+        <v>25.3</v>
+      </c>
+      <c r="D1646">
+        <v>19.399999999999999</v>
+      </c>
+      <c r="E1646">
+        <v>8</v>
+      </c>
+      <c r="F1646">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1647" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1647" t="s">
+        <v>155</v>
+      </c>
+      <c r="B1647">
+        <v>14</v>
+      </c>
+      <c r="C1647">
+        <v>34.5</v>
+      </c>
+      <c r="D1647">
+        <v>30.1</v>
+      </c>
+      <c r="E1647">
+        <v>7</v>
+      </c>
+      <c r="F1647">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1648" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1648" t="s">
+        <v>156</v>
+      </c>
+      <c r="B1648">
+        <v>14</v>
+      </c>
+      <c r="C1648">
+        <v>27.3</v>
+      </c>
+      <c r="D1648">
+        <v>32.799999999999997</v>
+      </c>
+      <c r="E1648">
+        <v>3</v>
+      </c>
+      <c r="F1648">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="1649" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1649" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1649">
+        <v>14</v>
+      </c>
+      <c r="C1649">
+        <v>13.8</v>
+      </c>
+      <c r="D1649">
+        <v>28.3</v>
+      </c>
+      <c r="E1649">
+        <v>1</v>
+      </c>
+      <c r="F1649">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1650" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1650" t="s">
+        <v>46</v>
+      </c>
+      <c r="B1650">
+        <v>14</v>
+      </c>
+      <c r="C1650">
+        <v>30.7</v>
+      </c>
+      <c r="D1650">
+        <v>21.8</v>
+      </c>
+      <c r="E1650">
+        <v>8</v>
+      </c>
+      <c r="F1650">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1651" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1651" t="s">
+        <v>157</v>
+      </c>
+      <c r="B1651">
+        <v>14</v>
+      </c>
+      <c r="C1651">
+        <v>34</v>
+      </c>
+      <c r="D1651">
+        <v>29.3</v>
+      </c>
+      <c r="E1651">
+        <v>9</v>
+      </c>
+      <c r="F1651">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1652" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1652" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1652">
+        <v>14</v>
+      </c>
+      <c r="C1652">
+        <v>44.5</v>
+      </c>
+      <c r="D1652">
+        <v>19.3</v>
+      </c>
+      <c r="E1652">
+        <v>11</v>
+      </c>
+      <c r="F1652">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1653" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1653" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1653">
+        <v>14</v>
+      </c>
+      <c r="C1653">
+        <v>32.9</v>
+      </c>
+      <c r="D1653">
+        <v>29.6</v>
+      </c>
+      <c r="E1653">
+        <v>6</v>
+      </c>
+      <c r="F1653">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1654" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1654" t="s">
+        <v>56</v>
+      </c>
+      <c r="B1654">
+        <v>14</v>
+      </c>
+      <c r="C1654">
+        <v>31.8</v>
+      </c>
+      <c r="D1654">
+        <v>29.3</v>
+      </c>
+      <c r="E1654">
+        <v>7</v>
+      </c>
+      <c r="F1654">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1655" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1655" t="s">
+        <v>158</v>
+      </c>
+      <c r="B1655">
+        <v>14</v>
+      </c>
+      <c r="C1655">
+        <v>19.5</v>
+      </c>
+      <c r="D1655">
+        <v>26.6</v>
+      </c>
+      <c r="E1655">
+        <v>3</v>
+      </c>
+      <c r="F1655">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="1656" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1656" t="s">
+        <v>49</v>
+      </c>
+      <c r="B1656">
+        <v>14</v>
+      </c>
+      <c r="C1656">
+        <v>39.700000000000003</v>
+      </c>
+      <c r="D1656">
+        <v>27.4</v>
+      </c>
+      <c r="E1656">
+        <v>9</v>
+      </c>
+      <c r="F1656">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1657" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1657" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1657">
+        <v>14</v>
+      </c>
+      <c r="C1657">
+        <v>32.4</v>
+      </c>
+      <c r="D1657">
+        <v>21.4</v>
+      </c>
+      <c r="E1657">
+        <v>9</v>
+      </c>
+      <c r="F1657">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1658" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1658" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1658">
+        <v>14</v>
+      </c>
+      <c r="C1658">
+        <v>35.799999999999997</v>
+      </c>
+      <c r="D1658">
+        <v>18</v>
+      </c>
+      <c r="E1658">
+        <v>10</v>
+      </c>
+      <c r="F1658">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1659" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1659" t="s">
+        <v>51</v>
+      </c>
+      <c r="B1659">
+        <v>14</v>
+      </c>
+      <c r="C1659">
+        <v>30.8</v>
+      </c>
+      <c r="D1659">
+        <v>23.4</v>
+      </c>
+      <c r="E1659">
+        <v>8</v>
+      </c>
+      <c r="F1659">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1660" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1660" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1660">
+        <v>14</v>
+      </c>
+      <c r="C1660">
+        <v>28.6</v>
+      </c>
+      <c r="D1660">
+        <v>23.1</v>
+      </c>
+      <c r="E1660">
+        <v>8</v>
+      </c>
+      <c r="F1660">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1661" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1661" t="s">
+        <v>159</v>
+      </c>
+      <c r="B1661">
+        <v>14</v>
+      </c>
+      <c r="C1661">
+        <v>25.3</v>
+      </c>
+      <c r="D1661">
+        <v>33.799999999999997</v>
+      </c>
+      <c r="E1661">
+        <v>5</v>
+      </c>
+      <c r="F1661">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1662" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1662" t="s">
+        <v>160</v>
+      </c>
+      <c r="B1662">
+        <v>14</v>
+      </c>
+      <c r="C1662">
+        <v>17.399999999999999</v>
+      </c>
+      <c r="D1662">
+        <v>29.3</v>
+      </c>
+      <c r="E1662">
+        <v>4</v>
+      </c>
+      <c r="F1662">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="1663" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1663" t="s">
+        <v>161</v>
+      </c>
+      <c r="B1663">
+        <v>14</v>
+      </c>
+      <c r="C1663">
+        <v>21.3</v>
+      </c>
+      <c r="D1663">
+        <v>20.2</v>
+      </c>
+      <c r="E1663">
+        <v>7</v>
+      </c>
+      <c r="F1663">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1664" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1664" t="s">
+        <v>162</v>
+      </c>
+      <c r="B1664">
+        <v>14</v>
+      </c>
+      <c r="C1664">
+        <v>27.5</v>
+      </c>
+      <c r="D1664">
+        <v>20.3</v>
+      </c>
+      <c r="E1664">
+        <v>7</v>
+      </c>
+      <c r="F1664">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1665" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1665" t="s">
+        <v>163</v>
+      </c>
+      <c r="B1665">
+        <v>14</v>
+      </c>
+      <c r="C1665">
+        <v>38.4</v>
+      </c>
+      <c r="D1665">
+        <v>34.700000000000003</v>
+      </c>
+      <c r="E1665">
+        <v>7</v>
+      </c>
+      <c r="F1665">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1666" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1666" t="s">
+        <v>164</v>
+      </c>
+      <c r="B1666">
+        <v>14</v>
+      </c>
+      <c r="C1666">
+        <v>31.9</v>
+      </c>
+      <c r="D1666">
+        <v>19.399999999999999</v>
+      </c>
+      <c r="E1666">
+        <v>10</v>
+      </c>
+      <c r="F1666">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1667" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1667" t="s">
+        <v>92</v>
+      </c>
+      <c r="B1667">
+        <v>14</v>
+      </c>
+      <c r="C1667">
+        <v>31.7</v>
+      </c>
+      <c r="D1667">
+        <v>27.5</v>
+      </c>
+      <c r="E1667">
+        <v>8</v>
+      </c>
+      <c r="F1667">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1668" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1668" t="s">
+        <v>165</v>
+      </c>
+      <c r="B1668">
+        <v>14</v>
+      </c>
+      <c r="C1668">
+        <v>28</v>
+      </c>
+      <c r="D1668">
+        <v>41.2</v>
+      </c>
+      <c r="E1668">
+        <v>1</v>
+      </c>
+      <c r="F1668">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1669" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1669" t="s">
+        <v>166</v>
+      </c>
+      <c r="B1669">
+        <v>14</v>
+      </c>
+      <c r="C1669">
+        <v>24.3</v>
+      </c>
+      <c r="D1669">
+        <v>23.5</v>
+      </c>
+      <c r="E1669">
+        <v>6</v>
+      </c>
+      <c r="F1669">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1670" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1670" t="s">
+        <v>109</v>
+      </c>
+      <c r="B1670">
+        <v>14</v>
+      </c>
+      <c r="C1670">
+        <v>21.3</v>
+      </c>
+      <c r="D1670">
+        <v>32.200000000000003</v>
+      </c>
+      <c r="E1670">
+        <v>3</v>
+      </c>
+      <c r="F1670">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="1671" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1671" t="s">
+        <v>167</v>
+      </c>
+      <c r="B1671">
+        <v>14</v>
+      </c>
+      <c r="C1671">
+        <v>28.3</v>
+      </c>
+      <c r="D1671">
+        <v>22.7</v>
+      </c>
+      <c r="E1671">
+        <v>7</v>
+      </c>
+      <c r="F1671">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1672" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1672" t="s">
+        <v>168</v>
+      </c>
+      <c r="B1672">
+        <v>14</v>
+      </c>
+      <c r="C1672">
+        <v>41.3</v>
+      </c>
+      <c r="D1672">
+        <v>24.5</v>
+      </c>
+      <c r="E1672">
+        <v>12</v>
+      </c>
+      <c r="F1672">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1673" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1673" t="s">
+        <v>169</v>
+      </c>
+      <c r="B1673">
+        <v>14</v>
+      </c>
+      <c r="C1673">
+        <v>21.9</v>
+      </c>
+      <c r="D1673">
+        <v>29.3</v>
+      </c>
+      <c r="E1673">
+        <v>3</v>
+      </c>
+      <c r="F1673">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="1674" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1674" t="s">
+        <v>104</v>
+      </c>
+      <c r="B1674">
+        <v>14</v>
+      </c>
+      <c r="C1674">
+        <v>47.3</v>
+      </c>
+      <c r="D1674">
+        <v>23.5</v>
+      </c>
+      <c r="E1674">
+        <v>10</v>
+      </c>
+      <c r="F1674">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1675" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1675" t="s">
+        <v>90</v>
+      </c>
+      <c r="B1675">
+        <v>14</v>
+      </c>
+      <c r="C1675">
+        <v>35.700000000000003</v>
+      </c>
+      <c r="D1675">
+        <v>21.2</v>
+      </c>
+      <c r="E1675">
+        <v>8</v>
+      </c>
+      <c r="F1675">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1676" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1676" t="s">
+        <v>101</v>
+      </c>
+      <c r="B1676">
+        <v>14</v>
+      </c>
+      <c r="C1676">
+        <v>22.8</v>
+      </c>
+      <c r="D1676">
+        <v>21.2</v>
+      </c>
+      <c r="E1676">
+        <v>5</v>
+      </c>
+      <c r="F1676">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1677" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1677" t="s">
+        <v>170</v>
+      </c>
+      <c r="B1677">
+        <v>14</v>
+      </c>
+      <c r="C1677">
+        <v>21.1</v>
+      </c>
+      <c r="D1677">
+        <v>26.3</v>
+      </c>
+      <c r="E1677">
+        <v>4</v>
+      </c>
+      <c r="F1677">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="1678" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1678" t="s">
+        <v>95</v>
+      </c>
+      <c r="B1678">
+        <v>14</v>
+      </c>
+      <c r="C1678">
+        <v>33.6</v>
+      </c>
+      <c r="D1678">
+        <v>29.5</v>
+      </c>
+      <c r="E1678">
+        <v>7</v>
+      </c>
+      <c r="F1678">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1679" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1679" t="s">
+        <v>171</v>
+      </c>
+      <c r="B1679">
+        <v>14</v>
+      </c>
+      <c r="C1679">
+        <v>33.299999999999997</v>
+      </c>
+      <c r="D1679">
+        <v>27.1</v>
+      </c>
+      <c r="E1679">
+        <v>7</v>
+      </c>
+      <c r="F1679">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1680" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1680" t="s">
+        <v>172</v>
+      </c>
+      <c r="B1680">
+        <v>14</v>
+      </c>
+      <c r="C1680">
+        <v>24.6</v>
+      </c>
+      <c r="D1680">
+        <v>16.8</v>
+      </c>
+      <c r="E1680">
+        <v>10</v>
+      </c>
+      <c r="F1680">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1681" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1681" t="s">
+        <v>173</v>
+      </c>
+      <c r="B1681">
+        <v>14</v>
+      </c>
+      <c r="C1681">
+        <v>34.4</v>
+      </c>
+      <c r="D1681">
+        <v>19.8</v>
+      </c>
+      <c r="E1681">
+        <v>10</v>
+      </c>
+      <c r="F1681">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1682" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1682" t="s">
+        <v>55</v>
+      </c>
+      <c r="B1682">
+        <v>14</v>
+      </c>
+      <c r="C1682">
+        <v>30.6</v>
+      </c>
+      <c r="D1682">
+        <v>33.1</v>
+      </c>
+      <c r="E1682">
+        <v>5</v>
+      </c>
+      <c r="F1682">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1683" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1683" t="s">
+        <v>174</v>
+      </c>
+      <c r="B1683">
+        <v>14</v>
+      </c>
+      <c r="C1683">
+        <v>30.6</v>
+      </c>
+      <c r="D1683">
+        <v>23.4</v>
+      </c>
+      <c r="E1683">
+        <v>6</v>
+      </c>
+      <c r="F1683">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1684" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1684" t="s">
+        <v>88</v>
+      </c>
+      <c r="B1684">
+        <v>14</v>
+      </c>
+      <c r="C1684">
+        <v>34.9</v>
+      </c>
+      <c r="D1684">
+        <v>21.3</v>
+      </c>
+      <c r="E1684">
+        <v>9</v>
+      </c>
+      <c r="F1684">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1685" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1685" t="s">
+        <v>175</v>
+      </c>
+      <c r="B1685">
+        <v>14</v>
+      </c>
+      <c r="C1685">
+        <v>39.6</v>
+      </c>
+      <c r="D1685">
+        <v>28.3</v>
+      </c>
+      <c r="E1685">
+        <v>9</v>
+      </c>
+      <c r="F1685">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1686" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1686" t="s">
+        <v>176</v>
+      </c>
+      <c r="B1686">
+        <v>14</v>
+      </c>
+      <c r="C1686">
+        <v>26.3</v>
+      </c>
+      <c r="D1686">
+        <v>28.5</v>
+      </c>
+      <c r="E1686">
+        <v>5</v>
+      </c>
+      <c r="F1686">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1687" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1687" t="s">
+        <v>110</v>
+      </c>
+      <c r="B1687">
+        <v>14</v>
+      </c>
+      <c r="C1687">
+        <v>42.5</v>
+      </c>
+      <c r="D1687">
+        <v>26.3</v>
+      </c>
+      <c r="E1687">
+        <v>11</v>
+      </c>
+      <c r="F1687">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1688" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1688" t="s">
+        <v>53</v>
+      </c>
+      <c r="B1688">
+        <v>14</v>
+      </c>
+      <c r="C1688">
+        <v>39.4</v>
+      </c>
+      <c r="D1688">
+        <v>20.100000000000001</v>
+      </c>
+      <c r="E1688">
+        <v>9</v>
+      </c>
+      <c r="F1688">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1689" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1689" t="s">
+        <v>58</v>
+      </c>
+      <c r="B1689">
+        <v>14</v>
+      </c>
+      <c r="C1689">
+        <v>23.3</v>
+      </c>
+      <c r="D1689">
+        <v>30.6</v>
+      </c>
+      <c r="E1689">
+        <v>6</v>
+      </c>
+      <c r="F1689">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1690" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1690" t="s">
+        <v>48</v>
+      </c>
+      <c r="B1690">
+        <v>14</v>
+      </c>
+      <c r="C1690">
+        <v>24.4</v>
+      </c>
+      <c r="D1690">
+        <v>27</v>
+      </c>
+      <c r="E1690">
+        <v>5</v>
+      </c>
+      <c r="F1690">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1691" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1691" t="s">
+        <v>45</v>
+      </c>
+      <c r="B1691">
+        <v>14</v>
+      </c>
+      <c r="C1691">
+        <v>37.9</v>
+      </c>
+      <c r="D1691">
+        <v>26.5</v>
+      </c>
+      <c r="E1691">
+        <v>10</v>
+      </c>
+      <c r="F1691">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1692" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1692" t="s">
+        <v>177</v>
+      </c>
+      <c r="B1692">
+        <v>14</v>
+      </c>
+      <c r="C1692">
+        <v>24.6</v>
+      </c>
+      <c r="D1692">
+        <v>36</v>
+      </c>
+      <c r="E1692">
+        <v>5</v>
+      </c>
+      <c r="F1692">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1693" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1693" t="s">
+        <v>178</v>
+      </c>
+      <c r="B1693">
+        <v>14</v>
+      </c>
+      <c r="C1693">
+        <v>17</v>
+      </c>
+      <c r="D1693">
+        <v>24</v>
+      </c>
+      <c r="E1693">
+        <v>3</v>
+      </c>
+      <c r="F1693">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1694" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1694" t="s">
+        <v>179</v>
+      </c>
+      <c r="B1694">
+        <v>14</v>
+      </c>
+      <c r="C1694">
+        <v>19.3</v>
+      </c>
+      <c r="D1694">
+        <v>24.7</v>
+      </c>
+      <c r="E1694">
+        <v>3</v>
+      </c>
+      <c r="F1694">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="1695" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1695" t="s">
+        <v>180</v>
+      </c>
+      <c r="B1695">
+        <v>14</v>
+      </c>
+      <c r="C1695">
+        <v>36.799999999999997</v>
+      </c>
+      <c r="D1695">
+        <v>29.3</v>
+      </c>
+      <c r="E1695">
+        <v>7</v>
+      </c>
+      <c r="F1695">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1696" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1696" t="s">
+        <v>181</v>
+      </c>
+      <c r="B1696">
+        <v>14</v>
+      </c>
+      <c r="C1696">
+        <v>40.799999999999997</v>
+      </c>
+      <c r="D1696">
+        <v>26.3</v>
+      </c>
+      <c r="E1696">
+        <v>10</v>
+      </c>
+      <c r="F1696">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1697" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1697" t="s">
+        <v>105</v>
+      </c>
+      <c r="B1697">
+        <v>14</v>
+      </c>
+      <c r="C1697">
+        <v>27.8</v>
+      </c>
+      <c r="D1697">
+        <v>22.4</v>
+      </c>
+      <c r="E1697">
+        <v>7</v>
+      </c>
+      <c r="F1697">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1698" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1698" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1698">
+        <v>14</v>
+      </c>
+      <c r="C1698">
+        <v>30.6</v>
+      </c>
+      <c r="D1698">
+        <v>32.9</v>
+      </c>
+      <c r="E1698">
+        <v>5</v>
+      </c>
+      <c r="F1698">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1699" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1699" t="s">
+        <v>182</v>
+      </c>
+      <c r="B1699">
+        <v>14</v>
+      </c>
+      <c r="C1699">
+        <v>35.799999999999997</v>
+      </c>
+      <c r="D1699">
+        <v>23.5</v>
+      </c>
+      <c r="E1699">
+        <v>8</v>
+      </c>
+      <c r="F1699">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1700" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1700" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1700">
+        <v>14</v>
+      </c>
+      <c r="C1700">
+        <v>19</v>
+      </c>
+      <c r="D1700">
+        <v>24.1</v>
+      </c>
+      <c r="E1700">
+        <v>5</v>
+      </c>
+      <c r="F1700">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1701" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1701" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1701">
+        <v>14</v>
+      </c>
+      <c r="C1701">
+        <v>26.5</v>
+      </c>
+      <c r="D1701">
+        <v>20.5</v>
+      </c>
+      <c r="E1701">
+        <v>6</v>
+      </c>
+      <c r="F1701">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1702" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1702" t="s">
+        <v>62</v>
+      </c>
+      <c r="B1702">
+        <v>14</v>
+      </c>
+      <c r="C1702">
+        <v>20.8</v>
+      </c>
+      <c r="D1702">
+        <v>23.4</v>
+      </c>
+      <c r="E1702">
+        <v>7</v>
+      </c>
+      <c r="F1702">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -56008,10 +59333,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01ABCD41-9594-F549-BC55-37725303300E}">
-  <dimension ref="A1:C301"/>
+  <dimension ref="A1:C326"/>
   <sheetViews>
-    <sheetView topLeftCell="A289" workbookViewId="0">
-      <selection activeCell="C301" sqref="C301"/>
+    <sheetView topLeftCell="A313" workbookViewId="0">
+      <selection activeCell="C327" sqref="C327"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -59325,6 +62650,281 @@
       </c>
       <c r="C301" t="s">
         <v>89</v>
+      </c>
+    </row>
+    <row r="302" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A302">
+        <v>14</v>
+      </c>
+      <c r="B302">
+        <v>1</v>
+      </c>
+      <c r="C302" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="303" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A303">
+        <v>14</v>
+      </c>
+      <c r="B303">
+        <v>2</v>
+      </c>
+      <c r="C303" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="304" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A304">
+        <v>14</v>
+      </c>
+      <c r="B304">
+        <v>3</v>
+      </c>
+      <c r="C304" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="305" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A305">
+        <v>14</v>
+      </c>
+      <c r="B305">
+        <v>4</v>
+      </c>
+      <c r="C305" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="306" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A306">
+        <v>14</v>
+      </c>
+      <c r="B306">
+        <v>5</v>
+      </c>
+      <c r="C306" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="307" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A307">
+        <v>14</v>
+      </c>
+      <c r="B307">
+        <v>6</v>
+      </c>
+      <c r="C307" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="308" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A308">
+        <v>14</v>
+      </c>
+      <c r="B308">
+        <v>7</v>
+      </c>
+      <c r="C308" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="309" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A309">
+        <v>14</v>
+      </c>
+      <c r="B309">
+        <v>8</v>
+      </c>
+      <c r="C309" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="310" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A310">
+        <v>14</v>
+      </c>
+      <c r="B310">
+        <v>9</v>
+      </c>
+      <c r="C310" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="311" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A311">
+        <v>14</v>
+      </c>
+      <c r="B311">
+        <v>10</v>
+      </c>
+      <c r="C311" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="312" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A312">
+        <v>14</v>
+      </c>
+      <c r="B312">
+        <v>11</v>
+      </c>
+      <c r="C312" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="313" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A313">
+        <v>14</v>
+      </c>
+      <c r="B313">
+        <v>12</v>
+      </c>
+      <c r="C313" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="314" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A314">
+        <v>14</v>
+      </c>
+      <c r="B314">
+        <v>13</v>
+      </c>
+      <c r="C314" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="315" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A315">
+        <v>14</v>
+      </c>
+      <c r="B315">
+        <v>14</v>
+      </c>
+      <c r="C315" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="316" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A316">
+        <v>14</v>
+      </c>
+      <c r="B316">
+        <v>15</v>
+      </c>
+      <c r="C316" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="317" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A317">
+        <v>14</v>
+      </c>
+      <c r="B317">
+        <v>16</v>
+      </c>
+      <c r="C317" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="318" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A318">
+        <v>14</v>
+      </c>
+      <c r="B318">
+        <v>17</v>
+      </c>
+      <c r="C318" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="319" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A319">
+        <v>14</v>
+      </c>
+      <c r="B319">
+        <v>18</v>
+      </c>
+      <c r="C319" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="320" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A320">
+        <v>14</v>
+      </c>
+      <c r="B320">
+        <v>19</v>
+      </c>
+      <c r="C320" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="321" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A321">
+        <v>14</v>
+      </c>
+      <c r="B321">
+        <v>20</v>
+      </c>
+      <c r="C321" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="322" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A322">
+        <v>14</v>
+      </c>
+      <c r="B322">
+        <v>21</v>
+      </c>
+      <c r="C322" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="323" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A323">
+        <v>14</v>
+      </c>
+      <c r="B323">
+        <v>22</v>
+      </c>
+      <c r="C323" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="324" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A324">
+        <v>14</v>
+      </c>
+      <c r="B324">
+        <v>23</v>
+      </c>
+      <c r="C324" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="325" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A325">
+        <v>14</v>
+      </c>
+      <c r="B325">
+        <v>24</v>
+      </c>
+      <c r="C325" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="326" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A326">
+        <v>14</v>
+      </c>
+      <c r="B326">
+        <v>25</v>
+      </c>
+      <c r="C326" t="s">
+        <v>84</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Week 13 viewership / week 14 predictions
</commit_message>
<xml_diff>
--- a/ratings-2022.xlsx
+++ b/ratings-2022.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mike/PycharmProjects/tvratings-ssac2023/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51D42F34-44F8-2948-9372-4691FA04AF75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75FAE34C-281F-F14F-B8EE-C40F63AD5007}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1560" yWindow="14120" windowWidth="37240" windowHeight="10280" xr2:uid="{BBDA95F9-3552-704A-ADE2-3350C5179C3F}"/>
   </bookViews>
@@ -994,9 +994,9 @@
   <dimension ref="A1:AA287"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="760" topLeftCell="A234" activePane="bottomLeft"/>
+      <pane ySplit="760" topLeftCell="A271" activePane="bottomLeft"/>
       <selection sqref="A1:AA1"/>
-      <selection pane="bottomLeft" activeCell="F255" sqref="F255"/>
+      <selection pane="bottomLeft" activeCell="F284" sqref="F284"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -22555,7 +22555,7 @@
         <v>173</v>
       </c>
       <c r="F253">
-        <v>0</v>
+        <v>1719000</v>
       </c>
       <c r="G253">
         <v>2022</v>
@@ -22711,7 +22711,7 @@
         <v>58</v>
       </c>
       <c r="F255">
-        <v>0</v>
+        <v>1438000</v>
       </c>
       <c r="G255">
         <v>2022</v>
@@ -22867,7 +22867,7 @@
         <v>84</v>
       </c>
       <c r="F257">
-        <v>0</v>
+        <v>3605000</v>
       </c>
       <c r="G257">
         <v>2022</v>
@@ -22945,7 +22945,7 @@
         <v>50</v>
       </c>
       <c r="F258">
-        <v>0</v>
+        <v>3274000</v>
       </c>
       <c r="G258">
         <v>2022</v>
@@ -23101,7 +23101,7 @@
         <v>52</v>
       </c>
       <c r="F260">
-        <v>6711000</v>
+        <v>6710000</v>
       </c>
       <c r="G260">
         <v>2022</v>
@@ -23257,7 +23257,7 @@
         <v>86</v>
       </c>
       <c r="F262">
-        <v>0</v>
+        <v>2060000</v>
       </c>
       <c r="G262">
         <v>2022</v>
@@ -23335,7 +23335,7 @@
         <v>38</v>
       </c>
       <c r="F263">
-        <v>0</v>
+        <v>17137000</v>
       </c>
       <c r="G263">
         <v>2022</v>
@@ -23413,7 +23413,7 @@
         <v>92</v>
       </c>
       <c r="F264">
-        <v>0</v>
+        <v>2324000</v>
       </c>
       <c r="G264">
         <v>2022</v>
@@ -23491,7 +23491,7 @@
         <v>39</v>
       </c>
       <c r="F265">
-        <v>0</v>
+        <v>694000</v>
       </c>
       <c r="G265">
         <v>2022</v>
@@ -23569,7 +23569,7 @@
         <v>122</v>
       </c>
       <c r="F266">
-        <v>0</v>
+        <v>6271000</v>
       </c>
       <c r="G266">
         <v>2022</v>
@@ -23647,7 +23647,7 @@
         <v>49</v>
       </c>
       <c r="F267">
-        <v>0</v>
+        <v>3557000</v>
       </c>
       <c r="G267">
         <v>2022</v>
@@ -23725,7 +23725,7 @@
         <v>150</v>
       </c>
       <c r="F268">
-        <v>0</v>
+        <v>1705000</v>
       </c>
       <c r="G268">
         <v>2022</v>
@@ -23803,7 +23803,7 @@
         <v>146</v>
       </c>
       <c r="F269">
-        <v>0</v>
+        <v>213000</v>
       </c>
       <c r="G269">
         <v>2022</v>
@@ -23881,7 +23881,7 @@
         <v>136</v>
       </c>
       <c r="F270">
-        <v>0</v>
+        <v>4339000</v>
       </c>
       <c r="G270">
         <v>2022</v>
@@ -23959,7 +23959,7 @@
         <v>29</v>
       </c>
       <c r="F271">
-        <v>0</v>
+        <v>1991000</v>
       </c>
       <c r="G271">
         <v>2022</v>
@@ -24037,7 +24037,7 @@
         <v>114</v>
       </c>
       <c r="F272">
-        <v>0</v>
+        <v>3921000</v>
       </c>
       <c r="G272">
         <v>2022</v>
@@ -24115,7 +24115,7 @@
         <v>88</v>
       </c>
       <c r="F273">
-        <v>0</v>
+        <v>329000</v>
       </c>
       <c r="G273">
         <v>2022</v>
@@ -24193,7 +24193,7 @@
         <v>46</v>
       </c>
       <c r="F274">
-        <v>0</v>
+        <v>6681000</v>
       </c>
       <c r="G274">
         <v>2022</v>
@@ -24271,7 +24271,7 @@
         <v>36</v>
       </c>
       <c r="F275">
-        <v>0</v>
+        <v>1211000</v>
       </c>
       <c r="G275">
         <v>2022</v>
@@ -24349,7 +24349,7 @@
         <v>138</v>
       </c>
       <c r="F276">
-        <v>0</v>
+        <v>2316000</v>
       </c>
       <c r="G276">
         <v>2022</v>
@@ -24427,7 +24427,7 @@
         <v>181</v>
       </c>
       <c r="F277">
-        <v>0</v>
+        <v>2380000</v>
       </c>
       <c r="G277">
         <v>2022</v>
@@ -24505,7 +24505,7 @@
         <v>97</v>
       </c>
       <c r="F278">
-        <v>0</v>
+        <v>453000</v>
       </c>
       <c r="G278">
         <v>2022</v>

</xml_diff>

<commit_message>
Model update - calculation of addbin feature corrected and predictions regenerated with new model
</commit_message>
<xml_diff>
--- a/ratings-2022.xlsx
+++ b/ratings-2022.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mike/PycharmProjects/tvratings-ssac2023/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75FAE34C-281F-F14F-B8EE-C40F63AD5007}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBF76E32-0C5A-0B42-88BC-CA0E571C8CE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="14120" windowWidth="37240" windowHeight="10280" xr2:uid="{BBDA95F9-3552-704A-ADE2-3350C5179C3F}"/>
+    <workbookView xWindow="1560" yWindow="14120" windowWidth="37240" windowHeight="10280" activeTab="1" xr2:uid="{BBDA95F9-3552-704A-ADE2-3350C5179C3F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3504" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3504" uniqueCount="189">
   <si>
     <t>Time</t>
   </si>
@@ -632,9 +632,6 @@
   <si>
     <t>North Dakota State</t>
   </si>
-  <si>
-    <t>North Carolina State</t>
-  </si>
 </sst>
 </file>
 
@@ -993,8 +990,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78DF36B5-5368-0F4E-AE20-BC9ECC5E0688}">
   <dimension ref="A1:AA287"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="760" topLeftCell="A271" activePane="bottomLeft"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="760" topLeftCell="A316" activePane="bottomLeft"/>
       <selection sqref="A1:AA1"/>
       <selection pane="bottomLeft" activeCell="F284" sqref="F284"/>
     </sheetView>
@@ -25279,8 +25276,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF262906-C2E8-EB40-9ABF-94137CE271DB}">
   <dimension ref="A1:F1702"/>
   <sheetViews>
-    <sheetView topLeftCell="A1614" workbookViewId="0">
-      <selection activeCell="B1624" sqref="B1624"/>
+    <sheetView tabSelected="1" topLeftCell="A1638" workbookViewId="0">
+      <selection activeCell="A1647" sqref="A1647"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -58187,7 +58184,7 @@
     </row>
     <row r="1646" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1646" t="s">
-        <v>189</v>
+        <v>84</v>
       </c>
       <c r="B1646">
         <v>14</v>

</xml_diff>

<commit_message>
Final 2022 season predictions and results
</commit_message>
<xml_diff>
--- a/ratings-2022.xlsx
+++ b/ratings-2022.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mike/PycharmProjects/tvratings-ssac2023/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBF76E32-0C5A-0B42-88BC-CA0E571C8CE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9A77461-A7A0-324A-BC7C-8F44D5ED3610}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="14120" windowWidth="37240" windowHeight="10280" activeTab="1" xr2:uid="{BBDA95F9-3552-704A-ADE2-3350C5179C3F}"/>
+    <workbookView xWindow="1540" yWindow="14120" windowWidth="37240" windowHeight="10280" xr2:uid="{BBDA95F9-3552-704A-ADE2-3350C5179C3F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -990,10 +990,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78DF36B5-5368-0F4E-AE20-BC9ECC5E0688}">
   <dimension ref="A1:AA287"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="760" topLeftCell="A316" activePane="bottomLeft"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="760" topLeftCell="A276" activePane="bottomLeft"/>
       <selection sqref="A1:AA1"/>
-      <selection pane="bottomLeft" activeCell="F284" sqref="F284"/>
+      <selection pane="bottomLeft" activeCell="F288" sqref="F288"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -24580,7 +24580,7 @@
         <v>53</v>
       </c>
       <c r="F279">
-        <v>0</v>
+        <v>5967000</v>
       </c>
       <c r="G279">
         <v>2022</v>
@@ -24658,7 +24658,7 @@
         <v>93</v>
       </c>
       <c r="F280">
-        <v>0</v>
+        <v>9413000</v>
       </c>
       <c r="G280">
         <v>2022</v>
@@ -24736,7 +24736,7 @@
         <v>171</v>
       </c>
       <c r="F281">
-        <v>0</v>
+        <v>721000</v>
       </c>
       <c r="G281">
         <v>2022</v>
@@ -24814,7 +24814,7 @@
         <v>128</v>
       </c>
       <c r="F282">
-        <v>0</v>
+        <v>332000</v>
       </c>
       <c r="G282">
         <v>2022</v>
@@ -24892,7 +24892,7 @@
         <v>114</v>
       </c>
       <c r="F283">
-        <v>0</v>
+        <v>10894000</v>
       </c>
       <c r="G283">
         <v>2022</v>
@@ -24970,7 +24970,7 @@
         <v>88</v>
       </c>
       <c r="F284">
-        <v>0</v>
+        <v>2695000</v>
       </c>
       <c r="G284">
         <v>2022</v>
@@ -25048,7 +25048,7 @@
         <v>132</v>
       </c>
       <c r="F285">
-        <v>0</v>
+        <v>1938000</v>
       </c>
       <c r="G285">
         <v>2022</v>
@@ -25126,7 +25126,7 @@
         <v>43</v>
       </c>
       <c r="F286">
-        <v>0</v>
+        <v>10699000</v>
       </c>
       <c r="G286">
         <v>2022</v>
@@ -25204,7 +25204,7 @@
         <v>87</v>
       </c>
       <c r="F287">
-        <v>0</v>
+        <v>3467000</v>
       </c>
       <c r="G287">
         <v>2022</v>
@@ -25276,7 +25276,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF262906-C2E8-EB40-9ABF-94137CE271DB}">
   <dimension ref="A1:F1702"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1638" workbookViewId="0">
+    <sheetView topLeftCell="A1683" workbookViewId="0">
       <selection activeCell="A1647" sqref="A1647"/>
     </sheetView>
   </sheetViews>

</xml_diff>